<commit_message>
Update to aggregation database to remove commas in headings
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Risk_sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53EA7F2-D5E8-144D-B92F-85FF3486AB0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B23CAB-B959-C249-A46A-80FB8E9319B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="-4640" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -317,21 +317,6 @@
     <t>D_IMF_debt2020.2019_norm</t>
   </si>
   <si>
-    <t xml:space="preserve">H_Oxrollback_score_norm, </t>
-  </si>
-  <si>
-    <t>H_Covidgrowth_casesnorm,</t>
-  </si>
-  <si>
-    <t>H_Covidgrowth_deathsnorm,</t>
-  </si>
-  <si>
-    <t>H_new_cases_smoothed_per_million_norm,</t>
-  </si>
-  <si>
-    <t>H_new_deaths_smoothed_per_million_norm,</t>
-  </si>
-  <si>
     <t>H_Covidproj_Projected_Deaths_._1M_norm</t>
   </si>
   <si>
@@ -1246,6 +1231,21 @@
 ----------------------------------------
 Macro = max(ED, FC)
 </t>
+  </si>
+  <si>
+    <t>H_Covidgrowth_casesnorm</t>
+  </si>
+  <si>
+    <t>H_Covidgrowth_deathsnorm</t>
+  </si>
+  <si>
+    <t>H_new_cases_smoothed_per_million_norm</t>
+  </si>
+  <si>
+    <t>H_new_deaths_smoothed_per_million_norm</t>
+  </si>
+  <si>
+    <t>H_Oxrollback_score_norm</t>
   </si>
 </sst>
 </file>
@@ -1709,81 +1709,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1822,6 +1747,81 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2787,8 +2787,8 @@
   </sheetPr>
   <dimension ref="A1:CR29"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="89" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2811,7 +2811,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D1" s="35" t="s">
         <v>9</v>
@@ -2824,14 +2824,14 @@
       </c>
     </row>
     <row r="2" spans="1:96" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="60"/>
+      <c r="A2" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="58"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
@@ -2928,19 +2928,19 @@
         <v>24</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="63" t="s">
-        <v>62</v>
+        <v>71</v>
+      </c>
+      <c r="D3" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>57</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
@@ -3038,14 +3038,14 @@
         <v>26</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="63"/>
+        <v>70</v>
+      </c>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="61"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
@@ -3142,14 +3142,14 @@
         <v>25</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="63"/>
+        <v>72</v>
+      </c>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="61"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
@@ -3241,14 +3241,14 @@
       <c r="CQ5" s="15"/>
     </row>
     <row r="6" spans="1:96" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
+      <c r="A6" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
@@ -3341,22 +3341,22 @@
     </row>
     <row r="7" spans="1:96" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="41" t="s">
-        <v>91</v>
+        <v>73</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="65" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" s="72" t="s">
+        <v>86</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
@@ -3450,17 +3450,17 @@
     </row>
     <row r="8" spans="1:96" s="2" customFormat="1" ht="49" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="42"/>
+        <v>74</v>
+      </c>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="73"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
@@ -3556,14 +3556,14 @@
         <v>27</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="42"/>
+        <v>99</v>
+      </c>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="73"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
@@ -3662,11 +3662,11 @@
         <v>7</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="42"/>
+        <v>82</v>
+      </c>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="73"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
@@ -3759,17 +3759,17 @@
     </row>
     <row r="11" spans="1:96" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="42"/>
+        <v>98</v>
+      </c>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
@@ -3868,11 +3868,11 @@
         <v>1</v>
       </c>
       <c r="C12" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="43"/>
+        <v>98</v>
+      </c>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="74"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
@@ -3964,14 +3964,14 @@
       <c r="CQ12" s="15"/>
     </row>
     <row r="13" spans="1:96" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="61" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
+      <c r="A13" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -4067,18 +4067,18 @@
         <v>31</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E14" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="64" t="s">
+      <c r="F14" s="62" t="s">
         <v>15</v>
       </c>
       <c r="G14" s="15"/>
@@ -4176,14 +4176,14 @@
         <v>30</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="64"/>
+        <v>75</v>
+      </c>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="62"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
@@ -4275,14 +4275,14 @@
       <c r="CQ15" s="15"/>
     </row>
     <row r="16" spans="1:96" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
+      <c r="A16" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="58"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
@@ -4379,16 +4379,16 @@
         <v>32</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D17" s="32" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F17" s="33" t="s">
         <v>16</v>
@@ -4485,14 +4485,14 @@
       <c r="CR17" s="15"/>
     </row>
     <row r="18" spans="1:96" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="61" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
+      <c r="A18" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
@@ -4586,21 +4586,21 @@
     </row>
     <row r="19" spans="1:96" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="53" t="s">
+      <c r="E19" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="65" t="s">
+      <c r="F19" s="71" t="s">
         <v>19</v>
       </c>
       <c r="G19" s="15"/>
@@ -4696,17 +4696,17 @@
     </row>
     <row r="20" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="65"/>
+        <v>78</v>
+      </c>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="71"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
@@ -4800,20 +4800,20 @@
     </row>
     <row r="21" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>35</v>
+        <v>127</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="65"/>
+        <v>78</v>
+      </c>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="71"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
@@ -4906,17 +4906,17 @@
     </row>
     <row r="22" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="65"/>
+        <v>79</v>
+      </c>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="71"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
@@ -5010,17 +5010,17 @@
     </row>
     <row r="23" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>37</v>
+        <v>129</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="65"/>
+        <v>80</v>
+      </c>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="71"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
@@ -5114,17 +5114,17 @@
     </row>
     <row r="24" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>33</v>
+        <v>130</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="65"/>
+        <v>81</v>
+      </c>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="71"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
@@ -5217,14 +5217,14 @@
       <c r="CR24" s="15"/>
     </row>
     <row r="25" spans="1:96" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="57"/>
+      <c r="A25" s="68" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="70"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
@@ -5318,22 +5318,22 @@
     </row>
     <row r="26" spans="1:96" s="5" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="F26" s="50" t="s">
-        <v>97</v>
+        <v>81</v>
+      </c>
+      <c r="D26" s="75" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="78" t="s">
+        <v>92</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -5428,17 +5428,17 @@
     </row>
     <row r="27" spans="1:96" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="51"/>
+        <v>83</v>
+      </c>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="79"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
@@ -5532,17 +5532,17 @@
     </row>
     <row r="28" spans="1:96" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="52"/>
+        <v>37</v>
+      </c>
+      <c r="D28" s="77"/>
+      <c r="E28" s="77"/>
+      <c r="F28" s="80"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
@@ -5650,6 +5650,16 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="D19:D24"/>
+    <mergeCell ref="E19:E24"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="F19:F24"/>
+    <mergeCell ref="F7:F12"/>
+    <mergeCell ref="E7:E12"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A16:F16"/>
@@ -5661,16 +5671,6 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E19:E24"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="F19:F24"/>
-    <mergeCell ref="F7:F12"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="D19:D24"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -5695,7 +5695,7 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="107" workbookViewId="0">
+    <sheetView zoomScale="107" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -5716,188 +5716,188 @@
         <v>20</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
+      <c r="A2" s="56" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="72" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="69" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="69" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" s="69" t="s">
-        <v>124</v>
+        <v>102</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
+      <c r="A4" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="57"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="70" t="s">
-        <v>111</v>
-      </c>
-      <c r="B5" s="69" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
+      <c r="A5" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="61" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
+      <c r="A6" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
     </row>
     <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="69" t="s">
-        <v>122</v>
+        <v>111</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>117</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" s="78" t="s">
-        <v>106</v>
+        <v>125</v>
+      </c>
+      <c r="G7" s="53" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="G8" s="79"/>
+      <c r="A8" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="G8" s="54"/>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="68" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="68" t="s">
-        <v>121</v>
+        <v>104</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>116</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>125</v>
-      </c>
-      <c r="G9" s="79" t="s">
-        <v>106</v>
+        <v>120</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="G10" s="80"/>
+      <c r="A10" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="G10" s="55"/>
     </row>
     <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="73" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="69" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="G11" s="79"/>
+      <c r="C11" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="G11" s="54"/>
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="56"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="G12" s="78"/>
+      <c r="A12" s="68" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="G12" s="53"/>
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="69" t="s">
-        <v>120</v>
-      </c>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="G13" s="78" t="s">
-        <v>106</v>
+        <v>34</v>
+      </c>
+      <c r="B13" s="41"/>
+      <c r="C13" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="G13" s="53" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="55" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" s="56"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="56"/>
+      <c r="A14" s="68" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
     </row>
     <row r="15" spans="1:7" ht="248" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="71" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="74" t="s">
-        <v>119</v>
-      </c>
-      <c r="C15" s="69" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15" s="75" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" s="76" t="s">
-        <v>127</v>
-      </c>
-      <c r="F15" s="77" t="s">
-        <v>106</v>
+      <c r="A15" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="F15" s="52" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -5939,46 +5939,46 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Adding debt variable (D_EconomicSupportIndexForDisplay and D_fiscalgdpnum_norm) to the debt risk sheet
removing CESI from Macro and placing in Debt
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B23CAB-B959-C249-A46A-80FB8E9319B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F57187C2-98E1-8747-88AB-64F63B7617F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4640" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="139">
   <si>
     <r>
       <t xml:space="preserve">Growth in conflict fatalities - </t>
@@ -81,9 +81,6 @@
     <t>INFORM crisis monitor</t>
   </si>
   <si>
-    <t>D = D_IMF_debt2020.2019_norm</t>
-  </si>
-  <si>
     <t>RISK SCORES AS MAX VALUES</t>
   </si>
   <si>
@@ -108,30 +105,6 @@
         <family val="1"/>
       </rPr>
       <t>MAX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>(M_GDP_IMF_2019minus2020_norm, M_GDP_WB_2019minus2020_norm)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">M_AV = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>GEOMETRICMEAN</t>
     </r>
     <r>
       <rPr>
@@ -220,30 +193,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">H_AV = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>GEOMETRICMEAN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>(H_Oxrollback_score_norm, H_Covidgrowth_casesnorm, H_Covidgrowth_deathsnorm, H_new_cases_smoothed_per_million_norm, H_new_deaths_smoothed_per_million_norm, H_Covidproj_Projected_Deaths_._1M_norm)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">H_SQ = </t>
     </r>
     <r>
@@ -281,18 +230,12 @@
     <t>INDICATOR DESCRIPTION</t>
   </si>
   <si>
-    <t>RISK SCORES AS MEANS</t>
-  </si>
-  <si>
     <t>RISK SCORES AS GEOMETRIC MEANS</t>
   </si>
   <si>
     <t>INDICATOR NAME</t>
   </si>
   <si>
-    <t>F_FAO_6mFPV_norm</t>
-  </si>
-  <si>
     <t>F_Artemis_Score_norm</t>
   </si>
   <si>
@@ -347,9 +290,6 @@
     <t>NATURAL HAZARD RISK</t>
   </si>
   <si>
-    <t xml:space="preserve">Food price volatility (FAOSTAT and DFPM) </t>
-  </si>
-  <si>
     <t>FEWSNET IPC classification (near term)</t>
   </si>
   <si>
@@ -377,145 +317,10 @@
     <t>Oxford Lockdown rollback index (source)</t>
   </si>
   <si>
-    <t>Natural multi-hazard rating (INFORM) – 2020 data
- (details of methodology; source)</t>
-  </si>
-  <si>
     <t>COVID RESPONSE</t>
   </si>
   <si>
     <t>MACRO-ECONOMIC VULNERABILITY</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>IF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> FEWSNET country then FS = F_FEWSNET_SCORE,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>ELSE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> FS = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>MAX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>(F_FPV, F_AFTEMIS)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">IF </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">FEWSNET country then FS_SQ = FS,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> ELSE </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">FS_SQ </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>= GEOMETRICMEAN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">(EXISTING_RISK_FS, FS)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>Note: FS calculated as max values</t>
-    </r>
   </si>
   <si>
     <t>Max score</t>
@@ -701,19 +506,6 @@
       </rPr>
       <t xml:space="preserve"> Risk Component_SQ  &gt; 7)</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> &gt; 3
-7 = 7 
-1 = 1</t>
-  </si>
-  <si>
-    <t>10 &gt;= 0.9 pct
-0 &lt;=  0.1 pct</t>
-  </si>
-  <si>
-    <t>10 &gt;= 0.2
-0 &lt;=  0</t>
   </si>
   <si>
     <t>10 &gt; 300
@@ -868,151 +660,6 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>IF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> FEWSNET country then FS_AV = F_FEWSNET_SCORE,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>ELSE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> FS_AV = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>MAX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>(F_FPV, F_AFTEMIS)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>IF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> C_INFORM_CRISIS = "Ongoing Complex Crisis" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>AND</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> EXISTING_RISK_Fr &lt;=5 then Fr_AV = 10,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>ELSE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Fr_AV = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>GEOMETRICMEAN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>(Fr_FSI_2019minus2020_norm, Fr_REIGN_couprisk3m_norm, Fr_ACLED_event_same_month_difference_perc_norm, Fr_ACLED_fatal_same_month_difference_perc_norm)</t>
-    </r>
-  </si>
-  <si>
-    <t>D_AV = D_IMF_debt2020.2019_norm</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Garamond"/>
@@ -1042,36 +689,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>NH_AV =</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> MAX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>(NH_UKMO_TOTAL.RISK.NEXT.6.MONTHS_norm, NH_GDAC_Hazard_Score_Norm, NH_INFORM_Crisis_Norm)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve"> </t>
     </r>
     <r>
@@ -1247,12 +864,120 @@
   <si>
     <t>H_Oxrollback_score_norm</t>
   </si>
+  <si>
+    <t>10 &gt; 3
+7 = 7 
+1 = 1</t>
+  </si>
+  <si>
+    <t>F_fpv_alt</t>
+  </si>
+  <si>
+    <t>F_food_acaps</t>
+  </si>
+  <si>
+    <t>Metric to track if price of one or more basic food commodities is abnormally high in main markets (identified using FAO Indicator of Price Anomaly and GIEWS)</t>
+  </si>
+  <si>
+    <t>Metric to track if country is affected by famine or food crises as reported under the ACAPS real-time risk repository</t>
+  </si>
+  <si>
+    <t>High &gt;= 0.2
+Low &lt;=  0</t>
+  </si>
+  <si>
+    <t>10 = above IPA threshold
+0 = below IPA threshold</t>
+  </si>
+  <si>
+    <t>10 = ACAPS famine/food crisis
+0 = Otherwise</t>
+  </si>
+  <si>
+    <t>IF FEWSNET country then FS = MAX(F_FEWSNET_SCORE,  F_AFTEMIS)
+ELSE FS = MAX(F_fpv_alt, F_food_acaps)</t>
+  </si>
+  <si>
+    <t>IF FEWSNET country then FS_SQ = FS,
+ ELSE FS_SQ = GEOMETRICMEAN(EXISTING_RISK_FS, FS)
+Note: FS calculated as max values</t>
+  </si>
+  <si>
+    <t>H_GovernmentResponseIndexForDisplay</t>
+  </si>
+  <si>
+    <t>Oxford Government Response Index</t>
+  </si>
+  <si>
+    <t>10 &gt; 80
+0 &lt; 15</t>
+  </si>
+  <si>
+    <t>D_fiscalgdpnum_norm</t>
+  </si>
+  <si>
+    <t>Fiscal Support Package as percentage of GDP (measured by IGC)</t>
+  </si>
+  <si>
+    <t>10 &lt; 5 pct
+0 &gt; 95 pct</t>
+  </si>
+  <si>
+    <t>COVID Economic Support Index (as measured by Oxford University Blavatnik)</t>
+  </si>
+  <si>
+    <t>H_EconomicSupportIndexForDisplay</t>
+  </si>
+  <si>
+    <t>10 &lt; 15
+0 &gt; 80</t>
+  </si>
+  <si>
+    <t>D_CESI_Index_norm</t>
+  </si>
+  <si>
+    <t>COVID Economic Stimus Index (as measured by Elgin et al)</t>
+  </si>
+  <si>
+    <t>10 &lt; 10 pct
+0 &gt; 95 pct</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">D = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>MAX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>(D_CESI_Index_norm,
+H_EconomicSupportIndexForDisplay,
+D_fiscalgdpnum_norm,
+D_IMF_debt2020.2019_norm)</t>
+    </r>
+  </si>
+  <si>
+    <t>Natural multi-hazard rating (INFORM) – 2020 data (details of methodology; source)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1354,8 +1079,28 @@
       <name val="Garamond"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Garamond"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1458,8 +1203,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFACB9CA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD6DCE4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1596,12 +1359,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1667,12 +1463,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1680,12 +1470,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1748,6 +1532,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1772,56 +1613,42 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2785,10 +2612,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:CR29"/>
+  <dimension ref="A1:CQ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="89" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2797,41 +2624,37 @@
     <col min="2" max="2" width="42.33203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="22" style="26" customWidth="1"/>
     <col min="4" max="4" width="52.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="48.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="47.33203125" style="7" customWidth="1"/>
-    <col min="7" max="96" width="10.83203125" style="15"/>
-    <col min="97" max="16384" width="10.83203125" style="7"/>
+    <col min="5" max="5" width="47.33203125" style="7" customWidth="1"/>
+    <col min="6" max="95" width="10.83203125" style="15"/>
+    <col min="96" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:95" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:96" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="58"/>
+    <row r="2" spans="1:95" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
       <c r="I2" s="15"/>
@@ -2921,27 +2744,24 @@
       <c r="CO2" s="15"/>
       <c r="CP2" s="15"/>
       <c r="CQ2" s="15"/>
-      <c r="CR2" s="15"/>
     </row>
-    <row r="3" spans="1:96" s="1" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="63" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" s="61" t="s">
-        <v>57</v>
-      </c>
+    <row r="3" spans="1:95" s="1" customFormat="1" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="80" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="78" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="15"/>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
       <c r="I3" s="15"/>
@@ -3031,21 +2851,20 @@
       <c r="CO3" s="15"/>
       <c r="CP3" s="15"/>
       <c r="CQ3" s="15"/>
-      <c r="CR3" s="15"/>
     </row>
-    <row r="4" spans="1:96" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="61"/>
+    <row r="4" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="80" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="78"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
@@ -3135,21 +2954,20 @@
       <c r="CO4" s="15"/>
       <c r="CP4" s="15"/>
       <c r="CQ4" s="15"/>
-      <c r="CR4" s="15"/>
     </row>
-    <row r="5" spans="1:96" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="61"/>
+    <row r="5" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="80" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="79" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="78"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
@@ -3240,15 +3058,19 @@
       <c r="CP5" s="15"/>
       <c r="CQ5" s="15"/>
     </row>
-    <row r="6" spans="1:96" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="58"/>
+    <row r="6" spans="1:95" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="80" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="81" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="78"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
@@ -3337,27 +3159,16 @@
       <c r="CN6" s="15"/>
       <c r="CO6" s="15"/>
       <c r="CP6" s="15"/>
-      <c r="CQ6" s="15"/>
     </row>
-    <row r="7" spans="1:96" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="65" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="72" t="s">
-        <v>86</v>
-      </c>
+    <row r="7" spans="1:95" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
@@ -3446,21 +3257,24 @@
       <c r="CN7" s="15"/>
       <c r="CO7" s="15"/>
       <c r="CP7" s="15"/>
-      <c r="CQ7" s="15"/>
     </row>
-    <row r="8" spans="1:96" s="2" customFormat="1" ht="49" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:95" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C8" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="61" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="73"/>
+      <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
@@ -3549,21 +3363,20 @@
       <c r="CN8" s="15"/>
       <c r="CO8" s="15"/>
       <c r="CP8" s="15"/>
-      <c r="CQ8" s="15"/>
     </row>
-    <row r="9" spans="1:96" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:95" s="2" customFormat="1" ht="49" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="73"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="62"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
@@ -3652,21 +3465,20 @@
       <c r="CN9" s="15"/>
       <c r="CO9" s="15"/>
       <c r="CP9" s="15"/>
-      <c r="CQ9" s="15"/>
     </row>
-    <row r="10" spans="1:96" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="73"/>
+        <v>41</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="62"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
@@ -3755,21 +3567,20 @@
       <c r="CN10" s="15"/>
       <c r="CO10" s="15"/>
       <c r="CP10" s="15"/>
-      <c r="CQ10" s="15"/>
     </row>
-    <row r="11" spans="1:96" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="73"/>
+        <v>7</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="62"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
@@ -3858,21 +3669,20 @@
       <c r="CN11" s="15"/>
       <c r="CO11" s="15"/>
       <c r="CP11" s="15"/>
-      <c r="CQ11" s="15"/>
     </row>
-    <row r="12" spans="1:96" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="74"/>
+        <v>81</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="62"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
@@ -3961,17 +3771,20 @@
       <c r="CN12" s="15"/>
       <c r="CO12" s="15"/>
       <c r="CP12" s="15"/>
-      <c r="CQ12" s="15"/>
     </row>
-    <row r="13" spans="1:96" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
+    <row r="13" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="63"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
@@ -4060,27 +3873,16 @@
       <c r="CN13" s="15"/>
       <c r="CO13" s="15"/>
       <c r="CP13" s="15"/>
-      <c r="CQ13" s="15"/>
     </row>
-    <row r="14" spans="1:96" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="10" t="s">
+    <row r="14" spans="1:95" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="63" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="63" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="62" t="s">
-        <v>15</v>
-      </c>
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
@@ -4169,21 +3971,24 @@
       <c r="CN14" s="15"/>
       <c r="CO14" s="15"/>
       <c r="CP14" s="15"/>
-      <c r="CQ14" s="15"/>
     </row>
-    <row r="15" spans="1:96" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="62"/>
+        <v>63</v>
+      </c>
+      <c r="D15" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="77" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
@@ -4272,17 +4077,20 @@
       <c r="CN15" s="15"/>
       <c r="CO15" s="15"/>
       <c r="CP15" s="15"/>
-      <c r="CQ15" s="15"/>
     </row>
-    <row r="16" spans="1:96" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
+    <row r="16" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="78"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
@@ -4371,28 +4179,16 @@
       <c r="CN16" s="15"/>
       <c r="CO16" s="15"/>
       <c r="CP16" s="15"/>
-      <c r="CQ16" s="15"/>
-      <c r="CR16" s="15"/>
     </row>
-    <row r="17" spans="1:96" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>16</v>
-      </c>
+    <row r="17" spans="1:95" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
@@ -4482,18 +4278,25 @@
       <c r="CO17" s="15"/>
       <c r="CP17" s="15"/>
       <c r="CQ17" s="15"/>
-      <c r="CR17" s="15"/>
     </row>
-    <row r="18" spans="1:96" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="15"/>
+    <row r="18" spans="1:95" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" s="87" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="88" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="89" t="s">
+        <v>137</v>
+      </c>
+      <c r="E18" s="89" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="15"/>
+      <c r="G18" s="86"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
@@ -4582,27 +4385,20 @@
       <c r="CO18" s="15"/>
       <c r="CP18" s="15"/>
       <c r="CQ18" s="15"/>
-      <c r="CR18" s="15"/>
     </row>
-    <row r="19" spans="1:96" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="64" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="71" t="s">
-        <v>19</v>
-      </c>
+    <row r="19" spans="1:95" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B19" s="83" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="90" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="84"/>
+      <c r="E19" s="89"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
@@ -4692,21 +4488,20 @@
       <c r="CO19" s="15"/>
       <c r="CP19" s="15"/>
       <c r="CQ19" s="15"/>
-      <c r="CR19" s="15"/>
     </row>
-    <row r="20" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="71"/>
+    <row r="20" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="90" t="s">
+        <v>130</v>
+      </c>
+      <c r="D20" s="84"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
@@ -4796,25 +4591,22 @@
       <c r="CO20" s="15"/>
       <c r="CP20" s="15"/>
       <c r="CQ20" s="15"/>
-      <c r="CR20" s="15"/>
     </row>
-    <row r="21" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="71"/>
+    <row r="21" spans="1:95" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="84"/>
+      <c r="E21" s="89"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="15"/>
-      <c r="H21" s="15" t="s">
-        <v>93</v>
-      </c>
+      <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -4902,21 +4694,16 @@
       <c r="CO21" s="15"/>
       <c r="CP21" s="15"/>
       <c r="CQ21" s="15"/>
-      <c r="CR21" s="15"/>
     </row>
-    <row r="22" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="71"/>
+    <row r="22" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="85"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
@@ -5006,21 +4793,24 @@
       <c r="CO22" s="15"/>
       <c r="CP22" s="15"/>
       <c r="CQ22" s="15"/>
-      <c r="CR22" s="15"/>
     </row>
-    <row r="23" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="B23" s="91" t="s">
+        <v>45</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="71"/>
+        <v>65</v>
+      </c>
+      <c r="D23" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
@@ -5110,21 +4900,20 @@
       <c r="CO23" s="15"/>
       <c r="CP23" s="15"/>
       <c r="CQ23" s="15"/>
-      <c r="CR23" s="15"/>
     </row>
-    <row r="24" spans="1:96" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="71"/>
+        <v>66</v>
+      </c>
+      <c r="D24" s="60"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
@@ -5214,18 +5003,23 @@
       <c r="CO24" s="15"/>
       <c r="CP24" s="15"/>
       <c r="CQ24" s="15"/>
-      <c r="CR24" s="15"/>
     </row>
-    <row r="25" spans="1:96" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="15"/>
+    <row r="25" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="60"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15" t="s">
+        <v>77</v>
+      </c>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
@@ -5314,27 +5108,20 @@
       <c r="CO25" s="15"/>
       <c r="CP25" s="15"/>
       <c r="CQ25" s="15"/>
-      <c r="CR25" s="15"/>
     </row>
-    <row r="26" spans="1:96" s="5" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="75" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="75" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="78" t="s">
-        <v>92</v>
-      </c>
+    <row r="26" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="60"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
@@ -5424,21 +5211,20 @@
       <c r="CO26" s="15"/>
       <c r="CP26" s="15"/>
       <c r="CQ26" s="15"/>
-      <c r="CR26" s="15"/>
     </row>
-    <row r="27" spans="1:96" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="79"/>
+    <row r="27" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="60"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
@@ -5528,21 +5314,20 @@
       <c r="CO27" s="15"/>
       <c r="CP27" s="15"/>
       <c r="CQ27" s="15"/>
-      <c r="CR27" s="15"/>
     </row>
-    <row r="28" spans="1:96" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="77"/>
-      <c r="E28" s="77"/>
-      <c r="F28" s="80"/>
+    <row r="28" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="60"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
@@ -5632,57 +5417,566 @@
       <c r="CO28" s="15"/>
       <c r="CP28" s="15"/>
       <c r="CQ28" s="15"/>
-      <c r="CR28" s="15"/>
     </row>
-    <row r="29" spans="1:96" ht="51" x14ac:dyDescent="0.2">
-      <c r="C29" s="20" t="s">
+    <row r="29" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="60"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="15"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="15"/>
+      <c r="X29" s="15"/>
+      <c r="Y29" s="15"/>
+      <c r="Z29" s="15"/>
+      <c r="AA29" s="15"/>
+      <c r="AB29" s="15"/>
+      <c r="AC29" s="15"/>
+      <c r="AD29" s="15"/>
+      <c r="AE29" s="15"/>
+      <c r="AF29" s="15"/>
+      <c r="AG29" s="15"/>
+      <c r="AH29" s="15"/>
+      <c r="AI29" s="15"/>
+      <c r="AJ29" s="15"/>
+      <c r="AK29" s="15"/>
+      <c r="AL29" s="15"/>
+      <c r="AM29" s="15"/>
+      <c r="AN29" s="15"/>
+      <c r="AO29" s="15"/>
+      <c r="AP29" s="15"/>
+      <c r="AQ29" s="15"/>
+      <c r="AR29" s="15"/>
+      <c r="AS29" s="15"/>
+      <c r="AT29" s="15"/>
+      <c r="AU29" s="15"/>
+      <c r="AV29" s="15"/>
+      <c r="AW29" s="15"/>
+      <c r="AX29" s="15"/>
+      <c r="AY29" s="15"/>
+      <c r="AZ29" s="15"/>
+      <c r="BA29" s="15"/>
+      <c r="BB29" s="15"/>
+      <c r="BC29" s="15"/>
+      <c r="BD29" s="15"/>
+      <c r="BE29" s="15"/>
+      <c r="BF29" s="15"/>
+      <c r="BG29" s="15"/>
+      <c r="BH29" s="15"/>
+      <c r="BI29" s="15"/>
+      <c r="BJ29" s="15"/>
+      <c r="BK29" s="15"/>
+      <c r="BL29" s="15"/>
+      <c r="BM29" s="15"/>
+      <c r="BN29" s="15"/>
+      <c r="BO29" s="15"/>
+      <c r="BP29" s="15"/>
+      <c r="BQ29" s="15"/>
+      <c r="BR29" s="15"/>
+      <c r="BS29" s="15"/>
+      <c r="BT29" s="15"/>
+      <c r="BU29" s="15"/>
+      <c r="BV29" s="15"/>
+      <c r="BW29" s="15"/>
+      <c r="BX29" s="15"/>
+      <c r="BY29" s="15"/>
+      <c r="BZ29" s="15"/>
+      <c r="CA29" s="15"/>
+      <c r="CB29" s="15"/>
+      <c r="CC29" s="15"/>
+      <c r="CD29" s="15"/>
+      <c r="CE29" s="15"/>
+      <c r="CF29" s="15"/>
+      <c r="CG29" s="15"/>
+      <c r="CH29" s="15"/>
+      <c r="CI29" s="15"/>
+      <c r="CJ29" s="15"/>
+      <c r="CK29" s="15"/>
+      <c r="CL29" s="15"/>
+      <c r="CM29" s="15"/>
+      <c r="CN29" s="15"/>
+      <c r="CO29" s="15"/>
+      <c r="CP29" s="15"/>
+      <c r="CQ29" s="15"/>
+    </row>
+    <row r="30" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="15"/>
+      <c r="AA30" s="15"/>
+      <c r="AB30" s="15"/>
+      <c r="AC30" s="15"/>
+      <c r="AD30" s="15"/>
+      <c r="AE30" s="15"/>
+      <c r="AF30" s="15"/>
+      <c r="AG30" s="15"/>
+      <c r="AH30" s="15"/>
+      <c r="AI30" s="15"/>
+      <c r="AJ30" s="15"/>
+      <c r="AK30" s="15"/>
+      <c r="AL30" s="15"/>
+      <c r="AM30" s="15"/>
+      <c r="AN30" s="15"/>
+      <c r="AO30" s="15"/>
+      <c r="AP30" s="15"/>
+      <c r="AQ30" s="15"/>
+      <c r="AR30" s="15"/>
+      <c r="AS30" s="15"/>
+      <c r="AT30" s="15"/>
+      <c r="AU30" s="15"/>
+      <c r="AV30" s="15"/>
+      <c r="AW30" s="15"/>
+      <c r="AX30" s="15"/>
+      <c r="AY30" s="15"/>
+      <c r="AZ30" s="15"/>
+      <c r="BA30" s="15"/>
+      <c r="BB30" s="15"/>
+      <c r="BC30" s="15"/>
+      <c r="BD30" s="15"/>
+      <c r="BE30" s="15"/>
+      <c r="BF30" s="15"/>
+      <c r="BG30" s="15"/>
+      <c r="BH30" s="15"/>
+      <c r="BI30" s="15"/>
+      <c r="BJ30" s="15"/>
+      <c r="BK30" s="15"/>
+      <c r="BL30" s="15"/>
+      <c r="BM30" s="15"/>
+      <c r="BN30" s="15"/>
+      <c r="BO30" s="15"/>
+      <c r="BP30" s="15"/>
+      <c r="BQ30" s="15"/>
+      <c r="BR30" s="15"/>
+      <c r="BS30" s="15"/>
+      <c r="BT30" s="15"/>
+      <c r="BU30" s="15"/>
+      <c r="BV30" s="15"/>
+      <c r="BW30" s="15"/>
+      <c r="BX30" s="15"/>
+      <c r="BY30" s="15"/>
+      <c r="BZ30" s="15"/>
+      <c r="CA30" s="15"/>
+      <c r="CB30" s="15"/>
+      <c r="CC30" s="15"/>
+      <c r="CD30" s="15"/>
+      <c r="CE30" s="15"/>
+      <c r="CF30" s="15"/>
+      <c r="CG30" s="15"/>
+      <c r="CH30" s="15"/>
+      <c r="CI30" s="15"/>
+      <c r="CJ30" s="15"/>
+      <c r="CK30" s="15"/>
+      <c r="CL30" s="15"/>
+      <c r="CM30" s="15"/>
+      <c r="CN30" s="15"/>
+      <c r="CO30" s="15"/>
+      <c r="CP30" s="15"/>
+      <c r="CQ30" s="15"/>
+    </row>
+    <row r="31" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="15"/>
+      <c r="V31" s="15"/>
+      <c r="W31" s="15"/>
+      <c r="X31" s="15"/>
+      <c r="Y31" s="15"/>
+      <c r="Z31" s="15"/>
+      <c r="AA31" s="15"/>
+      <c r="AB31" s="15"/>
+      <c r="AC31" s="15"/>
+      <c r="AD31" s="15"/>
+      <c r="AE31" s="15"/>
+      <c r="AF31" s="15"/>
+      <c r="AG31" s="15"/>
+      <c r="AH31" s="15"/>
+      <c r="AI31" s="15"/>
+      <c r="AJ31" s="15"/>
+      <c r="AK31" s="15"/>
+      <c r="AL31" s="15"/>
+      <c r="AM31" s="15"/>
+      <c r="AN31" s="15"/>
+      <c r="AO31" s="15"/>
+      <c r="AP31" s="15"/>
+      <c r="AQ31" s="15"/>
+      <c r="AR31" s="15"/>
+      <c r="AS31" s="15"/>
+      <c r="AT31" s="15"/>
+      <c r="AU31" s="15"/>
+      <c r="AV31" s="15"/>
+      <c r="AW31" s="15"/>
+      <c r="AX31" s="15"/>
+      <c r="AY31" s="15"/>
+      <c r="AZ31" s="15"/>
+      <c r="BA31" s="15"/>
+      <c r="BB31" s="15"/>
+      <c r="BC31" s="15"/>
+      <c r="BD31" s="15"/>
+      <c r="BE31" s="15"/>
+      <c r="BF31" s="15"/>
+      <c r="BG31" s="15"/>
+      <c r="BH31" s="15"/>
+      <c r="BI31" s="15"/>
+      <c r="BJ31" s="15"/>
+      <c r="BK31" s="15"/>
+      <c r="BL31" s="15"/>
+      <c r="BM31" s="15"/>
+      <c r="BN31" s="15"/>
+      <c r="BO31" s="15"/>
+      <c r="BP31" s="15"/>
+      <c r="BQ31" s="15"/>
+      <c r="BR31" s="15"/>
+      <c r="BS31" s="15"/>
+      <c r="BT31" s="15"/>
+      <c r="BU31" s="15"/>
+      <c r="BV31" s="15"/>
+      <c r="BW31" s="15"/>
+      <c r="BX31" s="15"/>
+      <c r="BY31" s="15"/>
+      <c r="BZ31" s="15"/>
+      <c r="CA31" s="15"/>
+      <c r="CB31" s="15"/>
+      <c r="CC31" s="15"/>
+      <c r="CD31" s="15"/>
+      <c r="CE31" s="15"/>
+      <c r="CF31" s="15"/>
+      <c r="CG31" s="15"/>
+      <c r="CH31" s="15"/>
+      <c r="CI31" s="15"/>
+      <c r="CJ31" s="15"/>
+      <c r="CK31" s="15"/>
+      <c r="CL31" s="15"/>
+      <c r="CM31" s="15"/>
+      <c r="CN31" s="15"/>
+      <c r="CO31" s="15"/>
+      <c r="CP31" s="15"/>
+      <c r="CQ31" s="15"/>
+    </row>
+    <row r="32" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="55"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="15"/>
+      <c r="V32" s="15"/>
+      <c r="W32" s="15"/>
+      <c r="X32" s="15"/>
+      <c r="Y32" s="15"/>
+      <c r="Z32" s="15"/>
+      <c r="AA32" s="15"/>
+      <c r="AB32" s="15"/>
+      <c r="AC32" s="15"/>
+      <c r="AD32" s="15"/>
+      <c r="AE32" s="15"/>
+      <c r="AF32" s="15"/>
+      <c r="AG32" s="15"/>
+      <c r="AH32" s="15"/>
+      <c r="AI32" s="15"/>
+      <c r="AJ32" s="15"/>
+      <c r="AK32" s="15"/>
+      <c r="AL32" s="15"/>
+      <c r="AM32" s="15"/>
+      <c r="AN32" s="15"/>
+      <c r="AO32" s="15"/>
+      <c r="AP32" s="15"/>
+      <c r="AQ32" s="15"/>
+      <c r="AR32" s="15"/>
+      <c r="AS32" s="15"/>
+      <c r="AT32" s="15"/>
+      <c r="AU32" s="15"/>
+      <c r="AV32" s="15"/>
+      <c r="AW32" s="15"/>
+      <c r="AX32" s="15"/>
+      <c r="AY32" s="15"/>
+      <c r="AZ32" s="15"/>
+      <c r="BA32" s="15"/>
+      <c r="BB32" s="15"/>
+      <c r="BC32" s="15"/>
+      <c r="BD32" s="15"/>
+      <c r="BE32" s="15"/>
+      <c r="BF32" s="15"/>
+      <c r="BG32" s="15"/>
+      <c r="BH32" s="15"/>
+      <c r="BI32" s="15"/>
+      <c r="BJ32" s="15"/>
+      <c r="BK32" s="15"/>
+      <c r="BL32" s="15"/>
+      <c r="BM32" s="15"/>
+      <c r="BN32" s="15"/>
+      <c r="BO32" s="15"/>
+      <c r="BP32" s="15"/>
+      <c r="BQ32" s="15"/>
+      <c r="BR32" s="15"/>
+      <c r="BS32" s="15"/>
+      <c r="BT32" s="15"/>
+      <c r="BU32" s="15"/>
+      <c r="BV32" s="15"/>
+      <c r="BW32" s="15"/>
+      <c r="BX32" s="15"/>
+      <c r="BY32" s="15"/>
+      <c r="BZ32" s="15"/>
+      <c r="CA32" s="15"/>
+      <c r="CB32" s="15"/>
+      <c r="CC32" s="15"/>
+      <c r="CD32" s="15"/>
+      <c r="CE32" s="15"/>
+      <c r="CF32" s="15"/>
+      <c r="CG32" s="15"/>
+      <c r="CH32" s="15"/>
+      <c r="CI32" s="15"/>
+      <c r="CJ32" s="15"/>
+      <c r="CK32" s="15"/>
+      <c r="CL32" s="15"/>
+      <c r="CM32" s="15"/>
+      <c r="CN32" s="15"/>
+      <c r="CO32" s="15"/>
+      <c r="CP32" s="15"/>
+      <c r="CQ32" s="15"/>
+    </row>
+    <row r="33" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="56"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
+      <c r="U33" s="15"/>
+      <c r="V33" s="15"/>
+      <c r="W33" s="15"/>
+      <c r="X33" s="15"/>
+      <c r="Y33" s="15"/>
+      <c r="Z33" s="15"/>
+      <c r="AA33" s="15"/>
+      <c r="AB33" s="15"/>
+      <c r="AC33" s="15"/>
+      <c r="AD33" s="15"/>
+      <c r="AE33" s="15"/>
+      <c r="AF33" s="15"/>
+      <c r="AG33" s="15"/>
+      <c r="AH33" s="15"/>
+      <c r="AI33" s="15"/>
+      <c r="AJ33" s="15"/>
+      <c r="AK33" s="15"/>
+      <c r="AL33" s="15"/>
+      <c r="AM33" s="15"/>
+      <c r="AN33" s="15"/>
+      <c r="AO33" s="15"/>
+      <c r="AP33" s="15"/>
+      <c r="AQ33" s="15"/>
+      <c r="AR33" s="15"/>
+      <c r="AS33" s="15"/>
+      <c r="AT33" s="15"/>
+      <c r="AU33" s="15"/>
+      <c r="AV33" s="15"/>
+      <c r="AW33" s="15"/>
+      <c r="AX33" s="15"/>
+      <c r="AY33" s="15"/>
+      <c r="AZ33" s="15"/>
+      <c r="BA33" s="15"/>
+      <c r="BB33" s="15"/>
+      <c r="BC33" s="15"/>
+      <c r="BD33" s="15"/>
+      <c r="BE33" s="15"/>
+      <c r="BF33" s="15"/>
+      <c r="BG33" s="15"/>
+      <c r="BH33" s="15"/>
+      <c r="BI33" s="15"/>
+      <c r="BJ33" s="15"/>
+      <c r="BK33" s="15"/>
+      <c r="BL33" s="15"/>
+      <c r="BM33" s="15"/>
+      <c r="BN33" s="15"/>
+      <c r="BO33" s="15"/>
+      <c r="BP33" s="15"/>
+      <c r="BQ33" s="15"/>
+      <c r="BR33" s="15"/>
+      <c r="BS33" s="15"/>
+      <c r="BT33" s="15"/>
+      <c r="BU33" s="15"/>
+      <c r="BV33" s="15"/>
+      <c r="BW33" s="15"/>
+      <c r="BX33" s="15"/>
+      <c r="BY33" s="15"/>
+      <c r="BZ33" s="15"/>
+      <c r="CA33" s="15"/>
+      <c r="CB33" s="15"/>
+      <c r="CC33" s="15"/>
+      <c r="CD33" s="15"/>
+      <c r="CE33" s="15"/>
+      <c r="CF33" s="15"/>
+      <c r="CG33" s="15"/>
+      <c r="CH33" s="15"/>
+      <c r="CI33" s="15"/>
+      <c r="CJ33" s="15"/>
+      <c r="CK33" s="15"/>
+      <c r="CL33" s="15"/>
+      <c r="CM33" s="15"/>
+      <c r="CN33" s="15"/>
+      <c r="CO33" s="15"/>
+      <c r="CP33" s="15"/>
+      <c r="CQ33" s="15"/>
+    </row>
+    <row r="34" spans="1:95" ht="51" x14ac:dyDescent="0.2">
+      <c r="C34" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="21" t="s">
         <v>10</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="21" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="D19:D24"/>
-    <mergeCell ref="E19:E24"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="F19:F24"/>
-    <mergeCell ref="F7:F12"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="E14:E15"/>
+  <mergeCells count="18">
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D8:D13"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="E23:E29"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="D23:D29"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://datalab.review.fao.org/dailyprices.html" xr:uid="{9BFB1707-3A79-574B-BC47-65C0B4BD0E9C}"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://fews.net/" xr:uid="{84772C4A-4AD9-7840-815D-17F2F6B2D9A0}"/>
-    <hyperlink ref="B7" r:id="rId3" location="/dashboard" display="https://acleddata.com/dashboard/ - /dashboard" xr:uid="{F76E7675-2B2E-2D45-8C2B-2CB43E3D6E32}"/>
-    <hyperlink ref="B9" r:id="rId4" display="https://fragilestatesindex.org/data/" xr:uid="{A9B1CC3D-C0A1-C04F-BBD3-3E6A6BCE7B20}"/>
-    <hyperlink ref="B12" r:id="rId5" display="https://oefdatascience.github.io/REIGN.github.io/" xr:uid="{2AEFFF55-2CCA-7F42-82FE-4DED88CAF0DE}"/>
-    <hyperlink ref="B14" r:id="rId6" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
-    <hyperlink ref="B15" r:id="rId7" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
-    <hyperlink ref="B17" r:id="rId8" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
-    <hyperlink ref="B24" r:id="rId9" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
+    <hyperlink ref="B8" r:id="rId1" location="/dashboard" display="https://acleddata.com/dashboard/ - /dashboard" xr:uid="{F76E7675-2B2E-2D45-8C2B-2CB43E3D6E32}"/>
+    <hyperlink ref="B10" r:id="rId2" display="https://fragilestatesindex.org/data/" xr:uid="{A9B1CC3D-C0A1-C04F-BBD3-3E6A6BCE7B20}"/>
+    <hyperlink ref="B13" r:id="rId3" display="https://oefdatascience.github.io/REIGN.github.io/" xr:uid="{2AEFFF55-2CCA-7F42-82FE-4DED88CAF0DE}"/>
+    <hyperlink ref="B15" r:id="rId4" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
+    <hyperlink ref="B16" r:id="rId5" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
+    <hyperlink ref="B21" r:id="rId6" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
+    <hyperlink ref="B29" r:id="rId7" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
+    <hyperlink ref="B3" r:id="rId8" display="https://fews.net/" xr:uid="{3D674EBD-4EF9-1342-883D-87D2B91B65D7}"/>
+    <hyperlink ref="B6" r:id="rId9" display="https://www.acaps.org/countries" xr:uid="{323C0C04-FA1B-0C4D-B8B5-EB4AF4D1488B}"/>
+    <hyperlink ref="B18" r:id="rId10" xr:uid="{999A8B13-E27C-374A-82CC-F226FAFAE1F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5710,194 +6004,194 @@
   <sheetData>
     <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>118</v>
+        <v>34</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
+      <c r="A2" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="D3" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="44" t="s">
-        <v>119</v>
+        <v>86</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
+      <c r="A4" s="71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
+      <c r="A5" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
+      <c r="A6" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
     </row>
     <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>117</v>
+        <v>95</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>101</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="G7" s="53" t="s">
-        <v>101</v>
+        <v>109</v>
+      </c>
+      <c r="G7" s="49" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="G8" s="54"/>
+      <c r="A8" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="G8" s="50"/>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="E9" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="G9" s="54" t="s">
-        <v>101</v>
+      <c r="E9" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="50" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="G10" s="55"/>
+      <c r="A10" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="G10" s="51"/>
     </row>
     <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="G11" s="54"/>
+        <v>84</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="G11" s="50"/>
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="G12" s="53"/>
+      <c r="A12" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="G12" s="49"/>
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="G13" s="53" t="s">
-        <v>101</v>
+        <v>29</v>
+      </c>
+      <c r="B13" s="37"/>
+      <c r="C13" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="G13" s="49" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
+      <c r="A14" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
     </row>
     <row r="15" spans="1:7" ht="248" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="B15" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" s="50" t="s">
-        <v>121</v>
-      </c>
-      <c r="E15" s="51" t="s">
-        <v>122</v>
-      </c>
-      <c r="F15" s="52" t="s">
-        <v>101</v>
+      <c r="E15" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -5934,55 +6228,55 @@
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.1640625" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" style="36" customWidth="1"/>
+    <col min="3" max="3" width="35.1640625" style="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>59</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>60</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C8" s="37"/>
+      <c r="C8" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update to the XLSX indicator sheet with latest indicators and descriptors
Also an indicator for COVID has been added: H_Oxrollback_score_norm
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9CF8E5-1C0F-D84B-B3AB-51FA8FB896F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BE3BDD-9C8F-AB4A-AC69-73C86F5C40E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3700" yWindow="-21140" windowWidth="38400" windowHeight="17540" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="-3700" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
     <sheet name="Existing Risk" sheetId="3" r:id="rId2"/>
     <sheet name="Total Risk" sheetId="2" r:id="rId3"/>
+    <sheet name="Risk Category Desc." sheetId="4" r:id="rId4"/>
+    <sheet name="Indicator Label" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="196">
   <si>
     <t>Projected Coup risk (REIGN)</t>
   </si>
@@ -289,9 +291,6 @@
   </si>
   <si>
     <t>COVID-19 projected deaths (per 1M) by Nov 2020</t>
-  </si>
-  <si>
-    <t>Oxford Lockdown rollback index (source)</t>
   </si>
   <si>
     <t>COVID RESPONSE</t>
@@ -874,9 +873,6 @@
     <t>H_GovernmentResponseIndexForDisplay</t>
   </si>
   <si>
-    <t>Oxford Government Response Index</t>
-  </si>
-  <si>
     <t>10 &gt; 80
 0 &lt; 15</t>
   </si>
@@ -1065,12 +1061,189 @@
 Note: FS calculated as max values</t>
     </r>
   </si>
+  <si>
+    <t>Risk Category</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Existing/Emerging</t>
+  </si>
+  <si>
+    <t>Indicator Key</t>
+  </si>
+  <si>
+    <t>Indicator Label</t>
+  </si>
+  <si>
+    <t>Existing</t>
+  </si>
+  <si>
+    <t>Proteus Food Security Index</t>
+  </si>
+  <si>
+    <t>Fragility Index (WB)</t>
+  </si>
+  <si>
+    <t>Economic and Financial Dependence</t>
+  </si>
+  <si>
+    <t>Debt Distress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Health Security Index </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seasonal Natural Hazard Risk </t>
+  </si>
+  <si>
+    <t>Vulnerability Index (OCHA)</t>
+  </si>
+  <si>
+    <t>Emerging</t>
+  </si>
+  <si>
+    <t>FEWSNET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARTEMIS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fragile States Index </t>
+  </si>
+  <si>
+    <t>Fragility Index (INFORM)</t>
+  </si>
+  <si>
+    <t>Projected Coup Risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projected COVID deaths </t>
+  </si>
+  <si>
+    <t>H_Covidgrowth_casesnorm,</t>
+  </si>
+  <si>
+    <t>H_Covidgrowth_deathsnorm,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth in COVID deaths </t>
+  </si>
+  <si>
+    <t>H_new_cases_smoothed_per_million_norm,</t>
+  </si>
+  <si>
+    <t>Current new COVID cases</t>
+  </si>
+  <si>
+    <t>H_new_deaths_smoothed_per_million_norm,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current new COVID deaths </t>
+  </si>
+  <si>
+    <t>Government Response Index</t>
+  </si>
+  <si>
+    <t>Economic Support Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_Oxrollback_score_norm, </t>
+  </si>
+  <si>
+    <t>COVID Rollback Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projected Seasonal Hazards </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongoing Crisis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongoign Natural Hazard </t>
+  </si>
+  <si>
+    <t>NH_Hazard_Score_norm</t>
+  </si>
+  <si>
+    <t>Natural multi-hazard rating (INFORM) – 2020 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical rates of exposure and sensitivity to earthquake, tsunami, flood, cyclone, storm surge and drought risk. For more details see link. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GHS is made up of six categories (comrised of 34 indicators, 85 sub-indicators). The categories include: prevention; detection and reporting; rapid response; health system; compliance with international norms; and risk environment. For more details see link. </t>
+  </si>
+  <si>
+    <t>Aggregation primarily achieved through a Principle Components Analysis (PCA) with expert derived weights. See link for more details.</t>
+  </si>
+  <si>
+    <t>Food Prive Volatility</t>
+  </si>
+  <si>
+    <t>Ongoing Food Crisis/Famine</t>
+  </si>
+  <si>
+    <t>% Fiscal Stimulus to GDP</t>
+  </si>
+  <si>
+    <t>COVID Economic Stimulus Index</t>
+  </si>
+  <si>
+    <t>Change in Borrowing/Lending</t>
+  </si>
+  <si>
+    <t>Change in Events (ACLED)</t>
+  </si>
+  <si>
+    <t>Change in Fatalities (ACLED)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongoing Political Crisis </t>
+  </si>
+  <si>
+    <t>Difference in Projected GDP (WB)</t>
+  </si>
+  <si>
+    <t>Difference in Projected GDP (IMF)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth in COVID cases </t>
+  </si>
+  <si>
+    <t>Oxford Government Response Index (Oxford University - Blavatnik)</t>
+  </si>
+  <si>
+    <t>Oxford Lockdown rollback index (Oxford University - Blavatnik, source)</t>
+  </si>
+  <si>
+    <t>A measure of availability and access to food</t>
+  </si>
+  <si>
+    <t>A measure of a country's exposure and resilience to a variety of natural and seasonal hazards, including earthquakes, tsunamis, floods, cyclones, storm surge, pests and drought risk</t>
+  </si>
+  <si>
+    <t>A multi-dimensional measure of socio-economic vulnerability, focused predominantly on household level dynamics</t>
+  </si>
+  <si>
+    <t>A measure of institutional and social fragility as well as likehood of violent conflict</t>
+  </si>
+  <si>
+    <t>A measure of a country's exposure and resilience to macro-economic shock, focused primarily on economic and financial dependence</t>
+  </si>
+  <si>
+    <t>A measure of a country's fiscal risk, focused predominantly on debt burden as well as fiscal stimulus in response to COVID</t>
+  </si>
+  <si>
+    <t>A measure of of a country's response capacity to a pandemic (note: indicators for emerging risk are targetted specifically at COVID-related dynamic)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1173,8 +1346,16 @@
       <name val="Garamond"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1293,6 +1474,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1471,7 +1670,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1573,8 +1772,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1606,86 +1803,8 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1694,39 +1813,226 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2685,8 +2991,8 @@
   </sheetPr>
   <dimension ref="A1:CQ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2718,13 +3024,13 @@
       </c>
     </row>
     <row r="2" spans="1:95" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -2817,20 +3123,20 @@
       <c r="CQ2" s="14"/>
     </row>
     <row r="3" spans="1:95" s="1" customFormat="1" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="75" t="s">
-        <v>137</v>
-      </c>
-      <c r="E3" s="88" t="s">
-        <v>138</v>
+      <c r="C3" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>136</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -2924,17 +3230,17 @@
       <c r="CQ3" s="14"/>
     </row>
     <row r="4" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="50" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="75"/>
-      <c r="E4" s="89"/>
+      <c r="C4" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="69"/>
+      <c r="E4" s="66"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -3027,17 +3333,17 @@
       <c r="CQ4" s="14"/>
     </row>
     <row r="5" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="86" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="87" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="89"/>
+      <c r="A5" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="69"/>
+      <c r="E5" s="66"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -3130,17 +3436,17 @@
       <c r="CQ5" s="14"/>
     </row>
     <row r="6" spans="1:95" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="86" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="85" t="s">
-        <v>118</v>
-      </c>
-      <c r="C6" s="50" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="90"/>
+      <c r="A6" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="69"/>
+      <c r="E6" s="67"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -3232,13 +3538,13 @@
       <c r="CP6" s="14"/>
     </row>
     <row r="7" spans="1:95" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="71"/>
+      <c r="A7" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="61"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -3331,19 +3637,19 @@
     </row>
     <row r="8" spans="1:95" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="77" t="s">
         <v>72</v>
-      </c>
-      <c r="E8" s="66" t="s">
-        <v>73</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -3437,16 +3743,16 @@
     </row>
     <row r="9" spans="1:95" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="67"/>
+        <v>60</v>
+      </c>
+      <c r="D9" s="71"/>
+      <c r="E9" s="78"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -3545,10 +3851,10 @@
         <v>40</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="60"/>
-      <c r="E10" s="67"/>
+        <v>81</v>
+      </c>
+      <c r="D10" s="71"/>
+      <c r="E10" s="78"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -3647,10 +3953,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="67"/>
+        <v>68</v>
+      </c>
+      <c r="D11" s="71"/>
+      <c r="E11" s="78"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -3743,16 +4049,16 @@
     </row>
     <row r="12" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="60"/>
-      <c r="E12" s="67"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="78"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -3851,10 +4157,10 @@
         <v>0</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="61"/>
-      <c r="E13" s="68"/>
+        <v>80</v>
+      </c>
+      <c r="D13" s="72"/>
+      <c r="E13" s="79"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -3946,13 +4252,13 @@
       <c r="CP13" s="14"/>
     </row>
     <row r="14" spans="1:95" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="72" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="73"/>
-      <c r="E14" s="73"/>
+      <c r="A14" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -4050,13 +4356,13 @@
       <c r="B15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="75" t="s">
+      <c r="C15" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="74" t="s">
+      <c r="E15" s="68" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="14"/>
@@ -4156,11 +4462,11 @@
       <c r="B16" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="75"/>
-      <c r="E16" s="74"/>
+      <c r="C16" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="69"/>
+      <c r="E16" s="68"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -4252,13 +4558,13 @@
       <c r="CP16" s="14"/>
     </row>
     <row r="17" spans="1:95" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="70"/>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="71"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="61"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
@@ -4352,22 +4658,22 @@
     </row>
     <row r="18" spans="1:95" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="B18" s="80" t="s">
-        <v>135</v>
-      </c>
-      <c r="C18" s="81" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" s="82" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" s="82" t="s">
+      <c r="E18" s="80" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="14"/>
-      <c r="G18" s="79"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -4459,16 +4765,16 @@
     </row>
     <row r="19" spans="1:95" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" s="76" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="83" t="s">
-        <v>129</v>
-      </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="82"/>
+        <v>132</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" s="81"/>
+      <c r="E19" s="80"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -4562,16 +4868,16 @@
     </row>
     <row r="20" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="83" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" s="77"/>
-      <c r="E20" s="82"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="80"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -4671,10 +4977,10 @@
         <v>43</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="82"/>
+        <v>62</v>
+      </c>
+      <c r="D21" s="81"/>
+      <c r="E21" s="80"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -4767,13 +5073,13 @@
       <c r="CQ21" s="14"/>
     </row>
     <row r="22" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="72" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="78"/>
+      <c r="A22" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -4869,16 +5175,16 @@
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="84" t="s">
+      <c r="B23" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="51" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="58" t="s">
+      <c r="C23" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="65" t="s">
+      <c r="E23" s="76" t="s">
         <v>15</v>
       </c>
       <c r="F23" s="14"/>
@@ -4974,16 +5280,16 @@
     </row>
     <row r="24" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="58"/>
-      <c r="E24" s="65"/>
+      <c r="C24" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="88"/>
+      <c r="E24" s="76"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -5077,19 +5383,19 @@
     </row>
     <row r="25" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="58"/>
-      <c r="E25" s="65"/>
+      <c r="C25" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="88"/>
+      <c r="E25" s="76"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
@@ -5182,16 +5488,16 @@
     </row>
     <row r="26" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="51" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="58"/>
-      <c r="E26" s="65"/>
+      <c r="C26" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="88"/>
+      <c r="E26" s="76"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -5285,16 +5591,16 @@
     </row>
     <row r="27" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="58"/>
-      <c r="E27" s="65"/>
+      <c r="C27" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="88"/>
+      <c r="E27" s="76"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
@@ -5388,16 +5694,16 @@
     </row>
     <row r="28" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C28" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C28" s="51" t="s">
-        <v>124</v>
-      </c>
-      <c r="D28" s="58"/>
-      <c r="E28" s="65"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="76"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
@@ -5491,16 +5797,16 @@
     </row>
     <row r="29" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" s="58"/>
-      <c r="E29" s="65"/>
+        <v>188</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="88"/>
+      <c r="E29" s="76"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
@@ -5593,13 +5899,13 @@
       <c r="CQ29" s="14"/>
     </row>
     <row r="30" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="62" t="s">
+      <c r="A30" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="64"/>
+      <c r="B30" s="74"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="75"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -5696,16 +6002,16 @@
         <v>28</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="85" t="s">
         <v>74</v>
-      </c>
-      <c r="E31" s="55" t="s">
-        <v>75</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -5806,10 +6112,10 @@
         <v>5</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="53"/>
-      <c r="E32" s="56"/>
+        <v>69</v>
+      </c>
+      <c r="D32" s="83"/>
+      <c r="E32" s="86"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -5911,8 +6217,8 @@
       <c r="C33" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="54"/>
-      <c r="E33" s="57"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="87"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
@@ -6017,6 +6323,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="D23:D29"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="E23:E29"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A17:E17"/>
@@ -6027,14 +6341,6 @@
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="D8:D13"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="E23:E29"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="D23:D29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -6060,13 +6366,13 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView zoomScale="81" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.5" customWidth="1"/>
+    <col min="1" max="1" width="41.5" style="109" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="4" max="4" width="62.33203125" customWidth="1"/>
@@ -6074,7 +6380,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="103" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -6084,185 +6390,194 @@
         <v>33</v>
       </c>
       <c r="D1" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="104" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+    </row>
+    <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="105" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="111" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="111"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+    </row>
+    <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="106" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="29" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-    </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-    </row>
-    <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-    </row>
-    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="72" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-    </row>
-    <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="15" t="s">
+      <c r="E7" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="G7" s="47" t="s">
-        <v>84</v>
+      <c r="G7" s="45" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="G8" s="48"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="G8" s="46"/>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="G10" s="47"/>
+    </row>
+    <row r="11" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" s="107" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="100" t="s">
+        <v>174</v>
+      </c>
+      <c r="E11" s="101" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" s="102"/>
+      <c r="G11" s="46"/>
+    </row>
+    <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="74"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="G12" s="45"/>
+    </row>
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="95" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="97" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="99" t="s">
+        <v>173</v>
+      </c>
+      <c r="E13" s="35"/>
+      <c r="G13" s="45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="73" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+    </row>
+    <row r="15" spans="1:7" ht="248" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="108" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="28" t="s">
+      <c r="B15" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="G9" s="48" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="72" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="G10" s="49"/>
-    </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="E15" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" s="44" t="s">
         <v>83</v>
-      </c>
-      <c r="B11" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="G11" s="48"/>
-    </row>
-    <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="62" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="G12" s="47"/>
-    </row>
-    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="G13" s="47" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-    </row>
-    <row r="15" spans="1:7" ht="248" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="F15" s="46" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -6278,9 +6593,12 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="WFP Proteus composite index: " xr:uid="{3B8342E4-A803-C342-923C-31BDAA92A373}"/>
     <hyperlink ref="B11" r:id="rId2" xr:uid="{95E245AA-F0BF-3C40-B212-C5EC3EDEDF2E}"/>
+    <hyperlink ref="D13" r:id="rId3" location=":~:text=INFORM%20Index%20for%20Risk%20Management%3A%20Concept%20and%20Methodology%2C%20Version%202017,-%C2%A9EU&amp;text=INFORM%20is%20a%20composite%20indicator,crisis%20and%20disaster%20management%20framework." xr:uid="{AF872891-F870-AA4C-B416-4F92600B17AE}"/>
+    <hyperlink ref="D11" r:id="rId4" xr:uid="{26B58F35-C97D-3F48-B110-F642D3427351}"/>
+    <hyperlink ref="E11" r:id="rId5" xr:uid="{2B1483A5-6E05-4E4E-A8CB-95D622233E3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -6292,7 +6610,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6304,46 +6622,46 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="22" t="s">
         <v>55</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -6352,4 +6670,605 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E658424-6FDF-FB4F-A908-E363FB27277D}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="46.5" customWidth="1"/>
+    <col min="2" max="2" width="53.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="89" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="112" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B8">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
+      <formula>LEN(TRIM(B2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FAE3D5-1E62-BD47-A72D-971150914E15}">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.5" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
+    <col min="6" max="6" width="37.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="89" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="89" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="89" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="90" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="91"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="92" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="90" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="95" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="96" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="110" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="110" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" t="s">
+        <v>154</v>
+      </c>
+      <c r="F17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D28" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D2:D34">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(D2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Indicator Aggregation xlsx with Fr_INFORM_CRISIS_Type
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BE3BDD-9C8F-AB4A-AC69-73C86F5C40E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F89335-BAC3-364A-8A67-1D42657E86EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3700" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="-4640" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="4" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -225,9 +225,6 @@
   </si>
   <si>
     <t>Fr_REIGN_couprisk3m_norm</t>
-  </si>
-  <si>
-    <t>NH_INFORM_CRISIS_Type</t>
   </si>
   <si>
     <t>M_GDP_IMF_2019minus2020_norm</t>
@@ -1237,6 +1234,9 @@
   </si>
   <si>
     <t>A measure of of a country's response capacity to a pandemic (note: indicators for emerging risk are targetted specifically at COVID-related dynamic)</t>
+  </si>
+  <si>
+    <t>Fr_INFORM_CRISIS_Type</t>
   </si>
 </sst>
 </file>
@@ -1828,96 +1828,6 @@
     <xf numFmtId="0" fontId="3" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1982,6 +1892,96 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2991,8 +2991,8 @@
   </sheetPr>
   <dimension ref="A1:CQ34"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A2" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3014,7 +3014,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" s="29" t="s">
         <v>7</v>
@@ -3024,13 +3024,13 @@
       </c>
     </row>
     <row r="2" spans="1:95" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="61"/>
+      <c r="A2" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="101"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -3127,16 +3127,16 @@
         <v>20</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="69" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="109" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="105" t="s">
         <v>135</v>
-      </c>
-      <c r="E3" s="65" t="s">
-        <v>136</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -3234,13 +3234,13 @@
         <v>19</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="69"/>
-      <c r="E4" s="66"/>
+        <v>117</v>
+      </c>
+      <c r="D4" s="109"/>
+      <c r="E4" s="106"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -3334,16 +3334,16 @@
     </row>
     <row r="5" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="69"/>
-      <c r="E5" s="66"/>
+        <v>118</v>
+      </c>
+      <c r="D5" s="109"/>
+      <c r="E5" s="106"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -3437,16 +3437,16 @@
     </row>
     <row r="6" spans="1:95" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="67"/>
+        <v>119</v>
+      </c>
+      <c r="D6" s="109"/>
+      <c r="E6" s="107"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -3538,13 +3538,13 @@
       <c r="CP6" s="14"/>
     </row>
     <row r="7" spans="1:95" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="59" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="61"/>
+      <c r="A7" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="100"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="101"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -3637,19 +3637,19 @@
     </row>
     <row r="8" spans="1:95" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="110" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="94" t="s">
         <v>71</v>
-      </c>
-      <c r="E8" s="77" t="s">
-        <v>72</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -3743,16 +3743,16 @@
     </row>
     <row r="9" spans="1:95" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="71"/>
-      <c r="E9" s="78"/>
+        <v>59</v>
+      </c>
+      <c r="D9" s="111"/>
+      <c r="E9" s="95"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -3848,13 +3848,13 @@
         <v>21</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="71"/>
-      <c r="E10" s="78"/>
+        <v>80</v>
+      </c>
+      <c r="D10" s="111"/>
+      <c r="E10" s="95"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -3947,16 +3947,16 @@
     </row>
     <row r="11" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>23</v>
+        <v>195</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="78"/>
+        <v>67</v>
+      </c>
+      <c r="D11" s="111"/>
+      <c r="E11" s="95"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -4049,16 +4049,16 @@
     </row>
     <row r="12" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="78"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="95"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -4157,10 +4157,10 @@
         <v>0</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="79"/>
+        <v>79</v>
+      </c>
+      <c r="D13" s="112"/>
+      <c r="E13" s="96"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -4252,13 +4252,13 @@
       <c r="CP13" s="14"/>
     </row>
     <row r="14" spans="1:95" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
+      <c r="A14" s="102" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="104"/>
+      <c r="C14" s="104"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="104"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -4351,18 +4351,18 @@
     </row>
     <row r="15" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="68" t="s">
+      <c r="E15" s="108" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="14"/>
@@ -4457,16 +4457,16 @@
     </row>
     <row r="16" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="69"/>
-      <c r="E16" s="68"/>
+        <v>60</v>
+      </c>
+      <c r="D16" s="109"/>
+      <c r="E16" s="108"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -4558,13 +4558,13 @@
       <c r="CP16" s="14"/>
     </row>
     <row r="17" spans="1:95" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="59" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="61"/>
+      <c r="A17" s="99" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="100"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="101"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
@@ -4658,18 +4658,18 @@
     </row>
     <row r="18" spans="1:95" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="B18" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="C18" s="53" t="s">
+      <c r="D18" s="97" t="s">
         <v>129</v>
       </c>
-      <c r="D18" s="80" t="s">
-        <v>130</v>
-      </c>
-      <c r="E18" s="80" t="s">
+      <c r="E18" s="97" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="14"/>
@@ -4765,16 +4765,16 @@
     </row>
     <row r="19" spans="1:95" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B19" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="D19" s="81"/>
-      <c r="E19" s="80"/>
+      <c r="D19" s="98"/>
+      <c r="E19" s="97"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -4868,16 +4868,16 @@
     </row>
     <row r="20" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="C20" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="C20" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" s="81"/>
-      <c r="E20" s="80"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="97"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -4971,16 +4971,16 @@
     </row>
     <row r="21" spans="1:95" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="81"/>
-      <c r="E21" s="80"/>
+        <v>61</v>
+      </c>
+      <c r="D21" s="98"/>
+      <c r="E21" s="97"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -5073,13 +5073,13 @@
       <c r="CQ21" s="14"/>
     </row>
     <row r="22" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
+      <c r="A22" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="103"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="103"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -5173,18 +5173,18 @@
     </row>
     <row r="23" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="76" t="s">
+      <c r="E23" s="93" t="s">
         <v>15</v>
       </c>
       <c r="F23" s="14"/>
@@ -5280,16 +5280,16 @@
     </row>
     <row r="24" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="88"/>
-      <c r="E24" s="76"/>
+        <v>63</v>
+      </c>
+      <c r="D24" s="89"/>
+      <c r="E24" s="93"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -5383,19 +5383,19 @@
     </row>
     <row r="25" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="88"/>
-      <c r="E25" s="76"/>
+        <v>63</v>
+      </c>
+      <c r="D25" s="89"/>
+      <c r="E25" s="93"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
@@ -5488,16 +5488,16 @@
     </row>
     <row r="26" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="88"/>
-      <c r="E26" s="76"/>
+        <v>64</v>
+      </c>
+      <c r="D26" s="89"/>
+      <c r="E26" s="93"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -5591,16 +5591,16 @@
     </row>
     <row r="27" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" s="88"/>
-      <c r="E27" s="76"/>
+        <v>65</v>
+      </c>
+      <c r="D27" s="89"/>
+      <c r="E27" s="93"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
@@ -5694,16 +5694,16 @@
     </row>
     <row r="28" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="C28" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="D28" s="88"/>
-      <c r="E28" s="76"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="93"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
@@ -5797,16 +5797,16 @@
     </row>
     <row r="29" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="88"/>
-      <c r="E29" s="76"/>
+        <v>66</v>
+      </c>
+      <c r="D29" s="89"/>
+      <c r="E29" s="93"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
@@ -5899,13 +5899,13 @@
       <c r="CQ29" s="14"/>
     </row>
     <row r="30" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="75"/>
+      <c r="A30" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="91"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="92"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -5999,19 +5999,19 @@
     </row>
     <row r="31" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="83" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="86" t="s">
         <v>73</v>
-      </c>
-      <c r="E31" s="85" t="s">
-        <v>74</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -6106,16 +6106,16 @@
     </row>
     <row r="32" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="83"/>
-      <c r="E32" s="86"/>
+        <v>68</v>
+      </c>
+      <c r="D32" s="84"/>
+      <c r="E32" s="87"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -6209,16 +6209,16 @@
     </row>
     <row r="33" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" s="84"/>
-      <c r="E33" s="87"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="88"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
@@ -6323,17 +6323,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="D23:D29"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="E23:E29"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A17:E17"/>
     <mergeCell ref="A22:E22"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="E3:E6"/>
@@ -6341,6 +6330,17 @@
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="D8:D13"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="D23:D29"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="E23:E29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -6372,7 +6372,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.5" style="109" customWidth="1"/>
+    <col min="1" max="1" width="41.5" style="79" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="4" max="4" width="62.33203125" customWidth="1"/>
@@ -6380,204 +6380,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="73" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+    </row>
+    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="99" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+    </row>
+    <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="75" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="81" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="102" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+    </row>
+    <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="29" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="59" t="s">
+      <c r="E7" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-    </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="104" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="59" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-    </row>
-    <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="105" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="111" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-    </row>
-    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-    </row>
-    <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="106" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" s="45" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
       <c r="G8" s="46"/>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="102" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="104"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="G10" s="47"/>
+    </row>
+    <row r="11" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="37" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" s="46" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="G10" s="47"/>
-    </row>
-    <row r="11" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="107" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>95</v>
-      </c>
       <c r="C11" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="70" t="s">
+        <v>173</v>
+      </c>
+      <c r="E11" s="71" t="s">
         <v>174</v>
       </c>
-      <c r="E11" s="101" t="s">
-        <v>175</v>
-      </c>
-      <c r="F11" s="102"/>
+      <c r="F11" s="72"/>
       <c r="G11" s="46"/>
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
+      <c r="A12" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
       <c r="G12" s="45"/>
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="65" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="67" t="s">
         <v>171</v>
       </c>
-      <c r="B13" s="97" t="s">
+      <c r="C13" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="69" t="s">
         <v>172</v>
-      </c>
-      <c r="C13" s="98" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" s="99" t="s">
-        <v>173</v>
       </c>
       <c r="E13" s="35"/>
       <c r="G13" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="73" t="s">
-        <v>89</v>
-      </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
+      <c r="A14" s="90" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="91"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
     </row>
     <row r="15" spans="1:7" ht="248" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="108" t="s">
-        <v>87</v>
+      <c r="A15" s="78" t="s">
+        <v>86</v>
       </c>
       <c r="B15" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="42" t="s">
-        <v>97</v>
-      </c>
       <c r="D15" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="43" t="s">
-        <v>104</v>
-      </c>
       <c r="F15" s="44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -6622,46 +6622,46 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="22" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -6676,7 +6676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E658424-6FDF-FB4F-A908-E363FB27277D}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -6687,72 +6687,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="59" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>137</v>
-      </c>
-      <c r="B1" s="89" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="53" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="112" t="s">
-        <v>83</v>
+      <c r="B24" s="82" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -6769,8 +6769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FAE3D5-1E62-BD47-A72D-971150914E15}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6784,483 +6784,483 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="59" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="89" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" s="89" t="s">
+      <c r="D1" s="59" t="s">
         <v>140</v>
-      </c>
-      <c r="D1" s="89" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
         <v>142</v>
       </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="90" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="91"/>
+      <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="92" t="s">
-        <v>88</v>
+        <v>69</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="93" t="s">
-        <v>85</v>
+        <v>45</v>
+      </c>
+      <c r="C4" s="63" t="s">
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="94" t="s">
-        <v>86</v>
+        <v>34</v>
+      </c>
+      <c r="C5" s="64" t="s">
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="90" t="s">
-        <v>82</v>
+        <v>44</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="95" t="s">
-        <v>171</v>
+        <v>35</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="96" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="110" t="s">
-        <v>177</v>
+        <v>114</v>
+      </c>
+      <c r="D9" s="80" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="110" t="s">
-        <v>176</v>
+        <v>113</v>
+      </c>
+      <c r="D10" s="80" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>23</v>
+        <v>195</v>
       </c>
       <c r="D16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C27" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27" t="s">
         <v>158</v>
-      </c>
-      <c r="D27" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D28" t="s">
         <v>160</v>
-      </c>
-      <c r="D28" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" t="s">
         <v>162</v>
-      </c>
-      <c r="D29" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D31" t="s">
         <v>166</v>
-      </c>
-      <c r="D31" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update R scripts to include Fr_INFORM_CRISIS_Norm
Changes Indicator xlsx sheet with new variable names
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F89335-BAC3-364A-8A67-1D42657E86EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAB4A8F-F0C7-4D4D-B84B-E8ED0ECB7C84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4640" yWindow="-21140" windowWidth="38400" windowHeight="21140" activeTab="4" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -515,9 +515,6 @@
   <si>
     <t xml:space="preserve">10 &lt;  pct
 0 &gt; 90 pct </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10 = Ongoing complex crisis</t>
   </si>
   <si>
     <t xml:space="preserve"> 10 = Ongoing Natural Hazard Crisis</t>
@@ -1236,7 +1233,11 @@
     <t>A measure of of a country's response capacity to a pandemic (note: indicators for emerging risk are targetted specifically at COVID-related dynamic)</t>
   </si>
   <si>
-    <t>Fr_INFORM_CRISIS_Type</t>
+    <t>Fr_INFORM_CRISIS_Norm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10 = Ongoing complex crisis
+0 = if no ongoing crisis </t>
   </si>
 </sst>
 </file>
@@ -2991,8 +2992,8 @@
   </sheetPr>
   <dimension ref="A1:CQ34"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3130,13 +3131,13 @@
         <v>36</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="109" t="s">
+        <v>133</v>
+      </c>
+      <c r="E3" s="105" t="s">
         <v>134</v>
-      </c>
-      <c r="E3" s="105" t="s">
-        <v>135</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -3237,7 +3238,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" s="109"/>
       <c r="E4" s="106"/>
@@ -3334,13 +3335,13 @@
     </row>
     <row r="5" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="109"/>
       <c r="E5" s="106"/>
@@ -3437,13 +3438,13 @@
     </row>
     <row r="6" spans="1:95" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" s="109"/>
       <c r="E6" s="107"/>
@@ -3539,7 +3540,7 @@
     </row>
     <row r="7" spans="1:95" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="99" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="100"/>
       <c r="C7" s="100"/>
@@ -3637,7 +3638,7 @@
     </row>
     <row r="8" spans="1:95" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>38</v>
@@ -3646,10 +3647,10 @@
         <v>58</v>
       </c>
       <c r="D8" s="110" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="94" t="s">
         <v>70</v>
-      </c>
-      <c r="E8" s="94" t="s">
-        <v>71</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -3743,10 +3744,10 @@
     </row>
     <row r="9" spans="1:95" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>59</v>
@@ -3851,7 +3852,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="111"/>
       <c r="E10" s="95"/>
@@ -3945,15 +3946,15 @@
       <c r="CO10" s="14"/>
       <c r="CP10" s="14"/>
     </row>
-    <row r="11" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:95" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>67</v>
+        <v>195</v>
       </c>
       <c r="D11" s="111"/>
       <c r="E11" s="95"/>
@@ -4049,13 +4050,13 @@
     </row>
     <row r="12" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="34" t="s">
         <v>78</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>79</v>
       </c>
       <c r="D12" s="111"/>
       <c r="E12" s="95"/>
@@ -4157,7 +4158,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="112"/>
       <c r="E13" s="96"/>
@@ -4658,16 +4659,16 @@
     </row>
     <row r="18" spans="1:95" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="52" t="s">
-        <v>132</v>
-      </c>
-      <c r="C18" s="53" t="s">
+      <c r="D18" s="97" t="s">
         <v>128</v>
-      </c>
-      <c r="D18" s="97" t="s">
-        <v>129</v>
       </c>
       <c r="E18" s="97" t="s">
         <v>13</v>
@@ -4765,13 +4766,13 @@
     </row>
     <row r="19" spans="1:95" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B19" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="54" t="s">
         <v>125</v>
-      </c>
-      <c r="C19" s="54" t="s">
-        <v>126</v>
       </c>
       <c r="D19" s="98"/>
       <c r="E19" s="97"/>
@@ -4868,13 +4869,13 @@
     </row>
     <row r="20" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="C20" s="54" t="s">
         <v>123</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>124</v>
       </c>
       <c r="D20" s="98"/>
       <c r="E20" s="97"/>
@@ -5280,7 +5281,7 @@
     </row>
     <row r="24" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>1</v>
@@ -5383,7 +5384,7 @@
     </row>
     <row r="25" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>2</v>
@@ -5395,7 +5396,7 @@
       <c r="E25" s="93"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
@@ -5488,7 +5489,7 @@
     </row>
     <row r="26" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>3</v>
@@ -5591,7 +5592,7 @@
     </row>
     <row r="27" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>4</v>
@@ -5694,13 +5695,13 @@
     </row>
     <row r="28" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" s="49" t="s">
         <v>120</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C28" s="49" t="s">
-        <v>121</v>
       </c>
       <c r="D28" s="89"/>
       <c r="E28" s="93"/>
@@ -5797,10 +5798,10 @@
     </row>
     <row r="29" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C29" s="49" t="s">
         <v>66</v>
@@ -6002,16 +6003,16 @@
         <v>27</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C31" s="23" t="s">
         <v>66</v>
       </c>
       <c r="D31" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="86" t="s">
         <v>72</v>
-      </c>
-      <c r="E31" s="86" t="s">
-        <v>73</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -6112,7 +6113,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D32" s="84"/>
       <c r="E32" s="87"/>
@@ -6390,10 +6391,10 @@
         <v>32</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6406,24 +6407,24 @@
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="99" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="100"/>
       <c r="C4" s="100"/>
@@ -6431,10 +6432,10 @@
     </row>
     <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="75" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="81"/>
       <c r="D5" s="81"/>
@@ -6450,22 +6451,22 @@
     </row>
     <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>106</v>
-      </c>
       <c r="G7" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6479,22 +6480,22 @@
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -6508,19 +6509,19 @@
     </row>
     <row r="11" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="71" t="s">
         <v>173</v>
-      </c>
-      <c r="E11" s="71" t="s">
-        <v>174</v>
       </c>
       <c r="F11" s="72"/>
       <c r="G11" s="46"/>
@@ -6536,25 +6537,25 @@
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="65" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="67" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="C13" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="69" t="s">
         <v>171</v>
-      </c>
-      <c r="C13" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" s="69" t="s">
-        <v>172</v>
       </c>
       <c r="E13" s="35"/>
       <c r="G13" s="45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="91"/>
       <c r="C14" s="91"/>
@@ -6562,22 +6563,22 @@
     </row>
     <row r="15" spans="1:7" ht="248" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="78" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="42" t="s">
-        <v>96</v>
-      </c>
       <c r="D15" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="43" t="s">
-        <v>103</v>
-      </c>
       <c r="F15" s="44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -6688,10 +6689,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="59" t="s">
         <v>136</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -6699,15 +6700,15 @@
         <v>33</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -6715,7 +6716,7 @@
         <v>45</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -6723,7 +6724,7 @@
         <v>34</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
@@ -6731,7 +6732,7 @@
         <v>44</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="53" customHeight="1" x14ac:dyDescent="0.2">
@@ -6739,20 +6740,20 @@
         <v>35</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="82" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -6770,7 +6771,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6785,148 +6786,148 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="59" t="s">
+      <c r="D1" s="59" t="s">
         <v>139</v>
-      </c>
-      <c r="D1" s="59" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B7" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D9" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10" s="80" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -6935,12 +6936,12 @@
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
@@ -6949,99 +6950,99 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B19" t="s">
         <v>45</v>
@@ -7050,12 +7051,12 @@
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B20" t="s">
         <v>45</v>
@@ -7064,54 +7065,54 @@
         <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B22" t="s">
         <v>34</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B24" t="s">
         <v>34</v>
@@ -7120,12 +7121,12 @@
         <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
@@ -7134,96 +7135,96 @@
         <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B26" t="s">
         <v>44</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D26" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B27" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" t="s">
         <v>157</v>
-      </c>
-      <c r="D27" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B28" t="s">
         <v>44</v>
       </c>
       <c r="C28" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D28" t="s">
         <v>159</v>
-      </c>
-      <c r="D28" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B29" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D29" t="s">
         <v>161</v>
-      </c>
-      <c r="D29" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B30" t="s">
         <v>44</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B31" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" t="s">
         <v>165</v>
-      </c>
-      <c r="D31" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
@@ -7232,12 +7233,12 @@
         <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
@@ -7246,12 +7247,12 @@
         <v>28</v>
       </c>
       <c r="D33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -7260,7 +7261,7 @@
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new covid projections (cov_forcast_alt)
Changing some of the thresholds for fragility
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAB4A8F-F0C7-4D4D-B84B-E8ED0ECB7C84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B220EAB5-1986-D54F-ACD8-D147D06E5F92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="197">
   <si>
     <t>Projected Coup risk (REIGN)</t>
   </si>
@@ -1230,14 +1230,17 @@
     <t>A measure of a country's fiscal risk, focused predominantly on debt burden as well as fiscal stimulus in response to COVID</t>
   </si>
   <si>
-    <t>A measure of of a country's response capacity to a pandemic (note: indicators for emerging risk are targetted specifically at COVID-related dynamic)</t>
-  </si>
-  <si>
     <t>Fr_INFORM_CRISIS_Norm</t>
   </si>
   <si>
     <t xml:space="preserve"> 10 = Ongoing complex crisis
 0 = if no ongoing crisis </t>
+  </si>
+  <si>
+    <t>COVID/PANDEMIC RISK</t>
+  </si>
+  <si>
+    <t>A measure of a country's exposure and response capacity to pandemic (note: indicators for emerging risk are targetted specifically at COVID-related dynamics)</t>
   </si>
 </sst>
 </file>
@@ -2992,7 +2995,7 @@
   </sheetPr>
   <dimension ref="A1:CQ34"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
       <selection activeCell="D8" sqref="D8:D13"/>
     </sheetView>
   </sheetViews>
@@ -3948,13 +3951,13 @@
     </row>
     <row r="11" spans="1:95" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D11" s="111"/>
       <c r="E11" s="95"/>
@@ -6677,7 +6680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E658424-6FDF-FB4F-A908-E363FB27277D}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -6729,10 +6732,10 @@
     </row>
     <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>195</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="53" customHeight="1" x14ac:dyDescent="0.2">
@@ -6770,7 +6773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FAE3D5-1E62-BD47-A72D-971150914E15}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -7003,7 +7006,7 @@
         <v>68</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D16" t="s">
         <v>181</v>

</xml_diff>

<commit_message>
Edits to indicator aggregation xls
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B220EAB5-1986-D54F-ACD8-D147D06E5F92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E0EB55-106D-9A4A-B5A3-DC0AB17128FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="3" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="193">
   <si>
     <t>Projected Coup risk (REIGN)</t>
   </si>
@@ -221,9 +221,6 @@
     <t>F_Fewsnet_Score_norm</t>
   </si>
   <si>
-    <t>Fr_FSI_2019minus2020_norm</t>
-  </si>
-  <si>
     <t>Fr_REIGN_couprisk3m_norm</t>
   </si>
   <si>
@@ -236,9 +233,6 @@
     <t>D_IMF_debt2020.2019_norm</t>
   </si>
   <si>
-    <t>H_Covidproj_Projected_Deaths_._1M_norm</t>
-  </si>
-  <si>
     <t>NH_UKMO_TOTAL.RISK.NEXT.6.MONTHS_norm</t>
   </si>
   <si>
@@ -275,9 +269,6 @@
     <t>Growth in reported number of conflict events (ACLED) – number of events in the prior month relative the same period last year  (source)</t>
   </si>
   <si>
-    <t>Change in Fragility (relative to 2019) (source)</t>
-  </si>
-  <si>
     <t>Change in forecast GDP growth: 2020 – 2019 (WB Global Economic Prospects) (source)</t>
   </si>
   <si>
@@ -285,9 +276,6 @@
   </si>
   <si>
     <t>Change in forecast government net lending/borrowing: 2020 – 2019 (IMF World Economic Outlook) (source)</t>
-  </si>
-  <si>
-    <t>COVID-19 projected deaths (per 1M) by Nov 2020</t>
   </si>
   <si>
     <t>COVID RESPONSE</t>
@@ -495,10 +483,6 @@
   <si>
     <t>10 &lt; -5
 0 &gt; 0</t>
-  </si>
-  <si>
-    <t>10 &gt; 80 pct
-0 &lt;  pct</t>
   </si>
   <si>
     <t xml:space="preserve">10 &gt; 150 
@@ -702,10 +686,6 @@
 0 &gt; 5 pct</t>
   </si>
   <si>
-    <t>10 &lt; 90 pct 
-0 &gt; 10 pct</t>
-  </si>
-  <si>
     <t>H_HIS_Score_norm</t>
   </si>
   <si>
@@ -716,15 +696,6 @@
   </si>
   <si>
     <t>M_Economic_and_Financial_score_norm</t>
-  </si>
-  <si>
-    <t>D_WB_Overall_debt_distress_norm</t>
-  </si>
-  <si>
-    <t>S_OCHA_Covid.vulnerability.index_norm</t>
-  </si>
-  <si>
-    <t>Fr_WB_structural_norm</t>
   </si>
   <si>
     <t>SOCIOECONOMIC VULNERABILITY RISK</t>
@@ -1092,9 +1063,6 @@
     <t xml:space="preserve">Seasonal Natural Hazard Risk </t>
   </si>
   <si>
-    <t>Vulnerability Index (OCHA)</t>
-  </si>
-  <si>
     <t>Emerging</t>
   </si>
   <si>
@@ -1102,9 +1070,6 @@
   </si>
   <si>
     <t xml:space="preserve">ARTEMIS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fragile States Index </t>
   </si>
   <si>
     <t>Fragility Index (INFORM)</t>
@@ -1241,6 +1206,28 @@
   </si>
   <si>
     <t>A measure of a country's exposure and response capacity to pandemic (note: indicators for emerging risk are targetted specifically at COVID-related dynamics)</t>
+  </si>
+  <si>
+    <t>S_INFORM_vul_norm</t>
+  </si>
+  <si>
+    <t>Socio-economic Vulnerability Index (INFORM)</t>
+  </si>
+  <si>
+    <t>D_WB_external_debt_distress_norm</t>
+  </si>
+  <si>
+    <t>Fr_number_flags_norm</t>
+  </si>
+  <si>
+    <t>H_add_death_prec_current_norm</t>
+  </si>
+  <si>
+    <t>8-week COVID-19 projected deaths as a percentage of current deaths (USC)</t>
+  </si>
+  <si>
+    <t>10 &gt; 100 pct
+0 &lt;  pct</t>
   </si>
 </sst>
 </file>
@@ -1674,7 +1661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1839,13 +1826,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1876,9 +1857,6 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1896,6 +1874,63 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1929,62 +1964,8 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2993,10 +2974,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:CQ34"/>
+  <dimension ref="A1:CQ33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:D13"/>
+    <sheetView topLeftCell="A18" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3018,7 +2999,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="29" t="s">
         <v>7</v>
@@ -3028,13 +3009,13 @@
       </c>
     </row>
     <row r="2" spans="1:95" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="99" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="101"/>
+      <c r="A2" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="98"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -3131,16 +3112,16 @@
         <v>20</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="109" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" s="105" t="s">
-        <v>134</v>
+        <v>102</v>
+      </c>
+      <c r="D3" s="87" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="83" t="s">
+        <v>125</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -3238,13 +3219,13 @@
         <v>19</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="109"/>
-      <c r="E4" s="106"/>
+        <v>107</v>
+      </c>
+      <c r="D4" s="87"/>
+      <c r="E4" s="84"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -3338,16 +3319,16 @@
     </row>
     <row r="5" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>117</v>
-      </c>
-      <c r="D5" s="109"/>
-      <c r="E5" s="106"/>
+        <v>108</v>
+      </c>
+      <c r="D5" s="87"/>
+      <c r="E5" s="84"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -3441,16 +3422,16 @@
     </row>
     <row r="6" spans="1:95" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="109"/>
-      <c r="E6" s="107"/>
+        <v>109</v>
+      </c>
+      <c r="D6" s="87"/>
+      <c r="E6" s="85"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -3542,13 +3523,13 @@
       <c r="CP6" s="14"/>
     </row>
     <row r="7" spans="1:95" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="99" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="100"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="101"/>
+      <c r="A7" s="96" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="97"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="98"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -3641,19 +3622,19 @@
     </row>
     <row r="8" spans="1:95" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="110" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="94" t="s">
-        <v>70</v>
+        <v>54</v>
+      </c>
+      <c r="D8" s="88" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="91" t="s">
+        <v>65</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -3747,16 +3728,16 @@
     </row>
     <row r="9" spans="1:95" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="111"/>
-      <c r="E9" s="95"/>
+        <v>55</v>
+      </c>
+      <c r="D9" s="89"/>
+      <c r="E9" s="92"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -3847,18 +3828,18 @@
       <c r="CO9" s="14"/>
       <c r="CP9" s="14"/>
     </row>
-    <row r="10" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:95" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="111"/>
-      <c r="E10" s="95"/>
+        <v>183</v>
+      </c>
+      <c r="D10" s="89"/>
+      <c r="E10" s="92"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -3949,18 +3930,18 @@
       <c r="CO10" s="14"/>
       <c r="CP10" s="14"/>
     </row>
-    <row r="11" spans="1:95" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>194</v>
-      </c>
-      <c r="D11" s="111"/>
-      <c r="E11" s="95"/>
+        <v>73</v>
+      </c>
+      <c r="D11" s="89"/>
+      <c r="E11" s="92"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -4053,16 +4034,16 @@
     </row>
     <row r="12" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="111"/>
-      <c r="E12" s="95"/>
+        <v>73</v>
+      </c>
+      <c r="D12" s="90"/>
+      <c r="E12" s="93"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -4153,18 +4134,14 @@
       <c r="CO12" s="14"/>
       <c r="CP12" s="14"/>
     </row>
-    <row r="13" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="112"/>
-      <c r="E13" s="96"/>
+    <row r="13" spans="1:95" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="80" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="82"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -4255,14 +4232,22 @@
       <c r="CO13" s="14"/>
       <c r="CP13" s="14"/>
     </row>
-    <row r="14" spans="1:95" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="102" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="104"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="104"/>
-      <c r="E14" s="104"/>
+    <row r="14" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="86" t="s">
+        <v>12</v>
+      </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -4353,22 +4338,18 @@
       <c r="CO14" s="14"/>
       <c r="CP14" s="14"/>
     </row>
-    <row r="15" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="109" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="108" t="s">
-        <v>12</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D15" s="87"/>
+      <c r="E15" s="86"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
@@ -4459,18 +4440,14 @@
       <c r="CO15" s="14"/>
       <c r="CP15" s="14"/>
     </row>
-    <row r="16" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="109"/>
-      <c r="E16" s="108"/>
+    <row r="16" spans="1:95" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="96" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="97"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="98"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -4560,17 +4537,26 @@
       <c r="CN16" s="14"/>
       <c r="CO16" s="14"/>
       <c r="CP16" s="14"/>
-    </row>
-    <row r="17" spans="1:95" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="100"/>
-      <c r="C17" s="100"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="101"/>
+      <c r="CQ16" s="14"/>
+    </row>
+    <row r="17" spans="1:95" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="94" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" s="94" t="s">
+        <v>13</v>
+      </c>
       <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="G17" s="51"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -4660,24 +4646,20 @@
       <c r="CP17" s="14"/>
       <c r="CQ17" s="14"/>
     </row>
-    <row r="18" spans="1:95" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:95" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" s="52" t="s">
-        <v>131</v>
-      </c>
-      <c r="C18" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="D18" s="97" t="s">
-        <v>128</v>
-      </c>
-      <c r="E18" s="97" t="s">
-        <v>13</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="95"/>
+      <c r="E18" s="94"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="51"/>
+      <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -4767,18 +4749,18 @@
       <c r="CP18" s="14"/>
       <c r="CQ18" s="14"/>
     </row>
-    <row r="19" spans="1:95" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="98"/>
-      <c r="E19" s="97"/>
+        <v>114</v>
+      </c>
+      <c r="D19" s="95"/>
+      <c r="E19" s="94"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -4870,18 +4852,18 @@
       <c r="CP19" s="14"/>
       <c r="CQ19" s="14"/>
     </row>
-    <row r="20" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:95" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="B20" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="98"/>
-      <c r="E20" s="97"/>
+        <v>24</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="95"/>
+      <c r="E20" s="94"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -4973,18 +4955,14 @@
       <c r="CP20" s="14"/>
       <c r="CQ20" s="14"/>
     </row>
-    <row r="21" spans="1:95" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="98"/>
-      <c r="E21" s="97"/>
+    <row r="21" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="80" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -5076,14 +5054,22 @@
       <c r="CP21" s="14"/>
       <c r="CQ21" s="14"/>
     </row>
-    <row r="22" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="102" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="103"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
+    <row r="22" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>192</v>
+      </c>
+      <c r="D22" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="109" t="s">
+        <v>15</v>
+      </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -5175,22 +5161,18 @@
       <c r="CP22" s="14"/>
       <c r="CQ22" s="14"/>
     </row>
-    <row r="23" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="55" t="s">
-        <v>43</v>
+        <v>97</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>1</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="89" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="93" t="s">
-        <v>15</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D23" s="105"/>
+      <c r="E23" s="109"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -5284,18 +5266,20 @@
     </row>
     <row r="24" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="89"/>
-      <c r="E24" s="93"/>
+        <v>58</v>
+      </c>
+      <c r="D24" s="105"/>
+      <c r="E24" s="109"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="G24" s="14" t="s">
+        <v>68</v>
+      </c>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -5387,20 +5371,18 @@
     </row>
     <row r="25" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="89"/>
-      <c r="E25" s="93"/>
+        <v>59</v>
+      </c>
+      <c r="D25" s="105"/>
+      <c r="E25" s="109"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="14" t="s">
-        <v>73</v>
-      </c>
+      <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
@@ -5492,16 +5474,16 @@
     </row>
     <row r="26" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="89"/>
-      <c r="E26" s="93"/>
+        <v>60</v>
+      </c>
+      <c r="D26" s="105"/>
+      <c r="E26" s="109"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -5595,16 +5577,16 @@
     </row>
     <row r="27" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>4</v>
+        <v>174</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="89"/>
-      <c r="E27" s="93"/>
+        <v>111</v>
+      </c>
+      <c r="D27" s="105"/>
+      <c r="E27" s="109"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
@@ -5698,16 +5680,16 @@
     </row>
     <row r="28" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="89"/>
-      <c r="E28" s="93"/>
+        <v>61</v>
+      </c>
+      <c r="D28" s="105"/>
+      <c r="E28" s="109"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
@@ -5799,18 +5781,14 @@
       <c r="CP28" s="14"/>
       <c r="CQ28" s="14"/>
     </row>
-    <row r="29" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C29" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="89"/>
-      <c r="E29" s="93"/>
+    <row r="29" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="106" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="107"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="107"/>
+      <c r="E29" s="108"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
@@ -5902,14 +5880,22 @@
       <c r="CP29" s="14"/>
       <c r="CQ29" s="14"/>
     </row>
-    <row r="30" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="90" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="91"/>
-      <c r="C30" s="91"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="92"/>
+    <row r="30" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="102" t="s">
+        <v>67</v>
+      </c>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -6001,22 +5987,18 @@
       <c r="CP30" s="14"/>
       <c r="CQ30" s="14"/>
     </row>
-    <row r="31" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>129</v>
+        <v>26</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>5</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="83" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31" s="86" t="s">
-        <v>72</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D31" s="100"/>
+      <c r="E31" s="103"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
@@ -6110,16 +6092,16 @@
     </row>
     <row r="32" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="84"/>
-      <c r="E32" s="87"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="104"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -6211,153 +6193,49 @@
       <c r="CP32" s="14"/>
       <c r="CQ32" s="14"/>
     </row>
-    <row r="33" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="85"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-      <c r="S33" s="14"/>
-      <c r="T33" s="14"/>
-      <c r="U33" s="14"/>
-      <c r="V33" s="14"/>
-      <c r="W33" s="14"/>
-      <c r="X33" s="14"/>
-      <c r="Y33" s="14"/>
-      <c r="Z33" s="14"/>
-      <c r="AA33" s="14"/>
-      <c r="AB33" s="14"/>
-      <c r="AC33" s="14"/>
-      <c r="AD33" s="14"/>
-      <c r="AE33" s="14"/>
-      <c r="AF33" s="14"/>
-      <c r="AG33" s="14"/>
-      <c r="AH33" s="14"/>
-      <c r="AI33" s="14"/>
-      <c r="AJ33" s="14"/>
-      <c r="AK33" s="14"/>
-      <c r="AL33" s="14"/>
-      <c r="AM33" s="14"/>
-      <c r="AN33" s="14"/>
-      <c r="AO33" s="14"/>
-      <c r="AP33" s="14"/>
-      <c r="AQ33" s="14"/>
-      <c r="AR33" s="14"/>
-      <c r="AS33" s="14"/>
-      <c r="AT33" s="14"/>
-      <c r="AU33" s="14"/>
-      <c r="AV33" s="14"/>
-      <c r="AW33" s="14"/>
-      <c r="AX33" s="14"/>
-      <c r="AY33" s="14"/>
-      <c r="AZ33" s="14"/>
-      <c r="BA33" s="14"/>
-      <c r="BB33" s="14"/>
-      <c r="BC33" s="14"/>
-      <c r="BD33" s="14"/>
-      <c r="BE33" s="14"/>
-      <c r="BF33" s="14"/>
-      <c r="BG33" s="14"/>
-      <c r="BH33" s="14"/>
-      <c r="BI33" s="14"/>
-      <c r="BJ33" s="14"/>
-      <c r="BK33" s="14"/>
-      <c r="BL33" s="14"/>
-      <c r="BM33" s="14"/>
-      <c r="BN33" s="14"/>
-      <c r="BO33" s="14"/>
-      <c r="BP33" s="14"/>
-      <c r="BQ33" s="14"/>
-      <c r="BR33" s="14"/>
-      <c r="BS33" s="14"/>
-      <c r="BT33" s="14"/>
-      <c r="BU33" s="14"/>
-      <c r="BV33" s="14"/>
-      <c r="BW33" s="14"/>
-      <c r="BX33" s="14"/>
-      <c r="BY33" s="14"/>
-      <c r="BZ33" s="14"/>
-      <c r="CA33" s="14"/>
-      <c r="CB33" s="14"/>
-      <c r="CC33" s="14"/>
-      <c r="CD33" s="14"/>
-      <c r="CE33" s="14"/>
-      <c r="CF33" s="14"/>
-      <c r="CG33" s="14"/>
-      <c r="CH33" s="14"/>
-      <c r="CI33" s="14"/>
-      <c r="CJ33" s="14"/>
-      <c r="CK33" s="14"/>
-      <c r="CL33" s="14"/>
-      <c r="CM33" s="14"/>
-      <c r="CN33" s="14"/>
-      <c r="CO33" s="14"/>
-      <c r="CP33" s="14"/>
-      <c r="CQ33" s="14"/>
-    </row>
-    <row r="34" spans="1:95" ht="51" x14ac:dyDescent="0.2">
-      <c r="C34" s="19" t="s">
+    <row r="33" spans="3:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="C33" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D33" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E33" s="20" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D8:D13"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="D23:D29"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="E23:E29"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="E22:E28"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="E17:E20"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" location="/dashboard" display="https://acleddata.com/dashboard/ - /dashboard" xr:uid="{F76E7675-2B2E-2D45-8C2B-2CB43E3D6E32}"/>
-    <hyperlink ref="B10" r:id="rId2" display="https://fragilestatesindex.org/data/" xr:uid="{A9B1CC3D-C0A1-C04F-BBD3-3E6A6BCE7B20}"/>
-    <hyperlink ref="B13" r:id="rId3" display="https://oefdatascience.github.io/REIGN.github.io/" xr:uid="{2AEFFF55-2CCA-7F42-82FE-4DED88CAF0DE}"/>
-    <hyperlink ref="B15" r:id="rId4" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
-    <hyperlink ref="B16" r:id="rId5" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
-    <hyperlink ref="B21" r:id="rId6" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
-    <hyperlink ref="B29" r:id="rId7" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
-    <hyperlink ref="B3" r:id="rId8" display="https://fews.net/" xr:uid="{3D674EBD-4EF9-1342-883D-87D2B91B65D7}"/>
-    <hyperlink ref="B6" r:id="rId9" display="https://www.acaps.org/countries" xr:uid="{323C0C04-FA1B-0C4D-B8B5-EB4AF4D1488B}"/>
-    <hyperlink ref="B18" r:id="rId10" display="COVID Economic Stimus Index (as measured by Elgin et al)" xr:uid="{999A8B13-E27C-374A-82CC-F226FAFAE1F4}"/>
+    <hyperlink ref="B12" r:id="rId2" display="https://oefdatascience.github.io/REIGN.github.io/" xr:uid="{2AEFFF55-2CCA-7F42-82FE-4DED88CAF0DE}"/>
+    <hyperlink ref="B14" r:id="rId3" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
+    <hyperlink ref="B15" r:id="rId4" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
+    <hyperlink ref="B20" r:id="rId5" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
+    <hyperlink ref="B28" r:id="rId6" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
+    <hyperlink ref="B3" r:id="rId7" display="https://fews.net/" xr:uid="{3D674EBD-4EF9-1342-883D-87D2B91B65D7}"/>
+    <hyperlink ref="B6" r:id="rId8" display="https://www.acaps.org/countries" xr:uid="{323C0C04-FA1B-0C4D-B8B5-EB4AF4D1488B}"/>
+    <hyperlink ref="B17" r:id="rId9" display="COVID Economic Stimus Index (as measured by Elgin et al)" xr:uid="{999A8B13-E27C-374A-82CC-F226FAFAE1F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6370,13 +6248,13 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.5" style="79" customWidth="1"/>
+    <col min="1" max="1" width="41.5" style="76" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="4" max="4" width="62.33203125" customWidth="1"/>
@@ -6384,204 +6262,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="71" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="29" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="96" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+    </row>
+    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="72" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="96" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+    </row>
+    <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="110" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+    </row>
+    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="80" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+    </row>
+    <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="73" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="99" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-    </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="74" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="99" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-    </row>
-    <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="75" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="81" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-    </row>
-    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="102" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="104"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="104"/>
-    </row>
-    <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="76" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" s="45" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="100"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="100"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="97"/>
       <c r="G8" s="46"/>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="80" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="G10" s="47"/>
+    </row>
+    <row r="11" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="G9" s="46" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="102" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="104"/>
-      <c r="C10" s="104"/>
-      <c r="D10" s="104"/>
-      <c r="G10" s="47"/>
-    </row>
-    <row r="11" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="77" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>93</v>
-      </c>
       <c r="C11" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="70" t="s">
-        <v>172</v>
-      </c>
-      <c r="E11" s="71" t="s">
-        <v>173</v>
-      </c>
-      <c r="F11" s="72"/>
+        <v>79</v>
+      </c>
+      <c r="D11" s="68" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" s="70"/>
       <c r="G11" s="46"/>
     </row>
     <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="90" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="91"/>
-      <c r="C12" s="91"/>
-      <c r="D12" s="91"/>
+      <c r="A12" s="106" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="107"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
       <c r="G12" s="45"/>
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="B13" s="67" t="s">
-        <v>170</v>
-      </c>
-      <c r="C13" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="D13" s="69" t="s">
-        <v>171</v>
+      <c r="A13" s="63" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="67" t="s">
+        <v>160</v>
       </c>
       <c r="E13" s="35"/>
       <c r="G13" s="45" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="90" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="91"/>
-      <c r="C14" s="91"/>
-      <c r="D14" s="91"/>
+      <c r="A14" s="106" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="107"/>
+      <c r="C14" s="107"/>
+      <c r="D14" s="107"/>
     </row>
     <row r="15" spans="1:7" ht="248" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="75" t="s">
+        <v>186</v>
+      </c>
+      <c r="B15" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="41" t="s">
-        <v>94</v>
-      </c>
       <c r="C15" s="42" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D15" s="42" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="E15" s="43" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F15" s="44" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -6626,46 +6504,46 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -6680,7 +6558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E658424-6FDF-FB4F-A908-E363FB27277D}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -6692,71 +6570,71 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="53" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="82" t="s">
-        <v>81</v>
+      <c r="B24" s="79" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -6771,10 +6649,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FAE3D5-1E62-BD47-A72D-971150914E15}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6787,488 +6665,474 @@
     <col min="6" max="6" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E2" s="61"/>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="63" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="59" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="59" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="59" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="61"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="63" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="66" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>148</v>
-      </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="57" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="80" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D9" s="77" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>112</v>
-      </c>
-      <c r="D10" s="80" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>148</v>
-      </c>
-      <c r="B14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>148</v>
-      </c>
-      <c r="B15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="D16" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" t="s">
-        <v>152</v>
-      </c>
-      <c r="F17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>148</v>
-      </c>
-      <c r="B18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>148</v>
-      </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>148</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="D21" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>148</v>
-      </c>
-      <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>148</v>
-      </c>
-      <c r="B23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="D23" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>148</v>
-      </c>
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="28" t="s">
+      <c r="D30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>148</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="17" t="s">
+      <c r="D31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D25" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>148</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="D26" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>148</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="17" t="s">
+      <c r="D32" t="s">
         <v>156</v>
-      </c>
-      <c r="D27" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>148</v>
-      </c>
-      <c r="B28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="D28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>148</v>
-      </c>
-      <c r="B29" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="D29" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>148</v>
-      </c>
-      <c r="B30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="D30" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>148</v>
-      </c>
-      <c r="B31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="D31" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>148</v>
-      </c>
-      <c r="B32" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>148</v>
-      </c>
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D34">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fix remaining issues with adding forward-looking socio-economic risk variable
Now included in the xlsx file

Updated indicator xlsx file too
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E0EB55-106D-9A4A-B5A3-DC0AB17128FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47457B6C-1031-4841-B710-9CD33BEBF88E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="205">
   <si>
     <t>Projected Coup risk (REIGN)</t>
   </si>
@@ -1228,6 +1228,88 @@
   <si>
     <t>10 &gt; 100 pct
 0 &lt;  pct</t>
+  </si>
+  <si>
+    <t>SOCIO-ECONOMIC RISK</t>
+  </si>
+  <si>
+    <t>S_gdp_change.Rating_norm</t>
+  </si>
+  <si>
+    <t>S_unemployment.Rating_norm</t>
+  </si>
+  <si>
+    <t>S_income_support.Rating_norm</t>
+  </si>
+  <si>
+    <t>Change in GDP growth (INFORM COVID Warning tool)</t>
+  </si>
+  <si>
+    <t>Unemployment rate</t>
+  </si>
+  <si>
+    <t>Whether income support is provided</t>
+  </si>
+  <si>
+    <t>10 = Government replacing &gt; 50% of lost salary
+7 = Government replacing &lt; 50% of lost salary
+0 = No income support</t>
+  </si>
+  <si>
+    <t>INFORM threshold</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">S = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>MAX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>(S_gdp_change.Rating_norm
+S_unemployment.Rating_norm
+S_income_support.Rating_norm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">S_SQ = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>GEOMETRICMEAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>(EXISTING_RISK_SOCIOECONOMIC, S)</t>
+    </r>
+  </si>
+  <si>
+    <t>INFORM COVID Warning Tracker (EU)</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1428,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1485,8 +1567,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1656,12 +1744,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1967,12 +2064,144 @@
     <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2974,10 +3203,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:CQ33"/>
+  <dimension ref="A1:CQ37"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4955,9 +5184,9 @@
       <c r="CP20" s="14"/>
       <c r="CQ20" s="14"/>
     </row>
-    <row r="21" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:95" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="80" t="s">
-        <v>40</v>
+        <v>193</v>
       </c>
       <c r="B21" s="81"/>
       <c r="C21" s="81"/>
@@ -5054,21 +5283,21 @@
       <c r="CP21" s="14"/>
       <c r="CQ21" s="14"/>
     </row>
-    <row r="22" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="B22" s="55" t="s">
-        <v>191</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>192</v>
-      </c>
-      <c r="D22" s="105" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="109" t="s">
-        <v>15</v>
+    <row r="22" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A22" s="111" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" s="112" t="s">
+        <v>197</v>
+      </c>
+      <c r="C22" s="113" t="s">
+        <v>201</v>
+      </c>
+      <c r="D22" s="116" t="s">
+        <v>202</v>
+      </c>
+      <c r="E22" s="116" t="s">
+        <v>203</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -5161,18 +5390,18 @@
       <c r="CP22" s="14"/>
       <c r="CQ22" s="14"/>
     </row>
-    <row r="23" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="105"/>
-      <c r="E23" s="109"/>
+    <row r="23" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="111" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="C23" s="113" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23" s="115"/>
+      <c r="E23" s="118"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -5264,22 +5493,20 @@
       <c r="CP23" s="14"/>
       <c r="CQ23" s="14"/>
     </row>
-    <row r="24" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" s="105"/>
-      <c r="E24" s="109"/>
+    <row r="24" spans="1:95" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A24" s="111" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="112" t="s">
+        <v>199</v>
+      </c>
+      <c r="C24" s="113" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24" s="114"/>
+      <c r="E24" s="117"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="14" t="s">
-        <v>68</v>
-      </c>
+      <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -5369,18 +5596,14 @@
       <c r="CP24" s="14"/>
       <c r="CQ24" s="14"/>
     </row>
-    <row r="25" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="105"/>
-      <c r="E25" s="109"/>
+    <row r="25" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="80" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
@@ -5472,18 +5695,22 @@
       <c r="CP25" s="14"/>
       <c r="CQ25" s="14"/>
     </row>
-    <row r="26" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>4</v>
+        <v>190</v>
+      </c>
+      <c r="B26" s="55" t="s">
+        <v>191</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="105"/>
-      <c r="E26" s="109"/>
+        <v>192</v>
+      </c>
+      <c r="D26" s="105" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="109" t="s">
+        <v>15</v>
+      </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -5577,13 +5804,13 @@
     </row>
     <row r="27" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>174</v>
+        <v>1</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="D27" s="105"/>
       <c r="E27" s="109"/>
@@ -5680,18 +5907,20 @@
     </row>
     <row r="28" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>175</v>
+        <v>2</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D28" s="105"/>
       <c r="E28" s="109"/>
       <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="G28" s="14" t="s">
+        <v>68</v>
+      </c>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
@@ -5781,14 +6010,18 @@
       <c r="CP28" s="14"/>
       <c r="CQ28" s="14"/>
     </row>
-    <row r="29" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="106" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
-      <c r="E29" s="108"/>
+    <row r="29" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="105"/>
+      <c r="E29" s="109"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
@@ -5880,22 +6113,18 @@
       <c r="CP29" s="14"/>
       <c r="CQ29" s="14"/>
     </row>
-    <row r="30" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="99" t="s">
-        <v>66</v>
-      </c>
-      <c r="E30" s="102" t="s">
-        <v>67</v>
-      </c>
+    <row r="30" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="105"/>
+      <c r="E30" s="109"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -5987,18 +6216,18 @@
       <c r="CP30" s="14"/>
       <c r="CQ30" s="14"/>
     </row>
-    <row r="31" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="100"/>
-      <c r="E31" s="103"/>
+    <row r="31" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="105"/>
+      <c r="E31" s="109"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
@@ -6090,18 +6319,18 @@
       <c r="CP31" s="14"/>
       <c r="CQ31" s="14"/>
     </row>
-    <row r="32" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="101"/>
-      <c r="E32" s="104"/>
+    <row r="32" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C32" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="105"/>
+      <c r="E32" s="109"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -6193,28 +6422,443 @@
       <c r="CP32" s="14"/>
       <c r="CQ32" s="14"/>
     </row>
-    <row r="33" spans="3:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="C33" s="19" t="s">
+    <row r="33" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="106" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="107"/>
+      <c r="C33" s="107"/>
+      <c r="D33" s="107"/>
+      <c r="E33" s="108"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
+      <c r="S33" s="14"/>
+      <c r="T33" s="14"/>
+      <c r="U33" s="14"/>
+      <c r="V33" s="14"/>
+      <c r="W33" s="14"/>
+      <c r="X33" s="14"/>
+      <c r="Y33" s="14"/>
+      <c r="Z33" s="14"/>
+      <c r="AA33" s="14"/>
+      <c r="AB33" s="14"/>
+      <c r="AC33" s="14"/>
+      <c r="AD33" s="14"/>
+      <c r="AE33" s="14"/>
+      <c r="AF33" s="14"/>
+      <c r="AG33" s="14"/>
+      <c r="AH33" s="14"/>
+      <c r="AI33" s="14"/>
+      <c r="AJ33" s="14"/>
+      <c r="AK33" s="14"/>
+      <c r="AL33" s="14"/>
+      <c r="AM33" s="14"/>
+      <c r="AN33" s="14"/>
+      <c r="AO33" s="14"/>
+      <c r="AP33" s="14"/>
+      <c r="AQ33" s="14"/>
+      <c r="AR33" s="14"/>
+      <c r="AS33" s="14"/>
+      <c r="AT33" s="14"/>
+      <c r="AU33" s="14"/>
+      <c r="AV33" s="14"/>
+      <c r="AW33" s="14"/>
+      <c r="AX33" s="14"/>
+      <c r="AY33" s="14"/>
+      <c r="AZ33" s="14"/>
+      <c r="BA33" s="14"/>
+      <c r="BB33" s="14"/>
+      <c r="BC33" s="14"/>
+      <c r="BD33" s="14"/>
+      <c r="BE33" s="14"/>
+      <c r="BF33" s="14"/>
+      <c r="BG33" s="14"/>
+      <c r="BH33" s="14"/>
+      <c r="BI33" s="14"/>
+      <c r="BJ33" s="14"/>
+      <c r="BK33" s="14"/>
+      <c r="BL33" s="14"/>
+      <c r="BM33" s="14"/>
+      <c r="BN33" s="14"/>
+      <c r="BO33" s="14"/>
+      <c r="BP33" s="14"/>
+      <c r="BQ33" s="14"/>
+      <c r="BR33" s="14"/>
+      <c r="BS33" s="14"/>
+      <c r="BT33" s="14"/>
+      <c r="BU33" s="14"/>
+      <c r="BV33" s="14"/>
+      <c r="BW33" s="14"/>
+      <c r="BX33" s="14"/>
+      <c r="BY33" s="14"/>
+      <c r="BZ33" s="14"/>
+      <c r="CA33" s="14"/>
+      <c r="CB33" s="14"/>
+      <c r="CC33" s="14"/>
+      <c r="CD33" s="14"/>
+      <c r="CE33" s="14"/>
+      <c r="CF33" s="14"/>
+      <c r="CG33" s="14"/>
+      <c r="CH33" s="14"/>
+      <c r="CI33" s="14"/>
+      <c r="CJ33" s="14"/>
+      <c r="CK33" s="14"/>
+      <c r="CL33" s="14"/>
+      <c r="CM33" s="14"/>
+      <c r="CN33" s="14"/>
+      <c r="CO33" s="14"/>
+      <c r="CP33" s="14"/>
+      <c r="CQ33" s="14"/>
+    </row>
+    <row r="34" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="102" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
+      <c r="S34" s="14"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="14"/>
+      <c r="V34" s="14"/>
+      <c r="W34" s="14"/>
+      <c r="X34" s="14"/>
+      <c r="Y34" s="14"/>
+      <c r="Z34" s="14"/>
+      <c r="AA34" s="14"/>
+      <c r="AB34" s="14"/>
+      <c r="AC34" s="14"/>
+      <c r="AD34" s="14"/>
+      <c r="AE34" s="14"/>
+      <c r="AF34" s="14"/>
+      <c r="AG34" s="14"/>
+      <c r="AH34" s="14"/>
+      <c r="AI34" s="14"/>
+      <c r="AJ34" s="14"/>
+      <c r="AK34" s="14"/>
+      <c r="AL34" s="14"/>
+      <c r="AM34" s="14"/>
+      <c r="AN34" s="14"/>
+      <c r="AO34" s="14"/>
+      <c r="AP34" s="14"/>
+      <c r="AQ34" s="14"/>
+      <c r="AR34" s="14"/>
+      <c r="AS34" s="14"/>
+      <c r="AT34" s="14"/>
+      <c r="AU34" s="14"/>
+      <c r="AV34" s="14"/>
+      <c r="AW34" s="14"/>
+      <c r="AX34" s="14"/>
+      <c r="AY34" s="14"/>
+      <c r="AZ34" s="14"/>
+      <c r="BA34" s="14"/>
+      <c r="BB34" s="14"/>
+      <c r="BC34" s="14"/>
+      <c r="BD34" s="14"/>
+      <c r="BE34" s="14"/>
+      <c r="BF34" s="14"/>
+      <c r="BG34" s="14"/>
+      <c r="BH34" s="14"/>
+      <c r="BI34" s="14"/>
+      <c r="BJ34" s="14"/>
+      <c r="BK34" s="14"/>
+      <c r="BL34" s="14"/>
+      <c r="BM34" s="14"/>
+      <c r="BN34" s="14"/>
+      <c r="BO34" s="14"/>
+      <c r="BP34" s="14"/>
+      <c r="BQ34" s="14"/>
+      <c r="BR34" s="14"/>
+      <c r="BS34" s="14"/>
+      <c r="BT34" s="14"/>
+      <c r="BU34" s="14"/>
+      <c r="BV34" s="14"/>
+      <c r="BW34" s="14"/>
+      <c r="BX34" s="14"/>
+      <c r="BY34" s="14"/>
+      <c r="BZ34" s="14"/>
+      <c r="CA34" s="14"/>
+      <c r="CB34" s="14"/>
+      <c r="CC34" s="14"/>
+      <c r="CD34" s="14"/>
+      <c r="CE34" s="14"/>
+      <c r="CF34" s="14"/>
+      <c r="CG34" s="14"/>
+      <c r="CH34" s="14"/>
+      <c r="CI34" s="14"/>
+      <c r="CJ34" s="14"/>
+      <c r="CK34" s="14"/>
+      <c r="CL34" s="14"/>
+      <c r="CM34" s="14"/>
+      <c r="CN34" s="14"/>
+      <c r="CO34" s="14"/>
+      <c r="CP34" s="14"/>
+      <c r="CQ34" s="14"/>
+    </row>
+    <row r="35" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="100"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="14"/>
+      <c r="W35" s="14"/>
+      <c r="X35" s="14"/>
+      <c r="Y35" s="14"/>
+      <c r="Z35" s="14"/>
+      <c r="AA35" s="14"/>
+      <c r="AB35" s="14"/>
+      <c r="AC35" s="14"/>
+      <c r="AD35" s="14"/>
+      <c r="AE35" s="14"/>
+      <c r="AF35" s="14"/>
+      <c r="AG35" s="14"/>
+      <c r="AH35" s="14"/>
+      <c r="AI35" s="14"/>
+      <c r="AJ35" s="14"/>
+      <c r="AK35" s="14"/>
+      <c r="AL35" s="14"/>
+      <c r="AM35" s="14"/>
+      <c r="AN35" s="14"/>
+      <c r="AO35" s="14"/>
+      <c r="AP35" s="14"/>
+      <c r="AQ35" s="14"/>
+      <c r="AR35" s="14"/>
+      <c r="AS35" s="14"/>
+      <c r="AT35" s="14"/>
+      <c r="AU35" s="14"/>
+      <c r="AV35" s="14"/>
+      <c r="AW35" s="14"/>
+      <c r="AX35" s="14"/>
+      <c r="AY35" s="14"/>
+      <c r="AZ35" s="14"/>
+      <c r="BA35" s="14"/>
+      <c r="BB35" s="14"/>
+      <c r="BC35" s="14"/>
+      <c r="BD35" s="14"/>
+      <c r="BE35" s="14"/>
+      <c r="BF35" s="14"/>
+      <c r="BG35" s="14"/>
+      <c r="BH35" s="14"/>
+      <c r="BI35" s="14"/>
+      <c r="BJ35" s="14"/>
+      <c r="BK35" s="14"/>
+      <c r="BL35" s="14"/>
+      <c r="BM35" s="14"/>
+      <c r="BN35" s="14"/>
+      <c r="BO35" s="14"/>
+      <c r="BP35" s="14"/>
+      <c r="BQ35" s="14"/>
+      <c r="BR35" s="14"/>
+      <c r="BS35" s="14"/>
+      <c r="BT35" s="14"/>
+      <c r="BU35" s="14"/>
+      <c r="BV35" s="14"/>
+      <c r="BW35" s="14"/>
+      <c r="BX35" s="14"/>
+      <c r="BY35" s="14"/>
+      <c r="BZ35" s="14"/>
+      <c r="CA35" s="14"/>
+      <c r="CB35" s="14"/>
+      <c r="CC35" s="14"/>
+      <c r="CD35" s="14"/>
+      <c r="CE35" s="14"/>
+      <c r="CF35" s="14"/>
+      <c r="CG35" s="14"/>
+      <c r="CH35" s="14"/>
+      <c r="CI35" s="14"/>
+      <c r="CJ35" s="14"/>
+      <c r="CK35" s="14"/>
+      <c r="CL35" s="14"/>
+      <c r="CM35" s="14"/>
+      <c r="CN35" s="14"/>
+      <c r="CO35" s="14"/>
+      <c r="CP35" s="14"/>
+      <c r="CQ35" s="14"/>
+    </row>
+    <row r="36" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="101"/>
+      <c r="E36" s="104"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="14"/>
+      <c r="X36" s="14"/>
+      <c r="Y36" s="14"/>
+      <c r="Z36" s="14"/>
+      <c r="AA36" s="14"/>
+      <c r="AB36" s="14"/>
+      <c r="AC36" s="14"/>
+      <c r="AD36" s="14"/>
+      <c r="AE36" s="14"/>
+      <c r="AF36" s="14"/>
+      <c r="AG36" s="14"/>
+      <c r="AH36" s="14"/>
+      <c r="AI36" s="14"/>
+      <c r="AJ36" s="14"/>
+      <c r="AK36" s="14"/>
+      <c r="AL36" s="14"/>
+      <c r="AM36" s="14"/>
+      <c r="AN36" s="14"/>
+      <c r="AO36" s="14"/>
+      <c r="AP36" s="14"/>
+      <c r="AQ36" s="14"/>
+      <c r="AR36" s="14"/>
+      <c r="AS36" s="14"/>
+      <c r="AT36" s="14"/>
+      <c r="AU36" s="14"/>
+      <c r="AV36" s="14"/>
+      <c r="AW36" s="14"/>
+      <c r="AX36" s="14"/>
+      <c r="AY36" s="14"/>
+      <c r="AZ36" s="14"/>
+      <c r="BA36" s="14"/>
+      <c r="BB36" s="14"/>
+      <c r="BC36" s="14"/>
+      <c r="BD36" s="14"/>
+      <c r="BE36" s="14"/>
+      <c r="BF36" s="14"/>
+      <c r="BG36" s="14"/>
+      <c r="BH36" s="14"/>
+      <c r="BI36" s="14"/>
+      <c r="BJ36" s="14"/>
+      <c r="BK36" s="14"/>
+      <c r="BL36" s="14"/>
+      <c r="BM36" s="14"/>
+      <c r="BN36" s="14"/>
+      <c r="BO36" s="14"/>
+      <c r="BP36" s="14"/>
+      <c r="BQ36" s="14"/>
+      <c r="BR36" s="14"/>
+      <c r="BS36" s="14"/>
+      <c r="BT36" s="14"/>
+      <c r="BU36" s="14"/>
+      <c r="BV36" s="14"/>
+      <c r="BW36" s="14"/>
+      <c r="BX36" s="14"/>
+      <c r="BY36" s="14"/>
+      <c r="BZ36" s="14"/>
+      <c r="CA36" s="14"/>
+      <c r="CB36" s="14"/>
+      <c r="CC36" s="14"/>
+      <c r="CD36" s="14"/>
+      <c r="CE36" s="14"/>
+      <c r="CF36" s="14"/>
+      <c r="CG36" s="14"/>
+      <c r="CH36" s="14"/>
+      <c r="CI36" s="14"/>
+      <c r="CJ36" s="14"/>
+      <c r="CK36" s="14"/>
+      <c r="CL36" s="14"/>
+      <c r="CM36" s="14"/>
+      <c r="CN36" s="14"/>
+      <c r="CO36" s="14"/>
+      <c r="CP36" s="14"/>
+      <c r="CQ36" s="14"/>
+    </row>
+    <row r="37" spans="1:95" ht="51" x14ac:dyDescent="0.2">
+      <c r="C37" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D37" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E37" s="20" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="21">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A16:E16"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="D22:D28"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="E22:E28"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="E34:E36"/>
+    <mergeCell ref="D26:D32"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="E26:E32"/>
     <mergeCell ref="A21:E21"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="A25:E25"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="E14:E15"/>
@@ -6232,7 +6876,7 @@
     <hyperlink ref="B14" r:id="rId3" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
     <hyperlink ref="B15" r:id="rId4" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
     <hyperlink ref="B20" r:id="rId5" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
-    <hyperlink ref="B28" r:id="rId6" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
+    <hyperlink ref="B32" r:id="rId6" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
     <hyperlink ref="B3" r:id="rId7" display="https://fews.net/" xr:uid="{3D674EBD-4EF9-1342-883D-87D2B91B65D7}"/>
     <hyperlink ref="B6" r:id="rId8" display="https://www.acaps.org/countries" xr:uid="{323C0C04-FA1B-0C4D-B8B5-EB4AF4D1488B}"/>
     <hyperlink ref="B17" r:id="rId9" display="COVID Economic Stimus Index (as measured by Elgin et al)" xr:uid="{999A8B13-E27C-374A-82CC-F226FAFAE1F4}"/>
@@ -6248,8 +6892,8 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView zoomScale="114" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A4" zoomScale="114" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6639,7 +7283,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B8">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="6" priority="1">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6649,10 +7293,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FAE3D5-1E62-BD47-A72D-971150914E15}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6940,13 +7584,13 @@
         <v>138</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>117</v>
+        <v>78</v>
+      </c>
+      <c r="C20" s="119" t="s">
+        <v>194</v>
       </c>
       <c r="D20" t="s">
-        <v>166</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6954,13 +7598,13 @@
         <v>138</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>121</v>
+        <v>78</v>
+      </c>
+      <c r="C21" s="119" t="s">
+        <v>195</v>
       </c>
       <c r="D21" t="s">
-        <v>152</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6968,16 +7612,16 @@
         <v>138</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>112</v>
+        <v>78</v>
+      </c>
+      <c r="C22" s="119" t="s">
+        <v>196</v>
       </c>
       <c r="D22" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>138</v>
       </c>
@@ -6985,24 +7629,24 @@
         <v>32</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>24</v>
+        <v>117</v>
       </c>
       <c r="D23" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>138</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>190</v>
+        <v>32</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>121</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7010,13 +7654,13 @@
         <v>138</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>144</v>
+        <v>32</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>112</v>
       </c>
       <c r="D25" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7024,16 +7668,16 @@
         <v>138</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>145</v>
+        <v>32</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>138</v>
       </c>
@@ -7041,10 +7685,10 @@
         <v>40</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="D27" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7055,10 +7699,10 @@
         <v>40</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D28" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7069,10 +7713,10 @@
         <v>40</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="D29" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7083,10 +7727,10 @@
         <v>40</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D30" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7094,13 +7738,13 @@
         <v>138</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>149</v>
       </c>
       <c r="D31" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7108,13 +7752,13 @@
         <v>138</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>26</v>
+        <v>40</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -7122,19 +7766,76 @@
         <v>138</v>
       </c>
       <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C34" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D36" t="s">
         <v>157</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D33">
+  <conditionalFormatting sqref="D2:D19 D23:D36">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(D2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(D20))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(D22))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(D2))=0</formula>
+      <formula>LEN(TRIM(D21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update excel indicator file
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47457B6C-1031-4841-B710-9CD33BEBF88E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B993026-9964-B040-9AA3-30725D812634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="-3220" yWindow="-18680" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="205">
-  <si>
-    <t>Projected Coup risk (REIGN)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="207">
   <si>
     <t>Bi-weekly percentage change in COVID cases (per 1M)</t>
   </si>
@@ -55,9 +52,6 @@
   </si>
   <si>
     <t>INFORM Crisis monitor</t>
-  </si>
-  <si>
-    <t>INFORM crisis monitor</t>
   </si>
   <si>
     <t>RISK SCORES AS MAX VALUES</t>
@@ -221,9 +215,6 @@
     <t>F_Fewsnet_Score_norm</t>
   </si>
   <si>
-    <t>Fr_REIGN_couprisk3m_norm</t>
-  </si>
-  <si>
     <t>M_GDP_IMF_2019minus2020_norm</t>
   </si>
   <si>
@@ -251,9 +242,6 @@
     <t xml:space="preserve"> NORMALISATION BOUNDS</t>
   </si>
   <si>
-    <t>FOOD SECURITY RISK</t>
-  </si>
-  <si>
     <t>FISCAL/DEBT RISK</t>
   </si>
   <si>
@@ -266,9 +254,6 @@
     <t>ARTEMIS (WB internal)</t>
   </si>
   <si>
-    <t>Growth in reported number of conflict events (ACLED) – number of events in the prior month relative the same period last year  (source)</t>
-  </si>
-  <si>
     <t>Change in forecast GDP growth: 2020 – 2019 (WB Global Economic Prospects) (source)</t>
   </si>
   <si>
@@ -276,9 +261,6 @@
   </si>
   <si>
     <t>Change in forecast government net lending/borrowing: 2020 – 2019 (IMF World Economic Outlook) (source)</t>
-  </si>
-  <si>
-    <t>COVID RESPONSE</t>
   </si>
   <si>
     <t>MACRO-ECONOMIC VULNERABILITY</t>
@@ -469,14 +451,6 @@
     </r>
   </si>
   <si>
-    <t>10 &gt; 300
-0 &lt; 0</t>
-  </si>
-  <si>
-    <t>10 &gt; 400
-0 &lt; 0</t>
-  </si>
-  <si>
     <t>10 &lt; 20 pct
 0 &gt; 95 pct</t>
   </si>
@@ -502,89 +476,6 @@
   </si>
   <si>
     <t xml:space="preserve"> 10 = Ongoing Natural Hazard Crisis</t>
-  </si>
-  <si>
-    <t>CONFLICT FRAGILITY AND INSTITUTIONAL RISK</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> IF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> C_INFORM_CRISIS = "Ongoing Complex Crisis" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>AND</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> EXISTING_RISK_Fr &lt;=5 then Fr = 10,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>ELSE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Fr = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>MAX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>(Fr_FSI_2019minus2020_norm, Fr_REIGN_couprisk3m_norm, Fr_ACLED_event_same_month_difference_perc_norm, 
-Fr_ACLED_fatal_same_month_difference_perc_norm)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -670,22 +561,6 @@
     <t>`</t>
   </si>
   <si>
-    <t>Fr_ACLED_event_same_month_difference_perc_norm</t>
-  </si>
-  <si>
-    <t>Fr_ACLED_fatal_same_month_difference_perc_norm</t>
-  </si>
-  <si>
-    <t>Fr_INFORM_Fragility_Score</t>
-  </si>
-  <si>
-    <t>INFORM institutional score</t>
-  </si>
-  <si>
-    <t>10 &lt; 95 pct 
-0 &gt; 5 pct</t>
-  </si>
-  <si>
     <t>H_HIS_Score_norm</t>
   </si>
   <si>
@@ -696,9 +571,6 @@
   </si>
   <si>
     <t>M_Economic_and_Financial_score_norm</t>
-  </si>
-  <si>
-    <t>SOCIOECONOMIC VULNERABILITY RISK</t>
   </si>
   <si>
     <t xml:space="preserve">10 &gt;= 20 
@@ -900,29 +772,6 @@
   </si>
   <si>
     <t>COVID Economic Stimulus Index (as measured by Elgin et al)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Growth in conflict fatalities - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">number of deaths in the prior month relative the same period last year  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">(ACLED) </t>
-    </r>
   </si>
   <si>
     <r>
@@ -1072,12 +921,6 @@
     <t xml:space="preserve">ARTEMIS </t>
   </si>
   <si>
-    <t>Fragility Index (INFORM)</t>
-  </si>
-  <si>
-    <t>Projected Coup Risk</t>
-  </si>
-  <si>
     <t xml:space="preserve">Projected COVID deaths </t>
   </si>
   <si>
@@ -1153,15 +996,6 @@
     <t>Change in Borrowing/Lending</t>
   </si>
   <si>
-    <t>Change in Events (ACLED)</t>
-  </si>
-  <si>
-    <t>Change in Fatalities (ACLED)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ongoing Political Crisis </t>
-  </si>
-  <si>
     <t>Difference in Projected GDP (WB)</t>
   </si>
   <si>
@@ -1193,16 +1027,6 @@
   </si>
   <si>
     <t>A measure of a country's fiscal risk, focused predominantly on debt burden as well as fiscal stimulus in response to COVID</t>
-  </si>
-  <si>
-    <t>Fr_INFORM_CRISIS_Norm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10 = Ongoing complex crisis
-0 = if no ongoing crisis </t>
-  </si>
-  <si>
-    <t>COVID/PANDEMIC RISK</t>
   </si>
   <si>
     <t>A measure of a country's exposure and response capacity to pandemic (note: indicators for emerging risk are targetted specifically at COVID-related dynamics)</t>
@@ -1228,9 +1052,6 @@
   <si>
     <t>10 &gt; 100 pct
 0 &lt;  pct</t>
-  </si>
-  <si>
-    <t>SOCIO-ECONOMIC RISK</t>
   </si>
   <si>
     <t>S_gdp_change.Rating_norm</t>
@@ -1310,6 +1131,159 @@
   </si>
   <si>
     <t>INFORM COVID Warning Tracker (EU)</t>
+  </si>
+  <si>
+    <t>Fr_combined_crisis_norm</t>
+  </si>
+  <si>
+    <t>Fr_state6m_norm</t>
+  </si>
+  <si>
+    <t>Fr_nonstate6m_norm</t>
+  </si>
+  <si>
+    <t>Fr_oneside6m_norm</t>
+  </si>
+  <si>
+    <t>Measure of whether a country is currently experiencing a crisis (based on the INFORM severty index)</t>
+  </si>
+  <si>
+    <t>10 &gt; 0.8
+0 &lt; 0.1</t>
+  </si>
+  <si>
+    <r>
+      <t>Likelihood of state-led violence in the next 6-months</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">(ViEWS) </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Likelihood of non-state violence in the next 6-months (ViEWS) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Likelihood of one-sided violence in the next 6-months (ViEWS) </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fr = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>MAX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>(Fr_combined_crisis_norm
+Fr_state6m_norm
+Fr_nonstate6m_norm
+Fr_oneside6m_norm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10 = Severity &gt; 3 &amp; Conditions worsening </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Severity &gt; 4 
+0 = Otherwise</t>
+    </r>
+  </si>
+  <si>
+    <t>FOOD SECURITY</t>
+  </si>
+  <si>
+    <t>CONFLICT AND FRAGILITY</t>
+  </si>
+  <si>
+    <t>SOCIO-ECONOMIC VULNERABILITY</t>
+  </si>
+  <si>
+    <t>COVID EXPOSURE AND RESPONSE CAPACITY</t>
+  </si>
+  <si>
+    <t>H_INFORM_rating.Value_norm</t>
+  </si>
+  <si>
+    <t>INFORM COVID vulnerability index (composite index)</t>
+  </si>
+  <si>
+    <t>10 &lt; 2
+0 &lt; 6</t>
+  </si>
+  <si>
+    <t>NH_multihazard_risk_norm</t>
+  </si>
+  <si>
+    <t>ThinkHazard! Database of natural hazard risks (World Bank)</t>
+  </si>
+  <si>
+    <t>10 &gt; 4 high risk hazards 
+0 = 0 high risk hazards</t>
+  </si>
+  <si>
+    <t>Ongoing crisis (ACAPS)</t>
+  </si>
+  <si>
+    <t>Likelihood of state-sponsored violence (ViEWS)</t>
+  </si>
+  <si>
+    <t>Likelihood of non-state violence (ViEWS)</t>
+  </si>
+  <si>
+    <t>Likelihood of one-sided violence (ViEWS)</t>
+  </si>
+  <si>
+    <t>Multi-hazard exposure (WB)</t>
+  </si>
+  <si>
+    <t>COVID RESPONSE AND RESPONSE CAPACITY</t>
+  </si>
+  <si>
+    <t>SOCIOECONOMIC VULNERABILITY</t>
   </si>
 </sst>
 </file>
@@ -1758,7 +1732,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1971,10 +1945,79 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2019,105 +2062,35 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -2265,13 +2238,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2136448</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>261122</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2847648</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>488298</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2336,13 +2309,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1994019</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>652803</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2768719</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>879979</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2407,13 +2380,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2077103</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>1044486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>477852</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>1271661</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2478,13 +2451,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2053365</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>1483645</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2599465</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>1710821</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2549,13 +2522,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2100841</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>1863457</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2786641</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>2103333</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2620,13 +2593,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2100840</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>2267010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2735840</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>2506886</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2691,13 +2664,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2480654</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>2682430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>17803</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>2922305</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3205,8 +3178,8 @@
   </sheetPr>
   <dimension ref="A1:CQ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3222,29 +3195,29 @@
   <sheetData>
     <row r="1" spans="1:95" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:95" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="96" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="98"/>
+      <c r="A2" s="85" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -3338,19 +3311,19 @@
     </row>
     <row r="3" spans="1:95" s="1" customFormat="1" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="57" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="87" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" s="83" t="s">
-        <v>125</v>
+        <v>86</v>
+      </c>
+      <c r="D3" s="110" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="106" t="s">
+        <v>108</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -3445,16 +3418,16 @@
     </row>
     <row r="4" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="87"/>
-      <c r="E4" s="84"/>
+        <v>91</v>
+      </c>
+      <c r="D4" s="110"/>
+      <c r="E4" s="107"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -3548,16 +3521,16 @@
     </row>
     <row r="5" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="87"/>
-      <c r="E5" s="84"/>
+        <v>92</v>
+      </c>
+      <c r="D5" s="110"/>
+      <c r="E5" s="107"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -3651,16 +3624,16 @@
     </row>
     <row r="6" spans="1:95" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="57" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="87"/>
-      <c r="E6" s="85"/>
+        <v>93</v>
+      </c>
+      <c r="D6" s="110"/>
+      <c r="E6" s="108"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -3752,13 +3725,13 @@
       <c r="CP6" s="14"/>
     </row>
     <row r="7" spans="1:95" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="96" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="98"/>
+      <c r="A7" s="85" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="87"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -3849,21 +3822,21 @@
       <c r="CO7" s="14"/>
       <c r="CP7" s="14"/>
     </row>
-    <row r="8" spans="1:95" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>69</v>
+    <row r="8" spans="1:95" s="2" customFormat="1" ht="89" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="72" t="s">
+        <v>179</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="88" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="91" t="s">
-        <v>65</v>
+        <v>189</v>
+      </c>
+      <c r="D8" s="111" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8" s="114" t="s">
+        <v>55</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -3955,18 +3928,18 @@
       <c r="CO8" s="14"/>
       <c r="CP8" s="14"/>
     </row>
-    <row r="9" spans="1:95" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>70</v>
+    <row r="9" spans="1:95" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="72" t="s">
+        <v>180</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="89"/>
-      <c r="E9" s="92"/>
+        <v>184</v>
+      </c>
+      <c r="D9" s="112"/>
+      <c r="E9" s="115"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -4057,18 +4030,18 @@
       <c r="CO9" s="14"/>
       <c r="CP9" s="14"/>
     </row>
-    <row r="10" spans="1:95" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>182</v>
+    <row r="10" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="72" t="s">
+        <v>181</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>6</v>
+        <v>186</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>183</v>
-      </c>
-      <c r="D10" s="89"/>
-      <c r="E10" s="92"/>
+        <v>184</v>
+      </c>
+      <c r="D10" s="112"/>
+      <c r="E10" s="115"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -4159,18 +4132,18 @@
       <c r="CO10" s="14"/>
       <c r="CP10" s="14"/>
     </row>
-    <row r="11" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="89"/>
-      <c r="E11" s="92"/>
+    <row r="11" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="121" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" s="119" t="s">
+        <v>187</v>
+      </c>
+      <c r="C11" s="111" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" s="112"/>
+      <c r="E11" s="115"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -4261,18 +4234,12 @@
       <c r="CO11" s="14"/>
       <c r="CP11" s="14"/>
     </row>
-    <row r="12" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="90"/>
-      <c r="E12" s="93"/>
+    <row r="12" spans="1:95" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="122"/>
+      <c r="B12" s="120"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="113"/>
+      <c r="E12" s="116"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -4364,13 +4331,13 @@
       <c r="CP12" s="14"/>
     </row>
     <row r="13" spans="1:95" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="80" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
+      <c r="A13" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -4463,19 +4430,19 @@
     </row>
     <row r="14" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="87" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="86" t="s">
-        <v>12</v>
+        <v>48</v>
+      </c>
+      <c r="D14" s="110" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="109" t="s">
+        <v>10</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -4569,16 +4536,16 @@
     </row>
     <row r="15" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="87"/>
-      <c r="E15" s="86"/>
+        <v>48</v>
+      </c>
+      <c r="D15" s="110"/>
+      <c r="E15" s="109"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
@@ -4670,13 +4637,13 @@
       <c r="CP15" s="14"/>
     </row>
     <row r="16" spans="1:95" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="96" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="97"/>
-      <c r="C16" s="97"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="98"/>
+      <c r="A16" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="87"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -4770,19 +4737,19 @@
     </row>
     <row r="17" spans="1:95" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C17" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="94" t="s">
-        <v>119</v>
-      </c>
-      <c r="E17" s="94" t="s">
-        <v>13</v>
+        <v>102</v>
+      </c>
+      <c r="D17" s="117" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="117" t="s">
+        <v>11</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="51"/>
@@ -4877,16 +4844,16 @@
     </row>
     <row r="18" spans="1:95" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="D18" s="95"/>
-      <c r="E18" s="94"/>
+        <v>100</v>
+      </c>
+      <c r="D18" s="118"/>
+      <c r="E18" s="117"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -4980,16 +4947,16 @@
     </row>
     <row r="19" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="95"/>
-      <c r="E19" s="94"/>
+        <v>98</v>
+      </c>
+      <c r="D19" s="118"/>
+      <c r="E19" s="117"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -5083,16 +5050,16 @@
     </row>
     <row r="20" spans="1:95" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="95"/>
-      <c r="E20" s="94"/>
+        <v>49</v>
+      </c>
+      <c r="D20" s="118"/>
+      <c r="E20" s="117"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -5184,14 +5151,14 @@
       <c r="CP20" s="14"/>
       <c r="CQ20" s="14"/>
     </row>
-    <row r="21" spans="1:95" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="80" t="s">
-        <v>193</v>
-      </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
+    <row r="21" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="99" t="s">
+        <v>192</v>
+      </c>
+      <c r="B21" s="105"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="105"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -5284,20 +5251,20 @@
       <c r="CQ21" s="14"/>
     </row>
     <row r="22" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="111" t="s">
-        <v>194</v>
-      </c>
-      <c r="B22" s="112" t="s">
-        <v>197</v>
-      </c>
-      <c r="C22" s="113" t="s">
-        <v>201</v>
-      </c>
-      <c r="D22" s="116" t="s">
-        <v>202</v>
-      </c>
-      <c r="E22" s="116" t="s">
-        <v>203</v>
+      <c r="A22" s="81" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="83" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="100" t="s">
+        <v>176</v>
+      </c>
+      <c r="E22" s="100" t="s">
+        <v>177</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -5391,17 +5358,17 @@
       <c r="CQ22" s="14"/>
     </row>
     <row r="23" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="111" t="s">
-        <v>195</v>
-      </c>
-      <c r="B23" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="C23" s="113" t="s">
-        <v>201</v>
-      </c>
-      <c r="D23" s="115"/>
-      <c r="E23" s="118"/>
+      <c r="A23" s="81" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="82" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="83" t="s">
+        <v>175</v>
+      </c>
+      <c r="D23" s="101"/>
+      <c r="E23" s="103"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -5494,17 +5461,17 @@
       <c r="CQ23" s="14"/>
     </row>
     <row r="24" spans="1:95" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A24" s="111" t="s">
-        <v>196</v>
-      </c>
-      <c r="B24" s="112" t="s">
-        <v>199</v>
-      </c>
-      <c r="C24" s="113" t="s">
-        <v>200</v>
-      </c>
-      <c r="D24" s="114"/>
-      <c r="E24" s="117"/>
+      <c r="A24" s="81" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" s="82" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="83" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" s="102"/>
+      <c r="E24" s="104"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -5597,13 +5564,13 @@
       <c r="CQ24" s="14"/>
     </row>
     <row r="25" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
+      <c r="A25" s="99" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" s="105"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="105"/>
+      <c r="E25" s="105"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
@@ -5697,19 +5664,19 @@
     </row>
     <row r="26" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="B26" s="55" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="C26" s="49" t="s">
-        <v>192</v>
-      </c>
-      <c r="D26" s="105" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="109" t="s">
-        <v>15</v>
+        <v>167</v>
+      </c>
+      <c r="D26" s="94" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="98" t="s">
+        <v>13</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -5804,16 +5771,16 @@
     </row>
     <row r="27" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="105"/>
-      <c r="E27" s="109"/>
+        <v>50</v>
+      </c>
+      <c r="D27" s="94"/>
+      <c r="E27" s="98"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
@@ -5907,19 +5874,19 @@
     </row>
     <row r="28" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="105"/>
-      <c r="E28" s="109"/>
+        <v>50</v>
+      </c>
+      <c r="D28" s="94"/>
+      <c r="E28" s="98"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
@@ -6012,16 +5979,16 @@
     </row>
     <row r="29" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="105"/>
-      <c r="E29" s="109"/>
+        <v>51</v>
+      </c>
+      <c r="D29" s="94"/>
+      <c r="E29" s="98"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
@@ -6115,16 +6082,16 @@
     </row>
     <row r="30" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="105"/>
-      <c r="E30" s="109"/>
+        <v>52</v>
+      </c>
+      <c r="D30" s="94"/>
+      <c r="E30" s="98"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -6218,16 +6185,16 @@
     </row>
     <row r="31" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="D31" s="105"/>
-      <c r="E31" s="109"/>
+        <v>95</v>
+      </c>
+      <c r="D31" s="94"/>
+      <c r="E31" s="98"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
@@ -6321,16 +6288,16 @@
     </row>
     <row r="32" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="105"/>
-      <c r="E32" s="109"/>
+        <v>53</v>
+      </c>
+      <c r="D32" s="94"/>
+      <c r="E32" s="98"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -6423,13 +6390,13 @@
       <c r="CQ32" s="14"/>
     </row>
     <row r="33" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="106" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="107"/>
-      <c r="C33" s="107"/>
-      <c r="D33" s="107"/>
-      <c r="E33" s="108"/>
+      <c r="A33" s="95" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="96"/>
+      <c r="C33" s="96"/>
+      <c r="D33" s="96"/>
+      <c r="E33" s="97"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
@@ -6523,19 +6490,19 @@
     </row>
     <row r="34" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" s="99" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="102" t="s">
-        <v>67</v>
+        <v>53</v>
+      </c>
+      <c r="D34" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="91" t="s">
+        <v>57</v>
       </c>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
@@ -6630,16 +6597,16 @@
     </row>
     <row r="35" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="100"/>
-      <c r="E35" s="103"/>
+        <v>54</v>
+      </c>
+      <c r="D35" s="89"/>
+      <c r="E35" s="92"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
@@ -6733,16 +6700,16 @@
     </row>
     <row r="36" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="101"/>
-      <c r="E36" s="104"/>
+        <v>25</v>
+      </c>
+      <c r="D36" s="90"/>
+      <c r="E36" s="93"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -6836,17 +6803,25 @@
     </row>
     <row r="37" spans="1:95" ht="51" x14ac:dyDescent="0.2">
       <c r="C37" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="20" t="s">
-        <v>10</v>
-      </c>
       <c r="E37" s="20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="24">
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="E17:E20"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A16:E16"/>
@@ -6863,23 +6838,17 @@
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="D3:D6"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="E17:E20"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" location="/dashboard" display="https://acleddata.com/dashboard/ - /dashboard" xr:uid="{F76E7675-2B2E-2D45-8C2B-2CB43E3D6E32}"/>
-    <hyperlink ref="B12" r:id="rId2" display="https://oefdatascience.github.io/REIGN.github.io/" xr:uid="{2AEFFF55-2CCA-7F42-82FE-4DED88CAF0DE}"/>
-    <hyperlink ref="B14" r:id="rId3" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
-    <hyperlink ref="B15" r:id="rId4" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
-    <hyperlink ref="B20" r:id="rId5" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
-    <hyperlink ref="B32" r:id="rId6" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
-    <hyperlink ref="B3" r:id="rId7" display="https://fews.net/" xr:uid="{3D674EBD-4EF9-1342-883D-87D2B91B65D7}"/>
-    <hyperlink ref="B6" r:id="rId8" display="https://www.acaps.org/countries" xr:uid="{323C0C04-FA1B-0C4D-B8B5-EB4AF4D1488B}"/>
-    <hyperlink ref="B17" r:id="rId9" display="COVID Economic Stimus Index (as measured by Elgin et al)" xr:uid="{999A8B13-E27C-374A-82CC-F226FAFAE1F4}"/>
+    <hyperlink ref="B14" r:id="rId2" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
+    <hyperlink ref="B15" r:id="rId3" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
+    <hyperlink ref="B20" r:id="rId4" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
+    <hyperlink ref="B32" r:id="rId5" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
+    <hyperlink ref="B3" r:id="rId6" display="https://fews.net/" xr:uid="{3D674EBD-4EF9-1342-883D-87D2B91B65D7}"/>
+    <hyperlink ref="B6" r:id="rId7" display="https://www.acaps.org/countries" xr:uid="{323C0C04-FA1B-0C4D-B8B5-EB4AF4D1488B}"/>
+    <hyperlink ref="B17" r:id="rId8" display="COVID Economic Stimus Index (as measured by Elgin et al)" xr:uid="{999A8B13-E27C-374A-82CC-F226FAFAE1F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6890,10 +6859,10 @@
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="114" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6905,223 +6874,299 @@
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="71" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="96" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-    </row>
-    <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="85" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+    </row>
+    <row r="3" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="72" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="96" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="97"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-    </row>
-    <row r="5" spans="1:7" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="110" t="s">
-        <v>189</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="85" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="87"/>
+    </row>
+    <row r="5" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="80" t="s">
+        <v>164</v>
       </c>
       <c r="B5" s="78" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C5" s="78"/>
       <c r="D5" s="78"/>
       <c r="E5" s="78"/>
-    </row>
-    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="80" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-    </row>
-    <row r="7" spans="1:7" ht="159" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="85"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="87"/>
+    </row>
+    <row r="6" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="99" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="105"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="105"/>
+    </row>
+    <row r="7" spans="1:12" ht="159" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="85"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="87"/>
+    </row>
+    <row r="8" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="85" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+    </row>
+    <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="99"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="105"/>
+    </row>
+    <row r="10" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="99" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="105"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="95"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="97"/>
+    </row>
+    <row r="11" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="74" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="124"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="124"/>
+    </row>
+    <row r="12" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12" s="69" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="70"/>
+      <c r="G12" s="46"/>
+    </row>
+    <row r="13" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="95" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="96"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="G13" s="45"/>
+    </row>
+    <row r="14" spans="1:12" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="63" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>198</v>
+      </c>
+      <c r="C14" s="65" t="s">
+        <v>199</v>
+      </c>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="G14" s="45"/>
+    </row>
+    <row r="15" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="63" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" s="35"/>
+      <c r="G15" s="45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="99" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="105"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+    </row>
+    <row r="17" spans="1:6" ht="248" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="75" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G7" s="45" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="96" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="97"/>
-      <c r="C8" s="97"/>
-      <c r="D8" s="97"/>
-      <c r="G8" s="46"/>
-    </row>
-    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" s="46" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="82"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="G10" s="47"/>
-    </row>
-    <row r="11" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="74" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="68" t="s">
-        <v>161</v>
-      </c>
-      <c r="E11" s="69" t="s">
-        <v>162</v>
-      </c>
-      <c r="F11" s="70"/>
-      <c r="G11" s="46"/>
-    </row>
-    <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="106" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="107"/>
-      <c r="C12" s="107"/>
-      <c r="D12" s="107"/>
-      <c r="G12" s="45"/>
-    </row>
-    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="63" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" s="65" t="s">
-        <v>159</v>
-      </c>
-      <c r="C13" s="66" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" s="67" t="s">
-        <v>160</v>
-      </c>
-      <c r="E13" s="35"/>
-      <c r="G13" s="45" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="106" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="107"/>
-      <c r="C14" s="107"/>
-      <c r="D14" s="107"/>
-    </row>
-    <row r="15" spans="1:7" ht="248" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="75" t="s">
-        <v>186</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="E15" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="F15" s="44" t="s">
-        <v>75</v>
+      <c r="F17" s="44" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="14">
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="H5:L5"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="H8:L8"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A14:D14"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A6:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="WFP Proteus composite index: " xr:uid="{3B8342E4-A803-C342-923C-31BDAA92A373}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{95E245AA-F0BF-3C40-B212-C5EC3EDEDF2E}"/>
-    <hyperlink ref="D13" r:id="rId3" location=":~:text=INFORM%20Index%20for%20Risk%20Management%3A%20Concept%20and%20Methodology%2C%20Version%202017,-%C2%A9EU&amp;text=INFORM%20is%20a%20composite%20indicator,crisis%20and%20disaster%20management%20framework." xr:uid="{AF872891-F870-AA4C-B416-4F92600B17AE}"/>
-    <hyperlink ref="D11" r:id="rId4" xr:uid="{26B58F35-C97D-3F48-B110-F642D3427351}"/>
-    <hyperlink ref="E11" r:id="rId5" xr:uid="{2B1483A5-6E05-4E4E-A8CB-95D622233E3B}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{95E245AA-F0BF-3C40-B212-C5EC3EDEDF2E}"/>
+    <hyperlink ref="D15" r:id="rId3" location=":~:text=INFORM%20Index%20for%20Risk%20Management%3A%20Concept%20and%20Methodology%2C%20Version%202017,-%C2%A9EU&amp;text=INFORM%20is%20a%20composite%20indicator,crisis%20and%20disaster%20management%20framework." xr:uid="{AF872891-F870-AA4C-B416-4F92600B17AE}"/>
+    <hyperlink ref="D12" r:id="rId4" xr:uid="{26B58F35-C97D-3F48-B110-F642D3427351}"/>
+    <hyperlink ref="E12" r:id="rId5" xr:uid="{2B1483A5-6E05-4E4E-A8CB-95D622233E3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId6"/>
@@ -7148,46 +7193,46 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B2" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B3" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B4" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>47</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -7200,10 +7245,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E658424-6FDF-FB4F-A908-E363FB27277D}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7212,78 +7257,122 @@
     <col min="2" max="2" width="53.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>190</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E2" s="85"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="87"/>
+    </row>
+    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>191</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+      <c r="E3" s="85"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="87"/>
+    </row>
+    <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="E4" s="99"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+    </row>
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+      <c r="E5" s="85"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="87"/>
+    </row>
+    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="E6" s="99"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="105"/>
+    </row>
+    <row r="7" spans="1:9" ht="53" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="E7" s="99"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="105"/>
+      <c r="I7" s="105"/>
+    </row>
+    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>206</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>178</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="E8" s="95"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="97"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="79" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="E7:I7"/>
+  </mergeCells>
   <conditionalFormatting sqref="B2:B8">
-    <cfRule type="containsBlanks" dxfId="6" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7295,8 +7384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FAE3D5-1E62-BD47-A72D-971150914E15}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7309,533 +7398,539 @@
     <col min="6" max="6" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="61"/>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="61"/>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="63" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="77" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C14" s="72" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C15" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" t="s">
+        <v>191</v>
+      </c>
+      <c r="C16" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="D16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="127" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" s="125" t="s">
+        <v>182</v>
+      </c>
+      <c r="D17" s="126" t="s">
+        <v>203</v>
+      </c>
+      <c r="F17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" s="84" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="D21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C22" s="84" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" t="s">
+        <v>205</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" t="s">
+        <v>205</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="59" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="59" t="s">
+      <c r="D30" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="59" t="s">
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D31" t="s">
         <v>131</v>
       </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" t="s">
+        <v>205</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" t="s">
         <v>132</v>
-      </c>
-      <c r="E2" s="61"/>
-    </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="D3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="D5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="60" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="63" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="64" t="s">
-        <v>186</v>
-      </c>
-      <c r="D8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="77" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>138</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="77" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>138</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>138</v>
-      </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>138</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="D15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>138</v>
-      </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" t="s">
-        <v>141</v>
-      </c>
-      <c r="F16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>138</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>138</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="119" t="s">
-        <v>194</v>
-      </c>
-      <c r="D20" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>138</v>
-      </c>
-      <c r="B21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="119" t="s">
-        <v>195</v>
-      </c>
-      <c r="D21" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>138</v>
-      </c>
-      <c r="B22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="119" t="s">
-        <v>196</v>
-      </c>
-      <c r="D22" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>138</v>
-      </c>
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>138</v>
-      </c>
-      <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>138</v>
-      </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>138</v>
-      </c>
-      <c r="B26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>138</v>
-      </c>
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="D27" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>138</v>
-      </c>
-      <c r="B28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="D28" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>138</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>138</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D30" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>138</v>
-      </c>
-      <c r="B31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D31" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>138</v>
-      </c>
-      <c r="B32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>205</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="D33" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" t="s">
         <v>138</v>
       </c>
-      <c r="B36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" t="s">
-        <v>157</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19 D23:D36">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+  <conditionalFormatting sqref="D23:D36 D2 D4:D19">
+    <cfRule type="containsBlanks" dxfId="4" priority="7">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="3" priority="6">
       <formula>LEN(TRIM(D20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(D22))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(D21))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(D21))=0</formula>
+      <formula>LEN(TRIM(D3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding another debt indicator (D_CPIA.scores_norm)
Changing FPV indicator to WB database (rather than an external one)

Adding a macro indicator based on WB database (M_macrofin_risk_norm)
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B993026-9964-B040-9AA3-30725D812634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E192DC6E-FED1-D146-AA48-689B05095186}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3220" yWindow="-18680" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="208">
   <si>
     <t>Bi-weekly percentage change in COVID cases (per 1M)</t>
   </si>
@@ -692,19 +692,12 @@
     <t>Metric to track if price of one or more basic food commodities is abnormally high in main markets (identified using FAO Indicator of Price Anomaly and GIEWS)</t>
   </si>
   <si>
-    <t>Metric to track if country is affected by famine or food crises as reported under the ACAPS real-time risk repository</t>
-  </si>
-  <si>
     <t>High &gt;= 0.2
 Low &lt;=  0</t>
   </si>
   <si>
     <t>10 = above IPA threshold
 0 = below IPA threshold</t>
-  </si>
-  <si>
-    <t>10 = ACAPS famine/food crisis
-0 = Otherwise</t>
   </si>
   <si>
     <t>H_GovernmentResponseIndexForDisplay</t>
@@ -772,6 +765,458 @@
   </si>
   <si>
     <t>COVID Economic Stimulus Index (as measured by Elgin et al)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> FEWSNET country then FS_SQ = FS,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ELSE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> FS_SQ = GEOMETRICMEAN(EXISTING_RISK_FS, FS)
+Note: FS calculated as max values</t>
+    </r>
+  </si>
+  <si>
+    <t>Risk Category</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Existing/Emerging</t>
+  </si>
+  <si>
+    <t>Indicator Key</t>
+  </si>
+  <si>
+    <t>Indicator Label</t>
+  </si>
+  <si>
+    <t>Existing</t>
+  </si>
+  <si>
+    <t>Proteus Food Security Index</t>
+  </si>
+  <si>
+    <t>Fragility Index (WB)</t>
+  </si>
+  <si>
+    <t>Economic and Financial Dependence</t>
+  </si>
+  <si>
+    <t>Debt Distress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global Health Security Index </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seasonal Natural Hazard Risk </t>
+  </si>
+  <si>
+    <t>Emerging</t>
+  </si>
+  <si>
+    <t>FEWSNET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARTEMIS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projected COVID deaths </t>
+  </si>
+  <si>
+    <t>H_Covidgrowth_casesnorm,</t>
+  </si>
+  <si>
+    <t>H_Covidgrowth_deathsnorm,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth in COVID deaths </t>
+  </si>
+  <si>
+    <t>H_new_cases_smoothed_per_million_norm,</t>
+  </si>
+  <si>
+    <t>Current new COVID cases</t>
+  </si>
+  <si>
+    <t>H_new_deaths_smoothed_per_million_norm,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current new COVID deaths </t>
+  </si>
+  <si>
+    <t>Government Response Index</t>
+  </si>
+  <si>
+    <t>Economic Support Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H_Oxrollback_score_norm, </t>
+  </si>
+  <si>
+    <t>COVID Rollback Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projected Seasonal Hazards </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongoing Crisis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ongoign Natural Hazard </t>
+  </si>
+  <si>
+    <t>NH_Hazard_Score_norm</t>
+  </si>
+  <si>
+    <t>Natural multi-hazard rating (INFORM) – 2020 data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical rates of exposure and sensitivity to earthquake, tsunami, flood, cyclone, storm surge and drought risk. For more details see link. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GHS is made up of six categories (comrised of 34 indicators, 85 sub-indicators). The categories include: prevention; detection and reporting; rapid response; health system; compliance with international norms; and risk environment. For more details see link. </t>
+  </si>
+  <si>
+    <t>Aggregation primarily achieved through a Principle Components Analysis (PCA) with expert derived weights. See link for more details.</t>
+  </si>
+  <si>
+    <t>Food Prive Volatility</t>
+  </si>
+  <si>
+    <t>Ongoing Food Crisis/Famine</t>
+  </si>
+  <si>
+    <t>% Fiscal Stimulus to GDP</t>
+  </si>
+  <si>
+    <t>COVID Economic Stimulus Index</t>
+  </si>
+  <si>
+    <t>Change in Borrowing/Lending</t>
+  </si>
+  <si>
+    <t>Difference in Projected GDP (WB)</t>
+  </si>
+  <si>
+    <t>Difference in Projected GDP (IMF)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth in COVID cases </t>
+  </si>
+  <si>
+    <t>Oxford Government Response Index (Oxford University - Blavatnik)</t>
+  </si>
+  <si>
+    <t>Oxford Lockdown rollback index (Oxford University - Blavatnik, source)</t>
+  </si>
+  <si>
+    <t>A measure of availability and access to food</t>
+  </si>
+  <si>
+    <t>A measure of a country's exposure and resilience to a variety of natural and seasonal hazards, including earthquakes, tsunamis, floods, cyclones, storm surge, pests and drought risk</t>
+  </si>
+  <si>
+    <t>A multi-dimensional measure of socio-economic vulnerability, focused predominantly on household level dynamics</t>
+  </si>
+  <si>
+    <t>A measure of institutional and social fragility as well as likehood of violent conflict</t>
+  </si>
+  <si>
+    <t>A measure of a country's exposure and resilience to macro-economic shock, focused primarily on economic and financial dependence</t>
+  </si>
+  <si>
+    <t>A measure of a country's fiscal risk, focused predominantly on debt burden as well as fiscal stimulus in response to COVID</t>
+  </si>
+  <si>
+    <t>A measure of a country's exposure and response capacity to pandemic (note: indicators for emerging risk are targetted specifically at COVID-related dynamics)</t>
+  </si>
+  <si>
+    <t>S_INFORM_vul_norm</t>
+  </si>
+  <si>
+    <t>Socio-economic Vulnerability Index (INFORM)</t>
+  </si>
+  <si>
+    <t>D_WB_external_debt_distress_norm</t>
+  </si>
+  <si>
+    <t>Fr_number_flags_norm</t>
+  </si>
+  <si>
+    <t>H_add_death_prec_current_norm</t>
+  </si>
+  <si>
+    <t>8-week COVID-19 projected deaths as a percentage of current deaths (USC)</t>
+  </si>
+  <si>
+    <t>10 &gt; 100 pct
+0 &lt;  pct</t>
+  </si>
+  <si>
+    <t>S_gdp_change.Rating_norm</t>
+  </si>
+  <si>
+    <t>S_unemployment.Rating_norm</t>
+  </si>
+  <si>
+    <t>S_income_support.Rating_norm</t>
+  </si>
+  <si>
+    <t>Change in GDP growth (INFORM COVID Warning tool)</t>
+  </si>
+  <si>
+    <t>Unemployment rate</t>
+  </si>
+  <si>
+    <t>Whether income support is provided</t>
+  </si>
+  <si>
+    <t>10 = Government replacing &gt; 50% of lost salary
+7 = Government replacing &lt; 50% of lost salary
+0 = No income support</t>
+  </si>
+  <si>
+    <t>INFORM threshold</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">S = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>MAX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>(S_gdp_change.Rating_norm
+S_unemployment.Rating_norm
+S_income_support.Rating_norm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">S_SQ = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>GEOMETRICMEAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>(EXISTING_RISK_SOCIOECONOMIC, S)</t>
+    </r>
+  </si>
+  <si>
+    <t>INFORM COVID Warning Tracker (EU)</t>
+  </si>
+  <si>
+    <t>Fr_combined_crisis_norm</t>
+  </si>
+  <si>
+    <t>Fr_state6m_norm</t>
+  </si>
+  <si>
+    <t>Fr_nonstate6m_norm</t>
+  </si>
+  <si>
+    <t>Fr_oneside6m_norm</t>
+  </si>
+  <si>
+    <t>Measure of whether a country is currently experiencing a crisis (based on the INFORM severty index)</t>
+  </si>
+  <si>
+    <t>10 &gt; 0.8
+0 &lt; 0.1</t>
+  </si>
+  <si>
+    <r>
+      <t>Likelihood of state-led violence in the next 6-months</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">(ViEWS) </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Likelihood of non-state violence in the next 6-months (ViEWS) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Likelihood of one-sided violence in the next 6-months (ViEWS) </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fr = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>MAX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>(Fr_combined_crisis_norm
+Fr_state6m_norm
+Fr_nonstate6m_norm
+Fr_oneside6m_norm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10 = Severity &gt; 3 &amp; Conditions worsening </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Severity &gt; 4 
+0 = Otherwise</t>
+    </r>
+  </si>
+  <si>
+    <t>FOOD SECURITY</t>
+  </si>
+  <si>
+    <t>CONFLICT AND FRAGILITY</t>
+  </si>
+  <si>
+    <t>SOCIO-ECONOMIC VULNERABILITY</t>
+  </si>
+  <si>
+    <t>COVID EXPOSURE AND RESPONSE CAPACITY</t>
+  </si>
+  <si>
+    <t>H_INFORM_rating.Value_norm</t>
+  </si>
+  <si>
+    <t>INFORM COVID vulnerability index (composite index)</t>
+  </si>
+  <si>
+    <t>10 &lt; 2
+0 &lt; 6</t>
+  </si>
+  <si>
+    <t>NH_multihazard_risk_norm</t>
+  </si>
+  <si>
+    <t>ThinkHazard! Database of natural hazard risks (World Bank)</t>
+  </si>
+  <si>
+    <t>10 &gt; 4 high risk hazards 
+0 = 0 high risk hazards</t>
+  </si>
+  <si>
+    <t>Ongoing crisis (ACAPS)</t>
+  </si>
+  <si>
+    <t>Likelihood of state-sponsored violence (ViEWS)</t>
+  </si>
+  <si>
+    <t>Likelihood of non-state violence (ViEWS)</t>
+  </si>
+  <si>
+    <t>Likelihood of one-sided violence (ViEWS)</t>
+  </si>
+  <si>
+    <t>Multi-hazard exposure (WB)</t>
+  </si>
+  <si>
+    <t>COVID RESPONSE AND RESPONSE CAPACITY</t>
+  </si>
+  <si>
+    <t>SOCIOECONOMIC VULNERABILITY</t>
   </si>
   <si>
     <r>
@@ -830,460 +1275,18 @@
         <rFont val="Garamond"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> FS = MAX(F_fpv_alt, F_food_acaps)</t>
+      <t xml:space="preserve"> FS = F_fpv_alt</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>IF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> FEWSNET country then FS_SQ = FS,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> ELSE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> FS_SQ = GEOMETRICMEAN(EXISTING_RISK_FS, FS)
-Note: FS calculated as max values</t>
-    </r>
-  </si>
-  <si>
-    <t>Risk Category</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Existing/Emerging</t>
-  </si>
-  <si>
-    <t>Indicator Key</t>
-  </si>
-  <si>
-    <t>Indicator Label</t>
-  </si>
-  <si>
-    <t>Existing</t>
-  </si>
-  <si>
-    <t>Proteus Food Security Index</t>
-  </si>
-  <si>
-    <t>Fragility Index (WB)</t>
-  </si>
-  <si>
-    <t>Economic and Financial Dependence</t>
-  </si>
-  <si>
-    <t>Debt Distress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global Health Security Index </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seasonal Natural Hazard Risk </t>
-  </si>
-  <si>
-    <t>Emerging</t>
-  </si>
-  <si>
-    <t>FEWSNET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARTEMIS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projected COVID deaths </t>
-  </si>
-  <si>
-    <t>H_Covidgrowth_casesnorm,</t>
-  </si>
-  <si>
-    <t>H_Covidgrowth_deathsnorm,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Growth in COVID deaths </t>
-  </si>
-  <si>
-    <t>H_new_cases_smoothed_per_million_norm,</t>
-  </si>
-  <si>
-    <t>Current new COVID cases</t>
-  </si>
-  <si>
-    <t>H_new_deaths_smoothed_per_million_norm,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current new COVID deaths </t>
-  </si>
-  <si>
-    <t>Government Response Index</t>
-  </si>
-  <si>
-    <t>Economic Support Index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H_Oxrollback_score_norm, </t>
-  </si>
-  <si>
-    <t>COVID Rollback Score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projected Seasonal Hazards </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ongoing Crisis </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ongoign Natural Hazard </t>
-  </si>
-  <si>
-    <t>NH_Hazard_Score_norm</t>
-  </si>
-  <si>
-    <t>Natural multi-hazard rating (INFORM) – 2020 data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Historical rates of exposure and sensitivity to earthquake, tsunami, flood, cyclone, storm surge and drought risk. For more details see link. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GHS is made up of six categories (comrised of 34 indicators, 85 sub-indicators). The categories include: prevention; detection and reporting; rapid response; health system; compliance with international norms; and risk environment. For more details see link. </t>
-  </si>
-  <si>
-    <t>Aggregation primarily achieved through a Principle Components Analysis (PCA) with expert derived weights. See link for more details.</t>
-  </si>
-  <si>
-    <t>Food Prive Volatility</t>
-  </si>
-  <si>
-    <t>Ongoing Food Crisis/Famine</t>
-  </si>
-  <si>
-    <t>% Fiscal Stimulus to GDP</t>
-  </si>
-  <si>
-    <t>COVID Economic Stimulus Index</t>
-  </si>
-  <si>
-    <t>Change in Borrowing/Lending</t>
-  </si>
-  <si>
-    <t>Difference in Projected GDP (WB)</t>
-  </si>
-  <si>
-    <t>Difference in Projected GDP (IMF)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Growth in COVID cases </t>
-  </si>
-  <si>
-    <t>Oxford Government Response Index (Oxford University - Blavatnik)</t>
-  </si>
-  <si>
-    <t>Oxford Lockdown rollback index (Oxford University - Blavatnik, source)</t>
-  </si>
-  <si>
-    <t>A measure of availability and access to food</t>
-  </si>
-  <si>
-    <t>A measure of a country's exposure and resilience to a variety of natural and seasonal hazards, including earthquakes, tsunamis, floods, cyclones, storm surge, pests and drought risk</t>
-  </si>
-  <si>
-    <t>A multi-dimensional measure of socio-economic vulnerability, focused predominantly on household level dynamics</t>
-  </si>
-  <si>
-    <t>A measure of institutional and social fragility as well as likehood of violent conflict</t>
-  </si>
-  <si>
-    <t>A measure of a country's exposure and resilience to macro-economic shock, focused primarily on economic and financial dependence</t>
-  </si>
-  <si>
-    <t>A measure of a country's fiscal risk, focused predominantly on debt burden as well as fiscal stimulus in response to COVID</t>
-  </si>
-  <si>
-    <t>A measure of a country's exposure and response capacity to pandemic (note: indicators for emerging risk are targetted specifically at COVID-related dynamics)</t>
-  </si>
-  <si>
-    <t>S_INFORM_vul_norm</t>
-  </si>
-  <si>
-    <t>Socio-economic Vulnerability Index (INFORM)</t>
-  </si>
-  <si>
-    <t>D_WB_external_debt_distress_norm</t>
-  </si>
-  <si>
-    <t>Fr_number_flags_norm</t>
-  </si>
-  <si>
-    <t>H_add_death_prec_current_norm</t>
-  </si>
-  <si>
-    <t>8-week COVID-19 projected deaths as a percentage of current deaths (USC)</t>
-  </si>
-  <si>
-    <t>10 &gt; 100 pct
-0 &lt;  pct</t>
-  </si>
-  <si>
-    <t>S_gdp_change.Rating_norm</t>
-  </si>
-  <si>
-    <t>S_unemployment.Rating_norm</t>
-  </si>
-  <si>
-    <t>S_income_support.Rating_norm</t>
-  </si>
-  <si>
-    <t>Change in GDP growth (INFORM COVID Warning tool)</t>
-  </si>
-  <si>
-    <t>Unemployment rate</t>
-  </si>
-  <si>
-    <t>Whether income support is provided</t>
-  </si>
-  <si>
-    <t>10 = Government replacing &gt; 50% of lost salary
-7 = Government replacing &lt; 50% of lost salary
-0 = No income support</t>
-  </si>
-  <si>
-    <t>INFORM threshold</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">S = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>MAX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>(S_gdp_change.Rating_norm
-S_unemployment.Rating_norm
-S_income_support.Rating_norm)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">S_SQ = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>GEOMETRICMEAN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>(EXISTING_RISK_SOCIOECONOMIC, S)</t>
-    </r>
-  </si>
-  <si>
-    <t>INFORM COVID Warning Tracker (EU)</t>
-  </si>
-  <si>
-    <t>Fr_combined_crisis_norm</t>
-  </si>
-  <si>
-    <t>Fr_state6m_norm</t>
-  </si>
-  <si>
-    <t>Fr_nonstate6m_norm</t>
-  </si>
-  <si>
-    <t>Fr_oneside6m_norm</t>
-  </si>
-  <si>
-    <t>Measure of whether a country is currently experiencing a crisis (based on the INFORM severty index)</t>
-  </si>
-  <si>
-    <t>10 &gt; 0.8
-0 &lt; 0.1</t>
-  </si>
-  <si>
-    <r>
-      <t>Likelihood of state-led violence in the next 6-months</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">(ViEWS) </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Likelihood of non-state violence in the next 6-months (ViEWS) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Likelihood of one-sided violence in the next 6-months (ViEWS) </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fr = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>MAX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>(Fr_combined_crisis_norm
-Fr_state6m_norm
-Fr_nonstate6m_norm
-Fr_oneside6m_norm)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">10 = Severity &gt; 3 &amp; Conditions worsening </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Severity &gt; 4 
-0 = Otherwise</t>
-    </r>
-  </si>
-  <si>
-    <t>FOOD SECURITY</t>
-  </si>
-  <si>
-    <t>CONFLICT AND FRAGILITY</t>
-  </si>
-  <si>
-    <t>SOCIO-ECONOMIC VULNERABILITY</t>
-  </si>
-  <si>
-    <t>COVID EXPOSURE AND RESPONSE CAPACITY</t>
-  </si>
-  <si>
-    <t>H_INFORM_rating.Value_norm</t>
-  </si>
-  <si>
-    <t>INFORM COVID vulnerability index (composite index)</t>
-  </si>
-  <si>
-    <t>10 &lt; 2
-0 &lt; 6</t>
-  </si>
-  <si>
-    <t>NH_multihazard_risk_norm</t>
-  </si>
-  <si>
-    <t>ThinkHazard! Database of natural hazard risks (World Bank)</t>
-  </si>
-  <si>
-    <t>10 &gt; 4 high risk hazards 
-0 = 0 high risk hazards</t>
-  </si>
-  <si>
-    <t>Ongoing crisis (ACAPS)</t>
-  </si>
-  <si>
-    <t>Likelihood of state-sponsored violence (ViEWS)</t>
-  </si>
-  <si>
-    <t>Likelihood of non-state violence (ViEWS)</t>
-  </si>
-  <si>
-    <t>Likelihood of one-sided violence (ViEWS)</t>
-  </si>
-  <si>
-    <t>Multi-hazard exposure (WB)</t>
-  </si>
-  <si>
-    <t>COVID RESPONSE AND RESPONSE CAPACITY</t>
-  </si>
-  <si>
-    <t>SOCIOECONOMIC VULNERABILITY</t>
+    <t>M_macrofin_risk_norm</t>
+  </si>
+  <si>
+    <t>WBG Macrofin heatmap</t>
+  </si>
+  <si>
+    <t>10 &lt; 4 risks
+0 = 0 risks</t>
   </si>
 </sst>
 </file>
@@ -1548,7 +1551,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1727,12 +1730,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1960,6 +2002,59 @@
     <xf numFmtId="0" fontId="6" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2005,6 +2100,9 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2020,9 +2118,6 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2035,56 +2130,24 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3176,10 +3239,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:CQ37"/>
+  <dimension ref="A1:CQ38"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:E13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3211,13 +3274,13 @@
       </c>
     </row>
     <row r="2" spans="1:95" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
-        <v>190</v>
-      </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87"/>
+      <c r="A2" s="104" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="106"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -3319,11 +3382,11 @@
       <c r="C3" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="110" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="106" t="s">
-        <v>108</v>
+      <c r="D3" s="97" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="125" t="s">
+        <v>105</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -3424,10 +3487,10 @@
         <v>31</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="110"/>
-      <c r="E4" s="107"/>
+        <v>90</v>
+      </c>
+      <c r="D4" s="97"/>
+      <c r="E4" s="126"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -3519,18 +3582,18 @@
       <c r="CP4" s="14"/>
       <c r="CQ4" s="14"/>
     </row>
-    <row r="5" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+    <row r="5" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="130" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="131" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="110"/>
-      <c r="E5" s="107"/>
+      <c r="C5" s="133" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="97"/>
+      <c r="E5" s="126"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -3622,18 +3685,12 @@
       <c r="CP5" s="14"/>
       <c r="CQ5" s="14"/>
     </row>
-    <row r="6" spans="1:95" s="1" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="110"/>
-      <c r="E6" s="108"/>
+    <row r="6" spans="1:95" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="129"/>
+      <c r="B6" s="132"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="127"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -3725,13 +3782,13 @@
       <c r="CP6" s="14"/>
     </row>
     <row r="7" spans="1:95" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="85" t="s">
-        <v>191</v>
-      </c>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="87"/>
+      <c r="A7" s="104" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="105"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="106"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -3824,18 +3881,18 @@
     </row>
     <row r="8" spans="1:95" s="2" customFormat="1" ht="89" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="72" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="D8" s="111" t="s">
-        <v>188</v>
-      </c>
-      <c r="E8" s="114" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="91" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" s="99" t="s">
         <v>55</v>
       </c>
       <c r="F8" s="14"/>
@@ -3930,16 +3987,16 @@
     </row>
     <row r="9" spans="1:95" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="72" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="D9" s="112"/>
-      <c r="E9" s="115"/>
+        <v>181</v>
+      </c>
+      <c r="D9" s="98"/>
+      <c r="E9" s="100"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -4032,16 +4089,16 @@
     </row>
     <row r="10" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="72" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="D10" s="112"/>
-      <c r="E10" s="115"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="100"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -4133,17 +4190,17 @@
       <c r="CP10" s="14"/>
     </row>
     <row r="11" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="121" t="s">
-        <v>182</v>
-      </c>
-      <c r="B11" s="119" t="s">
-        <v>187</v>
-      </c>
-      <c r="C11" s="111" t="s">
+      <c r="A11" s="95" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="93" t="s">
         <v>184</v>
       </c>
-      <c r="D11" s="112"/>
-      <c r="E11" s="115"/>
+      <c r="C11" s="91" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="98"/>
+      <c r="E11" s="100"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -4235,11 +4292,11 @@
       <c r="CP11" s="14"/>
     </row>
     <row r="12" spans="1:95" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="122"/>
-      <c r="B12" s="120"/>
-      <c r="C12" s="113"/>
-      <c r="D12" s="113"/>
-      <c r="E12" s="116"/>
+      <c r="A12" s="96"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="101"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -4331,13 +4388,13 @@
       <c r="CP12" s="14"/>
     </row>
     <row r="13" spans="1:95" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="99" t="s">
+      <c r="A13" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="105"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="119"/>
+      <c r="D13" s="119"/>
+      <c r="E13" s="119"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -4438,10 +4495,10 @@
       <c r="C14" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="110" t="s">
+      <c r="D14" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="109" t="s">
+      <c r="E14" s="128" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="14"/>
@@ -4534,7 +4591,7 @@
       <c r="CO14" s="14"/>
       <c r="CP14" s="14"/>
     </row>
-    <row r="15" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
@@ -4544,8 +4601,8 @@
       <c r="C15" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="110"/>
-      <c r="E15" s="109"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="128"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
@@ -4636,14 +4693,18 @@
       <c r="CO15" s="14"/>
       <c r="CP15" s="14"/>
     </row>
-    <row r="16" spans="1:95" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="85" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="87"/>
+    <row r="16" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" s="85" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="97"/>
+      <c r="E16" s="128"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -4733,26 +4794,17 @@
       <c r="CN16" s="14"/>
       <c r="CO16" s="14"/>
       <c r="CP16" s="14"/>
-      <c r="CQ16" s="14"/>
-    </row>
-    <row r="17" spans="1:95" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="B17" s="52" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" s="117" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="117" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="17" spans="1:95" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="104" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="105"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="105"/>
+      <c r="E17" s="106"/>
       <c r="F17" s="14"/>
-      <c r="G17" s="51"/>
+      <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -4842,20 +4894,24 @@
       <c r="CP17" s="14"/>
       <c r="CQ17" s="14"/>
     </row>
-    <row r="18" spans="1:95" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:95" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="B18" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="C18" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="118"/>
-      <c r="E18" s="117"/>
+      <c r="D18" s="102" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="102" t="s">
+        <v>11</v>
+      </c>
       <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="G18" s="51"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -4945,9 +5001,9 @@
       <c r="CP18" s="14"/>
       <c r="CQ18" s="14"/>
     </row>
-    <row r="19" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:95" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B19" s="50" t="s">
         <v>97</v>
@@ -4955,8 +5011,8 @@
       <c r="C19" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="118"/>
-      <c r="E19" s="117"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="102"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -5048,18 +5104,18 @@
       <c r="CP19" s="14"/>
       <c r="CQ19" s="14"/>
     </row>
-    <row r="20" spans="1:95" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="118"/>
-      <c r="E20" s="117"/>
+        <v>94</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="103"/>
+      <c r="E20" s="102"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -5151,14 +5207,18 @@
       <c r="CP20" s="14"/>
       <c r="CQ20" s="14"/>
     </row>
-    <row r="21" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="99" t="s">
-        <v>192</v>
-      </c>
-      <c r="B21" s="105"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="105"/>
+    <row r="21" spans="1:95" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="103"/>
+      <c r="E21" s="102"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -5250,22 +5310,14 @@
       <c r="CP21" s="14"/>
       <c r="CQ21" s="14"/>
     </row>
-    <row r="22" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A22" s="81" t="s">
-        <v>168</v>
-      </c>
-      <c r="B22" s="82" t="s">
-        <v>171</v>
-      </c>
-      <c r="C22" s="83" t="s">
-        <v>175</v>
-      </c>
-      <c r="D22" s="100" t="s">
-        <v>176</v>
-      </c>
-      <c r="E22" s="100" t="s">
-        <v>177</v>
-      </c>
+    <row r="22" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="119"/>
+      <c r="C22" s="119"/>
+      <c r="D22" s="119"/>
+      <c r="E22" s="119"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -5357,18 +5409,22 @@
       <c r="CP22" s="14"/>
       <c r="CQ22" s="14"/>
     </row>
-    <row r="23" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="81" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B23" s="82" t="s">
+        <v>168</v>
+      </c>
+      <c r="C23" s="83" t="s">
         <v>172</v>
       </c>
-      <c r="C23" s="83" t="s">
-        <v>175</v>
-      </c>
-      <c r="D23" s="101"/>
-      <c r="E23" s="103"/>
+      <c r="D23" s="120" t="s">
+        <v>173</v>
+      </c>
+      <c r="E23" s="120" t="s">
+        <v>174</v>
+      </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -5460,18 +5516,18 @@
       <c r="CP23" s="14"/>
       <c r="CQ23" s="14"/>
     </row>
-    <row r="24" spans="1:95" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="81" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B24" s="82" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C24" s="83" t="s">
-        <v>174</v>
-      </c>
-      <c r="D24" s="102"/>
-      <c r="E24" s="104"/>
+        <v>172</v>
+      </c>
+      <c r="D24" s="121"/>
+      <c r="E24" s="123"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -5563,14 +5619,18 @@
       <c r="CP24" s="14"/>
       <c r="CQ24" s="14"/>
     </row>
-    <row r="25" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="99" t="s">
-        <v>193</v>
-      </c>
-      <c r="B25" s="105"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="105"/>
-      <c r="E25" s="105"/>
+    <row r="25" spans="1:95" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A25" s="81" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="82" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25" s="83" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="122"/>
+      <c r="E25" s="124"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
@@ -5662,22 +5722,14 @@
       <c r="CP25" s="14"/>
       <c r="CQ25" s="14"/>
     </row>
-    <row r="26" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="B26" s="55" t="s">
-        <v>166</v>
-      </c>
-      <c r="C26" s="49" t="s">
-        <v>167</v>
-      </c>
-      <c r="D26" s="94" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="98" t="s">
-        <v>13</v>
-      </c>
+    <row r="26" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="118" t="s">
+        <v>190</v>
+      </c>
+      <c r="B26" s="119"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="119"/>
+      <c r="E26" s="119"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -5769,18 +5821,22 @@
       <c r="CP26" s="14"/>
       <c r="CQ26" s="14"/>
     </row>
-    <row r="27" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>0</v>
+        <v>162</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>163</v>
       </c>
       <c r="C27" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="94"/>
-      <c r="E27" s="98"/>
+        <v>164</v>
+      </c>
+      <c r="D27" s="113" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="117" t="s">
+        <v>13</v>
+      </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
@@ -5874,20 +5930,18 @@
     </row>
     <row r="28" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="94"/>
-      <c r="E28" s="98"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="117"/>
       <c r="F28" s="14"/>
-      <c r="G28" s="14" t="s">
-        <v>58</v>
-      </c>
+      <c r="G28" s="14"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
@@ -5979,18 +6033,20 @@
     </row>
     <row r="29" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="94"/>
-      <c r="E29" s="98"/>
+        <v>50</v>
+      </c>
+      <c r="D29" s="113"/>
+      <c r="E29" s="117"/>
       <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="G29" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
@@ -6082,16 +6138,16 @@
     </row>
     <row r="30" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="94"/>
-      <c r="E30" s="98"/>
+        <v>51</v>
+      </c>
+      <c r="D30" s="113"/>
+      <c r="E30" s="117"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -6185,16 +6241,16 @@
     </row>
     <row r="31" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>152</v>
+        <v>3</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="94"/>
-      <c r="E31" s="98"/>
+        <v>52</v>
+      </c>
+      <c r="D31" s="113"/>
+      <c r="E31" s="117"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
@@ -6288,16 +6344,16 @@
     </row>
     <row r="32" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="94"/>
-      <c r="E32" s="98"/>
+        <v>93</v>
+      </c>
+      <c r="D32" s="113"/>
+      <c r="E32" s="117"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -6389,14 +6445,18 @@
       <c r="CP32" s="14"/>
       <c r="CQ32" s="14"/>
     </row>
-    <row r="33" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="95" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="97"/>
+    <row r="33" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="113"/>
+      <c r="E33" s="117"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
@@ -6488,22 +6548,14 @@
       <c r="CP33" s="14"/>
       <c r="CQ33" s="14"/>
     </row>
-    <row r="34" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="88" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="91" t="s">
-        <v>57</v>
-      </c>
+    <row r="34" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="114" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="115"/>
+      <c r="C34" s="115"/>
+      <c r="D34" s="115"/>
+      <c r="E34" s="116"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
@@ -6595,18 +6647,22 @@
       <c r="CP34" s="14"/>
       <c r="CQ34" s="14"/>
     </row>
-    <row r="35" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>102</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D35" s="89"/>
-      <c r="E35" s="92"/>
+        <v>53</v>
+      </c>
+      <c r="D35" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="110" t="s">
+        <v>57</v>
+      </c>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
@@ -6700,16 +6756,16 @@
     </row>
     <row r="36" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="90"/>
-      <c r="E36" s="93"/>
+        <v>54</v>
+      </c>
+      <c r="D36" s="108"/>
+      <c r="E36" s="111"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -6801,54 +6857,159 @@
       <c r="CP36" s="14"/>
       <c r="CQ36" s="14"/>
     </row>
-    <row r="37" spans="1:95" ht="51" x14ac:dyDescent="0.2">
-      <c r="C37" s="19" t="s">
+    <row r="37" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="109"/>
+      <c r="E37" s="112"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="14"/>
+      <c r="P37" s="14"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="14"/>
+      <c r="U37" s="14"/>
+      <c r="V37" s="14"/>
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="14"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="14"/>
+      <c r="AF37" s="14"/>
+      <c r="AG37" s="14"/>
+      <c r="AH37" s="14"/>
+      <c r="AI37" s="14"/>
+      <c r="AJ37" s="14"/>
+      <c r="AK37" s="14"/>
+      <c r="AL37" s="14"/>
+      <c r="AM37" s="14"/>
+      <c r="AN37" s="14"/>
+      <c r="AO37" s="14"/>
+      <c r="AP37" s="14"/>
+      <c r="AQ37" s="14"/>
+      <c r="AR37" s="14"/>
+      <c r="AS37" s="14"/>
+      <c r="AT37" s="14"/>
+      <c r="AU37" s="14"/>
+      <c r="AV37" s="14"/>
+      <c r="AW37" s="14"/>
+      <c r="AX37" s="14"/>
+      <c r="AY37" s="14"/>
+      <c r="AZ37" s="14"/>
+      <c r="BA37" s="14"/>
+      <c r="BB37" s="14"/>
+      <c r="BC37" s="14"/>
+      <c r="BD37" s="14"/>
+      <c r="BE37" s="14"/>
+      <c r="BF37" s="14"/>
+      <c r="BG37" s="14"/>
+      <c r="BH37" s="14"/>
+      <c r="BI37" s="14"/>
+      <c r="BJ37" s="14"/>
+      <c r="BK37" s="14"/>
+      <c r="BL37" s="14"/>
+      <c r="BM37" s="14"/>
+      <c r="BN37" s="14"/>
+      <c r="BO37" s="14"/>
+      <c r="BP37" s="14"/>
+      <c r="BQ37" s="14"/>
+      <c r="BR37" s="14"/>
+      <c r="BS37" s="14"/>
+      <c r="BT37" s="14"/>
+      <c r="BU37" s="14"/>
+      <c r="BV37" s="14"/>
+      <c r="BW37" s="14"/>
+      <c r="BX37" s="14"/>
+      <c r="BY37" s="14"/>
+      <c r="BZ37" s="14"/>
+      <c r="CA37" s="14"/>
+      <c r="CB37" s="14"/>
+      <c r="CC37" s="14"/>
+      <c r="CD37" s="14"/>
+      <c r="CE37" s="14"/>
+      <c r="CF37" s="14"/>
+      <c r="CG37" s="14"/>
+      <c r="CH37" s="14"/>
+      <c r="CI37" s="14"/>
+      <c r="CJ37" s="14"/>
+      <c r="CK37" s="14"/>
+      <c r="CL37" s="14"/>
+      <c r="CM37" s="14"/>
+      <c r="CN37" s="14"/>
+      <c r="CO37" s="14"/>
+      <c r="CP37" s="14"/>
+      <c r="CQ37" s="14"/>
+    </row>
+    <row r="38" spans="1:95" ht="51" x14ac:dyDescent="0.2">
+      <c r="C38" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D38" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E38" s="20" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="27">
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="D27:D33"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="E27:E33"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D14:D16"/>
     <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="D26:D32"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="E26:E32"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="D3:D6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" location="/dashboard" display="https://acleddata.com/dashboard/ - /dashboard" xr:uid="{F76E7675-2B2E-2D45-8C2B-2CB43E3D6E32}"/>
     <hyperlink ref="B14" r:id="rId2" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
     <hyperlink ref="B15" r:id="rId3" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
-    <hyperlink ref="B20" r:id="rId4" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
-    <hyperlink ref="B32" r:id="rId5" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
+    <hyperlink ref="B21" r:id="rId4" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
+    <hyperlink ref="B33" r:id="rId5" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
     <hyperlink ref="B3" r:id="rId6" display="https://fews.net/" xr:uid="{3D674EBD-4EF9-1342-883D-87D2B91B65D7}"/>
-    <hyperlink ref="B6" r:id="rId7" display="https://www.acaps.org/countries" xr:uid="{323C0C04-FA1B-0C4D-B8B5-EB4AF4D1488B}"/>
-    <hyperlink ref="B17" r:id="rId8" display="COVID Economic Stimus Index (as measured by Elgin et al)" xr:uid="{999A8B13-E27C-374A-82CC-F226FAFAE1F4}"/>
+    <hyperlink ref="B18" r:id="rId7" display="COVID Economic Stimus Index (as measured by Elgin et al)" xr:uid="{999A8B13-E27C-374A-82CC-F226FAFAE1F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6861,8 +7022,8 @@
   </sheetPr>
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6892,12 +7053,12 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
-        <v>190</v>
-      </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
+      <c r="A2" s="104" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
     </row>
     <row r="3" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="72" t="s">
@@ -6917,21 +7078,21 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="85" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="87"/>
+      <c r="A4" s="104" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="105"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="106"/>
     </row>
     <row r="5" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="80" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B5" s="78" t="s">
         <v>65</v>
@@ -6939,24 +7100,24 @@
       <c r="C5" s="78"/>
       <c r="D5" s="78"/>
       <c r="E5" s="78"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
-      <c r="L5" s="87"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="106"/>
     </row>
     <row r="6" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="99" t="s">
+      <c r="A6" s="118" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="105"/>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
-      <c r="H6" s="99"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="105"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
     </row>
     <row r="7" spans="1:12" ht="159" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="73" t="s">
@@ -6977,29 +7138,29 @@
       <c r="G7" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="85"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86"/>
-      <c r="K7" s="86"/>
-      <c r="L7" s="87"/>
+      <c r="H7" s="104"/>
+      <c r="I7" s="105"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="105"/>
+      <c r="L7" s="106"/>
     </row>
     <row r="8" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
       <c r="G8" s="46"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
     </row>
     <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B9" s="37" t="s">
         <v>67</v>
@@ -7016,44 +7177,44 @@
       <c r="G9" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="99"/>
-      <c r="I9" s="105"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="105"/>
-      <c r="L9" s="105"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="119"/>
+      <c r="L9" s="119"/>
     </row>
     <row r="10" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="99" t="s">
-        <v>193</v>
-      </c>
-      <c r="B10" s="105"/>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
+      <c r="A10" s="118" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="119"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="119"/>
       <c r="G10" s="47"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="96"/>
-      <c r="J10" s="96"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="97"/>
+      <c r="H10" s="114"/>
+      <c r="I10" s="115"/>
+      <c r="J10" s="115"/>
+      <c r="K10" s="115"/>
+      <c r="L10" s="116"/>
     </row>
     <row r="11" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="74" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
-      <c r="G11" s="123"/>
-      <c r="H11" s="124"/>
-      <c r="I11" s="124"/>
-      <c r="J11" s="124"/>
-      <c r="K11" s="124"/>
-      <c r="L11" s="124"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
     </row>
     <row r="12" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="74" t="s">
@@ -7066,32 +7227,32 @@
         <v>63</v>
       </c>
       <c r="D12" s="68" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E12" s="69" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F12" s="70"/>
       <c r="G12" s="46"/>
     </row>
     <row r="13" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="96"/>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
+      <c r="B13" s="115"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
       <c r="G13" s="45"/>
     </row>
     <row r="14" spans="1:12" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="63" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C14" s="65" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D14" s="65"/>
       <c r="E14" s="65"/>
@@ -7099,16 +7260,16 @@
     </row>
     <row r="15" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="63" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C15" s="66" t="s">
         <v>70</v>
       </c>
       <c r="D15" s="67" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E15" s="35"/>
       <c r="G15" s="45" t="s">
@@ -7116,17 +7277,17 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="99" t="s">
-        <v>192</v>
-      </c>
-      <c r="B16" s="105"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
+      <c r="A16" s="118" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16" s="119"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="119"/>
+      <c r="E16" s="119"/>
     </row>
     <row r="17" spans="1:6" ht="248" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="75" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B17" s="41" t="s">
         <v>69</v>
@@ -7146,6 +7307,9 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A6:D6"/>
     <mergeCell ref="H9:L9"/>
     <mergeCell ref="H10:L10"/>
     <mergeCell ref="A16:E16"/>
@@ -7157,9 +7321,6 @@
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A6:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="WFP Proteus composite index: " xr:uid="{3B8342E4-A803-C342-923C-31BDAA92A373}"/>
@@ -7259,102 +7420,102 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="85"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="87"/>
+        <v>151</v>
+      </c>
+      <c r="E2" s="104"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="106"/>
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" s="85"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="87"/>
+        <v>154</v>
+      </c>
+      <c r="E3" s="104"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="106"/>
     </row>
     <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="E4" s="99"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
+        <v>155</v>
+      </c>
+      <c r="E4" s="118"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="119"/>
+      <c r="H4" s="119"/>
+      <c r="I4" s="119"/>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="E5" s="85"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="87"/>
+        <v>156</v>
+      </c>
+      <c r="E5" s="104"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="106"/>
     </row>
     <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="E6" s="99"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="105"/>
+        <v>157</v>
+      </c>
+      <c r="E6" s="118"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
     </row>
     <row r="7" spans="1:9" ht="53" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" s="99"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="105"/>
-      <c r="H7" s="105"/>
-      <c r="I7" s="105"/>
+        <v>152</v>
+      </c>
+      <c r="E7" s="118"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="E8" s="95"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="97"/>
+        <v>153</v>
+      </c>
+      <c r="E8" s="114"/>
+      <c r="F8" s="115"/>
+      <c r="G8" s="115"/>
+      <c r="H8" s="115"/>
+      <c r="I8" s="116"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="79" t="s">
@@ -7384,7 +7545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FAE3D5-1E62-BD47-A72D-971150914E15}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -7400,65 +7561,65 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B1" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="59" t="s">
-        <v>112</v>
-      </c>
       <c r="D1" s="59" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C2" s="60" t="s">
         <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E3" s="61"/>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
@@ -7467,175 +7628,175 @@
         <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C7" s="60" t="s">
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C10" s="57" t="s">
         <v>88</v>
       </c>
       <c r="D10" s="77" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C11" s="57" t="s">
         <v>87</v>
       </c>
       <c r="D11" s="77" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B14" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C14" s="72" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C15" s="72" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C16" s="72" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="127" t="s">
-        <v>121</v>
+      <c r="A17" s="90" t="s">
+        <v>118</v>
       </c>
       <c r="B17" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" s="125" t="s">
-        <v>182</v>
-      </c>
-      <c r="D17" s="126" t="s">
-        <v>203</v>
+        <v>188</v>
+      </c>
+      <c r="C17" s="88" t="s">
+        <v>179</v>
+      </c>
+      <c r="D17" s="89" t="s">
+        <v>200</v>
       </c>
       <c r="F17" t="s">
         <v>60</v>
@@ -7643,7 +7804,7 @@
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
@@ -7652,12 +7813,12 @@
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
@@ -7666,96 +7827,96 @@
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C20" s="84" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D20" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B21" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C21" s="84" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B22" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C22" s="84" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B23" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D23" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D25" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
@@ -7764,110 +7925,110 @@
         <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D27" t="s">
         <v>121</v>
-      </c>
-      <c r="B27" t="s">
-        <v>205</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D27" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B28" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D28" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B31" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B33" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
         <v>29</v>
@@ -7876,12 +8037,12 @@
         <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
         <v>29</v>
@@ -7890,12 +8051,12 @@
         <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
         <v>29</v>
@@ -7904,7 +8065,7 @@
         <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating indicator aggregation .xlsx
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E192DC6E-FED1-D146-AA48-689B05095186}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C93D952-E724-1E43-9D41-851277BCD3C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="211">
   <si>
     <t>Bi-weekly percentage change in COVID cases (per 1M)</t>
   </si>
@@ -683,21 +683,11 @@
 1 = 1</t>
   </si>
   <si>
-    <t>F_fpv_alt</t>
-  </si>
-  <si>
     <t>F_food_acaps</t>
-  </si>
-  <si>
-    <t>Metric to track if price of one or more basic food commodities is abnormally high in main markets (identified using FAO Indicator of Price Anomaly and GIEWS)</t>
   </si>
   <si>
     <t>High &gt;= 0.2
 Low &lt;=  0</t>
-  </si>
-  <si>
-    <t>10 = above IPA threshold
-0 = below IPA threshold</t>
   </si>
   <si>
     <t>H_GovernmentResponseIndexForDisplay</t>
@@ -1217,6 +1207,28 @@
   </si>
   <si>
     <t>SOCIOECONOMIC VULNERABILITY</t>
+  </si>
+  <si>
+    <t>M_macrofin_risk_norm</t>
+  </si>
+  <si>
+    <t>WBG Macrofin heatmap</t>
+  </si>
+  <si>
+    <t>10 &lt; 4 risks
+0 = 0 risks</t>
+  </si>
+  <si>
+    <t>F_fpv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metric to track if price of one or more basic food commodities is abnormally high in main markets </t>
+  </si>
+  <si>
+    <t>10 &gt; 30%
+7 &gt;= 5 &amp; &lt; 30
+5 &gt;= 2 &amp; &lt; 5
+1 &lt; 2</t>
   </si>
   <si>
     <r>
@@ -1275,18 +1287,18 @@
         <rFont val="Garamond"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> FS = F_fpv_alt</t>
+      <t xml:space="preserve"> FS = F_fpv</t>
     </r>
   </si>
   <si>
-    <t>M_macrofin_risk_norm</t>
-  </si>
-  <si>
-    <t>WBG Macrofin heatmap</t>
-  </si>
-  <si>
-    <t>10 &lt; 4 risks
-0 = 0 risks</t>
+    <t>Country Policy and Institutional Analysis rating</t>
+  </si>
+  <si>
+    <t>10 &lt; 2.9
+0 &gt; 5</t>
+  </si>
+  <si>
+    <t>D_CPIA.scores_norm</t>
   </si>
 </sst>
 </file>
@@ -1774,7 +1786,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2016,6 +2028,123 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2034,118 +2163,13 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2301,13 +2325,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2136448</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>261122</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2847648</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>488298</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2372,13 +2396,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1994019</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>652803</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2768719</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>879979</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2443,13 +2467,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2077103</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1044486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>477852</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1271661</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2514,13 +2538,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2053365</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1483645</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2599465</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1710821</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2585,13 +2609,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2100841</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1863457</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2786641</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>2103333</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2656,13 +2680,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2100840</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>2267010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2735840</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>2506886</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2727,13 +2751,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>2480654</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>2682430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>17803</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>2922305</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3239,10 +3263,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:CQ38"/>
+  <dimension ref="A1:CQ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A8" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3274,13 +3298,13 @@
       </c>
     </row>
     <row r="2" spans="1:95" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="104" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="106"/>
+      <c r="A2" s="117" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="119"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -3382,11 +3406,11 @@
       <c r="C3" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="97" t="s">
-        <v>204</v>
-      </c>
-      <c r="E3" s="125" t="s">
-        <v>105</v>
+      <c r="D3" s="123" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" s="120" t="s">
+        <v>102</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -3487,10 +3511,10 @@
         <v>31</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="97"/>
-      <c r="E4" s="126"/>
+        <v>88</v>
+      </c>
+      <c r="D4" s="123"/>
+      <c r="E4" s="121"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -3583,17 +3607,17 @@
       <c r="CQ4" s="14"/>
     </row>
     <row r="5" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="130" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="131" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="133" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="126"/>
+      <c r="A5" s="124" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="126" t="s">
+        <v>205</v>
+      </c>
+      <c r="C5" s="128" t="s">
+        <v>206</v>
+      </c>
+      <c r="D5" s="123"/>
+      <c r="E5" s="121"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -3686,11 +3710,11 @@
       <c r="CQ5" s="14"/>
     </row>
     <row r="6" spans="1:95" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="129"/>
-      <c r="B6" s="132"/>
-      <c r="C6" s="134"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="127"/>
+      <c r="A6" s="125"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="129"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="122"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -3782,13 +3806,13 @@
       <c r="CP6" s="14"/>
     </row>
     <row r="7" spans="1:95" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="104" t="s">
-        <v>188</v>
-      </c>
-      <c r="B7" s="105"/>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="106"/>
+      <c r="A7" s="117" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="118"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="119"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -3881,18 +3905,18 @@
     </row>
     <row r="8" spans="1:95" s="2" customFormat="1" ht="89" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="72" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="D8" s="91" t="s">
-        <v>185</v>
-      </c>
-      <c r="E8" s="99" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" s="130" t="s">
+        <v>182</v>
+      </c>
+      <c r="E8" s="112" t="s">
         <v>55</v>
       </c>
       <c r="F8" s="14"/>
@@ -3987,16 +4011,16 @@
     </row>
     <row r="9" spans="1:95" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="72" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="D9" s="98"/>
-      <c r="E9" s="100"/>
+        <v>178</v>
+      </c>
+      <c r="D9" s="136"/>
+      <c r="E9" s="113"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -4089,16 +4113,16 @@
     </row>
     <row r="10" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="72" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="D10" s="98"/>
-      <c r="E10" s="100"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="113"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -4190,17 +4214,17 @@
       <c r="CP10" s="14"/>
     </row>
     <row r="11" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="95" t="s">
-        <v>179</v>
-      </c>
-      <c r="B11" s="93" t="s">
-        <v>184</v>
-      </c>
-      <c r="C11" s="91" t="s">
+      <c r="A11" s="134" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="132" t="s">
         <v>181</v>
       </c>
-      <c r="D11" s="98"/>
-      <c r="E11" s="100"/>
+      <c r="C11" s="130" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" s="136"/>
+      <c r="E11" s="113"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -4292,11 +4316,11 @@
       <c r="CP11" s="14"/>
     </row>
     <row r="12" spans="1:95" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="96"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="92"/>
-      <c r="E12" s="101"/>
+      <c r="A12" s="135"/>
+      <c r="B12" s="133"/>
+      <c r="C12" s="131"/>
+      <c r="D12" s="131"/>
+      <c r="E12" s="114"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -4388,13 +4412,13 @@
       <c r="CP12" s="14"/>
     </row>
     <row r="13" spans="1:95" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="118" t="s">
+      <c r="A13" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="119"/>
-      <c r="C13" s="119"/>
-      <c r="D13" s="119"/>
-      <c r="E13" s="119"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="94"/>
+      <c r="E13" s="94"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -4495,10 +4519,10 @@
       <c r="C14" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="97" t="s">
+      <c r="D14" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="128" t="s">
+      <c r="E14" s="100" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="14"/>
@@ -4601,8 +4625,8 @@
       <c r="C15" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="97"/>
-      <c r="E15" s="128"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="100"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
@@ -4695,16 +4719,16 @@
     </row>
     <row r="16" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C16" s="85" t="s">
-        <v>207</v>
-      </c>
-      <c r="D16" s="97"/>
-      <c r="E16" s="128"/>
+        <v>203</v>
+      </c>
+      <c r="D16" s="123"/>
+      <c r="E16" s="100"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -4796,13 +4820,13 @@
       <c r="CP16" s="14"/>
     </row>
     <row r="17" spans="1:95" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="104" t="s">
+      <c r="A17" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="105"/>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
-      <c r="E17" s="106"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="119"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
@@ -4896,18 +4920,18 @@
     </row>
     <row r="18" spans="1:95" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C18" s="53" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="102" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" s="102" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="115" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="115" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="14"/>
@@ -5003,16 +5027,16 @@
     </row>
     <row r="19" spans="1:95" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="103"/>
-      <c r="E19" s="102"/>
+        <v>95</v>
+      </c>
+      <c r="D19" s="116"/>
+      <c r="E19" s="115"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -5106,16 +5130,16 @@
     </row>
     <row r="20" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" s="103"/>
-      <c r="E20" s="102"/>
+        <v>93</v>
+      </c>
+      <c r="D20" s="116"/>
+      <c r="E20" s="115"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -5207,18 +5231,9 @@
       <c r="CP20" s="14"/>
       <c r="CQ20" s="14"/>
     </row>
-    <row r="21" spans="1:95" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A21" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="103"/>
-      <c r="E21" s="102"/>
+    <row r="21" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="116"/>
+      <c r="E21" s="115"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -5310,14 +5325,18 @@
       <c r="CP21" s="14"/>
       <c r="CQ21" s="14"/>
     </row>
-    <row r="22" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="118" t="s">
-        <v>189</v>
-      </c>
-      <c r="B22" s="119"/>
-      <c r="C22" s="119"/>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
+    <row r="22" spans="1:95" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="116"/>
+      <c r="E22" s="115"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -5409,22 +5428,14 @@
       <c r="CP22" s="14"/>
       <c r="CQ22" s="14"/>
     </row>
-    <row r="23" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A23" s="81" t="s">
-        <v>165</v>
-      </c>
-      <c r="B23" s="82" t="s">
-        <v>168</v>
-      </c>
-      <c r="C23" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="D23" s="120" t="s">
-        <v>173</v>
-      </c>
-      <c r="E23" s="120" t="s">
-        <v>174</v>
-      </c>
+    <row r="23" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="93" t="s">
+        <v>186</v>
+      </c>
+      <c r="B23" s="94"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -5516,18 +5527,22 @@
       <c r="CP23" s="14"/>
       <c r="CQ23" s="14"/>
     </row>
-    <row r="24" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="81" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B24" s="82" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="83" t="s">
         <v>169</v>
       </c>
-      <c r="C24" s="83" t="s">
-        <v>172</v>
-      </c>
-      <c r="D24" s="121"/>
-      <c r="E24" s="123"/>
+      <c r="D24" s="95" t="s">
+        <v>170</v>
+      </c>
+      <c r="E24" s="95" t="s">
+        <v>171</v>
+      </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -5619,18 +5634,18 @@
       <c r="CP24" s="14"/>
       <c r="CQ24" s="14"/>
     </row>
-    <row r="25" spans="1:95" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="81" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B25" s="82" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C25" s="83" t="s">
-        <v>171</v>
-      </c>
-      <c r="D25" s="122"/>
-      <c r="E25" s="124"/>
+        <v>169</v>
+      </c>
+      <c r="D25" s="96"/>
+      <c r="E25" s="98"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
@@ -5722,14 +5737,18 @@
       <c r="CP25" s="14"/>
       <c r="CQ25" s="14"/>
     </row>
-    <row r="26" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="118" t="s">
-        <v>190</v>
-      </c>
-      <c r="B26" s="119"/>
-      <c r="C26" s="119"/>
-      <c r="D26" s="119"/>
-      <c r="E26" s="119"/>
+    <row r="26" spans="1:95" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A26" s="81" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" s="82" t="s">
+        <v>167</v>
+      </c>
+      <c r="C26" s="83" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" s="97"/>
+      <c r="E26" s="99"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -5821,22 +5840,14 @@
       <c r="CP26" s="14"/>
       <c r="CQ26" s="14"/>
     </row>
-    <row r="27" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="B27" s="55" t="s">
-        <v>163</v>
-      </c>
-      <c r="C27" s="49" t="s">
-        <v>164</v>
-      </c>
-      <c r="D27" s="113" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" s="117" t="s">
-        <v>13</v>
-      </c>
+    <row r="27" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="93" t="s">
+        <v>187</v>
+      </c>
+      <c r="B27" s="94"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="94"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
@@ -5928,18 +5939,22 @@
       <c r="CP27" s="14"/>
       <c r="CQ27" s="14"/>
     </row>
-    <row r="28" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>0</v>
+        <v>159</v>
+      </c>
+      <c r="B28" s="55" t="s">
+        <v>160</v>
       </c>
       <c r="C28" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="113"/>
-      <c r="E28" s="117"/>
+        <v>161</v>
+      </c>
+      <c r="D28" s="107" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="111" t="s">
+        <v>13</v>
+      </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
@@ -6033,20 +6048,18 @@
     </row>
     <row r="29" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="113"/>
-      <c r="E29" s="117"/>
+      <c r="D29" s="107"/>
+      <c r="E29" s="111"/>
       <c r="F29" s="14"/>
-      <c r="G29" s="14" t="s">
-        <v>58</v>
-      </c>
+      <c r="G29" s="14"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
@@ -6138,18 +6151,20 @@
     </row>
     <row r="30" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="113"/>
-      <c r="E30" s="117"/>
+        <v>50</v>
+      </c>
+      <c r="D30" s="107"/>
+      <c r="E30" s="111"/>
       <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+      <c r="G30" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
@@ -6241,16 +6256,16 @@
     </row>
     <row r="31" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="113"/>
-      <c r="E31" s="117"/>
+        <v>51</v>
+      </c>
+      <c r="D31" s="107"/>
+      <c r="E31" s="111"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
@@ -6344,16 +6359,16 @@
     </row>
     <row r="32" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>149</v>
+        <v>3</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="113"/>
-      <c r="E32" s="117"/>
+        <v>52</v>
+      </c>
+      <c r="D32" s="107"/>
+      <c r="E32" s="111"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -6447,16 +6462,16 @@
     </row>
     <row r="33" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="D33" s="113"/>
-      <c r="E33" s="117"/>
+        <v>90</v>
+      </c>
+      <c r="D33" s="107"/>
+      <c r="E33" s="111"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
@@ -6548,14 +6563,18 @@
       <c r="CP33" s="14"/>
       <c r="CQ33" s="14"/>
     </row>
-    <row r="34" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="114" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="115"/>
-      <c r="C34" s="115"/>
-      <c r="D34" s="115"/>
-      <c r="E34" s="116"/>
+    <row r="34" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C34" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="107"/>
+      <c r="E34" s="111"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
@@ -6647,22 +6666,14 @@
       <c r="CP34" s="14"/>
       <c r="CQ34" s="14"/>
     </row>
-    <row r="35" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="107" t="s">
-        <v>56</v>
-      </c>
-      <c r="E35" s="110" t="s">
-        <v>57</v>
-      </c>
+    <row r="35" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="108" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="109"/>
+      <c r="C35" s="109"/>
+      <c r="D35" s="109"/>
+      <c r="E35" s="110"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
@@ -6754,18 +6765,22 @@
       <c r="CP35" s="14"/>
       <c r="CQ35" s="14"/>
     </row>
-    <row r="36" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>99</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="108"/>
-      <c r="E36" s="111"/>
+        <v>53</v>
+      </c>
+      <c r="D36" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="104" t="s">
+        <v>57</v>
+      </c>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -6859,16 +6874,16 @@
     </row>
     <row r="37" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="109"/>
-      <c r="E37" s="112"/>
+        <v>54</v>
+      </c>
+      <c r="D37" s="102"/>
+      <c r="E37" s="105"/>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
@@ -6960,33 +6975,125 @@
       <c r="CP37" s="14"/>
       <c r="CQ37" s="14"/>
     </row>
-    <row r="38" spans="1:95" ht="51" x14ac:dyDescent="0.2">
-      <c r="C38" s="19" t="s">
+    <row r="38" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="103"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="14"/>
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="14"/>
+      <c r="W38" s="14"/>
+      <c r="X38" s="14"/>
+      <c r="Y38" s="14"/>
+      <c r="Z38" s="14"/>
+      <c r="AA38" s="14"/>
+      <c r="AB38" s="14"/>
+      <c r="AC38" s="14"/>
+      <c r="AD38" s="14"/>
+      <c r="AE38" s="14"/>
+      <c r="AF38" s="14"/>
+      <c r="AG38" s="14"/>
+      <c r="AH38" s="14"/>
+      <c r="AI38" s="14"/>
+      <c r="AJ38" s="14"/>
+      <c r="AK38" s="14"/>
+      <c r="AL38" s="14"/>
+      <c r="AM38" s="14"/>
+      <c r="AN38" s="14"/>
+      <c r="AO38" s="14"/>
+      <c r="AP38" s="14"/>
+      <c r="AQ38" s="14"/>
+      <c r="AR38" s="14"/>
+      <c r="AS38" s="14"/>
+      <c r="AT38" s="14"/>
+      <c r="AU38" s="14"/>
+      <c r="AV38" s="14"/>
+      <c r="AW38" s="14"/>
+      <c r="AX38" s="14"/>
+      <c r="AY38" s="14"/>
+      <c r="AZ38" s="14"/>
+      <c r="BA38" s="14"/>
+      <c r="BB38" s="14"/>
+      <c r="BC38" s="14"/>
+      <c r="BD38" s="14"/>
+      <c r="BE38" s="14"/>
+      <c r="BF38" s="14"/>
+      <c r="BG38" s="14"/>
+      <c r="BH38" s="14"/>
+      <c r="BI38" s="14"/>
+      <c r="BJ38" s="14"/>
+      <c r="BK38" s="14"/>
+      <c r="BL38" s="14"/>
+      <c r="BM38" s="14"/>
+      <c r="BN38" s="14"/>
+      <c r="BO38" s="14"/>
+      <c r="BP38" s="14"/>
+      <c r="BQ38" s="14"/>
+      <c r="BR38" s="14"/>
+      <c r="BS38" s="14"/>
+      <c r="BT38" s="14"/>
+      <c r="BU38" s="14"/>
+      <c r="BV38" s="14"/>
+      <c r="BW38" s="14"/>
+      <c r="BX38" s="14"/>
+      <c r="BY38" s="14"/>
+      <c r="BZ38" s="14"/>
+      <c r="CA38" s="14"/>
+      <c r="CB38" s="14"/>
+      <c r="CC38" s="14"/>
+      <c r="CD38" s="14"/>
+      <c r="CE38" s="14"/>
+      <c r="CF38" s="14"/>
+      <c r="CG38" s="14"/>
+      <c r="CH38" s="14"/>
+      <c r="CI38" s="14"/>
+      <c r="CJ38" s="14"/>
+      <c r="CK38" s="14"/>
+      <c r="CL38" s="14"/>
+      <c r="CM38" s="14"/>
+      <c r="CN38" s="14"/>
+      <c r="CO38" s="14"/>
+      <c r="CP38" s="14"/>
+      <c r="CQ38" s="14"/>
+    </row>
+    <row r="39" spans="1:95" ht="51" x14ac:dyDescent="0.2">
+      <c r="C39" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D39" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E39" s="20" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="D27:D33"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="E27:E33"/>
     <mergeCell ref="E8:E12"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="E18:E22"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A17:E17"/>
@@ -7000,14 +7107,25 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="D8:D12"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="D28:D34"/>
+    <mergeCell ref="A35:E35"/>
+    <mergeCell ref="E28:E34"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="E14:E16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" location="/dashboard" display="https://acleddata.com/dashboard/ - /dashboard" xr:uid="{F76E7675-2B2E-2D45-8C2B-2CB43E3D6E32}"/>
     <hyperlink ref="B14" r:id="rId2" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
     <hyperlink ref="B15" r:id="rId3" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
-    <hyperlink ref="B21" r:id="rId4" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
-    <hyperlink ref="B33" r:id="rId5" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
+    <hyperlink ref="B22" r:id="rId4" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
+    <hyperlink ref="B34" r:id="rId5" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
     <hyperlink ref="B3" r:id="rId6" display="https://fews.net/" xr:uid="{3D674EBD-4EF9-1342-883D-87D2B91B65D7}"/>
     <hyperlink ref="B18" r:id="rId7" display="COVID Economic Stimus Index (as measured by Elgin et al)" xr:uid="{999A8B13-E27C-374A-82CC-F226FAFAE1F4}"/>
   </hyperlinks>
@@ -7020,10 +7138,10 @@
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7053,12 +7171,12 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="104" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="105"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
+      <c r="A2" s="117" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
     </row>
     <row r="3" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="72" t="s">
@@ -7078,21 +7196,21 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="104" t="s">
-        <v>188</v>
-      </c>
-      <c r="B4" s="105"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="106"/>
+      <c r="A4" s="117" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="118"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="119"/>
     </row>
     <row r="5" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="80" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B5" s="78" t="s">
         <v>65</v>
@@ -7100,24 +7218,24 @@
       <c r="C5" s="78"/>
       <c r="D5" s="78"/>
       <c r="E5" s="78"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="106"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="118"/>
+      <c r="K5" s="118"/>
+      <c r="L5" s="119"/>
     </row>
     <row r="6" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="119"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="119"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="119"/>
-      <c r="J6" s="119"/>
-      <c r="K6" s="119"/>
-      <c r="L6" s="119"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="94"/>
     </row>
     <row r="7" spans="1:12" ht="159" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="73" t="s">
@@ -7138,196 +7256,215 @@
       <c r="G7" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="104"/>
-      <c r="I7" s="105"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="105"/>
-      <c r="L7" s="106"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="119"/>
     </row>
     <row r="8" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="105"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
       <c r="G8" s="46"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-    </row>
-    <row r="9" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="H8" s="93"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+    </row>
+    <row r="9" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="B9" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="137" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" s="138" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
+    </row>
+    <row r="10" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C10" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D10" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E10" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G10" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="118"/>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
-      <c r="K9" s="119"/>
-      <c r="L9" s="119"/>
-    </row>
-    <row r="10" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="118" t="s">
+      <c r="H10" s="93"/>
+      <c r="I10" s="94"/>
+      <c r="J10" s="94"/>
+      <c r="K10" s="94"/>
+      <c r="L10" s="94"/>
+    </row>
+    <row r="11" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="93" t="s">
+        <v>187</v>
+      </c>
+      <c r="B11" s="94"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="108"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="109"/>
+      <c r="K11" s="109"/>
+      <c r="L11" s="110"/>
+    </row>
+    <row r="12" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C12" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="B10" s="119"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="119"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="114"/>
-      <c r="I10" s="115"/>
-      <c r="J10" s="115"/>
-      <c r="K10" s="115"/>
-      <c r="L10" s="116"/>
-    </row>
-    <row r="11" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="74" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+    </row>
+    <row r="13" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="69" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="70"/>
+      <c r="G13" s="46"/>
+    </row>
+    <row r="14" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="108" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="109"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
+      <c r="G14" s="45"/>
+    </row>
+    <row r="15" spans="1:12" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="63" t="s">
         <v>191</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B15" s="65" t="s">
         <v>192</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C15" s="65" t="s">
         <v>193</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="87"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="87"/>
-    </row>
-    <row r="12" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="68" t="s">
-        <v>139</v>
-      </c>
-      <c r="E12" s="69" t="s">
-        <v>140</v>
-      </c>
-      <c r="F12" s="70"/>
-      <c r="G12" s="46"/>
-    </row>
-    <row r="13" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="114" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="115"/>
-      <c r="C13" s="115"/>
-      <c r="D13" s="115"/>
-      <c r="G13" s="45"/>
-    </row>
-    <row r="14" spans="1:12" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="63" t="s">
-        <v>194</v>
-      </c>
-      <c r="B14" s="65" t="s">
-        <v>195</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>196</v>
-      </c>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="G14" s="45"/>
-    </row>
-    <row r="15" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="63" t="s">
-        <v>136</v>
-      </c>
-      <c r="B15" s="65" t="s">
-        <v>137</v>
-      </c>
-      <c r="C15" s="66" t="s">
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="G15" s="45"/>
+    </row>
+    <row r="16" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="67" t="s">
-        <v>138</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="G15" s="45" t="s">
+      <c r="D16" s="67" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="35"/>
+      <c r="G16" s="45" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="118" t="s">
-        <v>189</v>
-      </c>
-      <c r="B16" s="119"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="119"/>
-      <c r="E16" s="119"/>
-    </row>
-    <row r="17" spans="1:6" ht="248" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="75" t="s">
-        <v>158</v>
-      </c>
-      <c r="B17" s="41" t="s">
+    <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="93" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" s="94"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
+    </row>
+    <row r="18" spans="1:6" ht="248" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="75" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C18" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D18" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E18" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="F18" s="44" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A14:D14"/>
     <mergeCell ref="H4:L4"/>
     <mergeCell ref="H5:L5"/>
     <mergeCell ref="H6:L6"/>
     <mergeCell ref="H7:L7"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="H11:L11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="WFP Proteus composite index: " xr:uid="{3B8342E4-A803-C342-923C-31BDAA92A373}"/>
-    <hyperlink ref="B12" r:id="rId2" xr:uid="{95E245AA-F0BF-3C40-B212-C5EC3EDEDF2E}"/>
-    <hyperlink ref="D15" r:id="rId3" location=":~:text=INFORM%20Index%20for%20Risk%20Management%3A%20Concept%20and%20Methodology%2C%20Version%202017,-%C2%A9EU&amp;text=INFORM%20is%20a%20composite%20indicator,crisis%20and%20disaster%20management%20framework." xr:uid="{AF872891-F870-AA4C-B416-4F92600B17AE}"/>
-    <hyperlink ref="D12" r:id="rId4" xr:uid="{26B58F35-C97D-3F48-B110-F642D3427351}"/>
-    <hyperlink ref="E12" r:id="rId5" xr:uid="{2B1483A5-6E05-4E4E-A8CB-95D622233E3B}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{95E245AA-F0BF-3C40-B212-C5EC3EDEDF2E}"/>
+    <hyperlink ref="D16" r:id="rId3" location=":~:text=INFORM%20Index%20for%20Risk%20Management%3A%20Concept%20and%20Methodology%2C%20Version%202017,-%C2%A9EU&amp;text=INFORM%20is%20a%20composite%20indicator,crisis%20and%20disaster%20management%20framework." xr:uid="{AF872891-F870-AA4C-B416-4F92600B17AE}"/>
+    <hyperlink ref="D13" r:id="rId4" xr:uid="{26B58F35-C97D-3F48-B110-F642D3427351}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{2B1483A5-6E05-4E4E-A8CB-95D622233E3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId6"/>
@@ -7420,102 +7557,102 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E2" s="104"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="106"/>
+        <v>148</v>
+      </c>
+      <c r="E2" s="117"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="119"/>
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="E3" s="104"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="106"/>
+        <v>151</v>
+      </c>
+      <c r="E3" s="117"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="119"/>
     </row>
     <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
+        <v>152</v>
+      </c>
+      <c r="E4" s="93"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" s="104"/>
-      <c r="F5" s="105"/>
-      <c r="G5" s="105"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="106"/>
+        <v>153</v>
+      </c>
+      <c r="E5" s="117"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="119"/>
     </row>
     <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="E6" s="118"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="119"/>
+        <v>154</v>
+      </c>
+      <c r="E6" s="93"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
     </row>
     <row r="7" spans="1:9" ht="53" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="E7" s="118"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
+        <v>149</v>
+      </c>
+      <c r="E7" s="93"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="E8" s="114"/>
-      <c r="F8" s="115"/>
-      <c r="G8" s="115"/>
-      <c r="H8" s="115"/>
-      <c r="I8" s="116"/>
+        <v>150</v>
+      </c>
+      <c r="E8" s="108"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="110"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="79" t="s">
@@ -7546,7 +7683,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7561,65 +7698,65 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B1" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="59" t="s">
-        <v>109</v>
-      </c>
       <c r="D1" s="59" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C2" s="60" t="s">
         <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E2" s="61"/>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E3" s="61"/>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
@@ -7628,175 +7765,175 @@
         <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C7" s="60" t="s">
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C10" s="57" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="77" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C11" s="57" t="s">
-        <v>87</v>
+        <v>204</v>
       </c>
       <c r="D11" s="77" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C14" s="72" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D14" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C15" s="72" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C16" s="72" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="90" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C17" s="88" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D17" s="89" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F17" t="s">
         <v>60</v>
@@ -7804,7 +7941,7 @@
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
@@ -7813,12 +7950,12 @@
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
@@ -7827,96 +7964,96 @@
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C20" s="84" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B21" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C21" s="84" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D21" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C22" s="84" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B23" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D24" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
@@ -7925,110 +8062,110 @@
         <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D27" t="s">
         <v>118</v>
-      </c>
-      <c r="B27" t="s">
-        <v>202</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="D27" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B28" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D29" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D31" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
         <v>29</v>
@@ -8037,12 +8174,12 @@
         <v>22</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
         <v>29</v>
@@ -8051,12 +8188,12 @@
         <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B36" t="s">
         <v>29</v>
@@ -8065,7 +8202,7 @@
         <v>26</v>
       </c>
       <c r="D36" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected a bug for covid growth
Corrected bug for COVID severity (inform_covid_warming_raw)

Added World Bank Phone Surveys (phone_index_data) for Socioeconomic Vulnerability

Added La Nina index for Natural Hazards
</commit_message>
<xml_diff>
--- a/Annotation and Data Architecture/Indicator aggregation.xlsx
+++ b/Annotation and Data Architecture/Indicator aggregation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ljmac/Google Drive/PhD/R code/Compound Risk/Compound Risk/covid/compoundriskdata/Annotation and Data Architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C93D952-E724-1E43-9D41-851277BCD3C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D4CE9E-B1F2-424E-B153-2BA48692E661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
+    <workbookView xWindow="-4640" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{B42EF1BE-965E-B741-ADF0-C68AD4A5C459}"/>
   </bookViews>
   <sheets>
     <sheet name="Emerging Risk" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Indicator Label" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="223">
   <si>
     <t>Bi-weekly percentage change in COVID cases (per 1M)</t>
   </si>
@@ -61,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">Given that any 0 values along a series in a geometric average will result in an overall score of 0, a 1 is added to any individual data source. </t>
-  </si>
-  <si>
-    <t>In the case of food security, FEWSNET is deemed to be a more robust source of information so is weighting is carried out hierarchically</t>
   </si>
   <si>
     <r>
@@ -678,11 +676,6 @@
     <t>H_Oxrollback_score_norm</t>
   </si>
   <si>
-    <t>10 &gt; 3
-7 = 7 
-1 = 1</t>
-  </si>
-  <si>
     <t>F_food_acaps</t>
   </si>
   <si>
@@ -757,48 +750,6 @@
     <t>COVID Economic Stimulus Index (as measured by Elgin et al)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t>IF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> FEWSNET country then FS_SQ = FS,
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> ELSE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Garamond"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> FS_SQ = GEOMETRICMEAN(EXISTING_RISK_FS, FS)
-Note: FS calculated as max values</t>
-    </r>
-  </si>
-  <si>
     <t>Risk Category</t>
   </si>
   <si>
@@ -984,12 +935,6 @@
   </si>
   <si>
     <t>S_income_support.Rating_norm</t>
-  </si>
-  <si>
-    <t>Change in GDP growth (INFORM COVID Warning tool)</t>
-  </si>
-  <si>
-    <t>Unemployment rate</t>
   </si>
   <si>
     <t>Whether income support is provided</t>
@@ -998,9 +943,6 @@
     <t>10 = Government replacing &gt; 50% of lost salary
 7 = Government replacing &lt; 50% of lost salary
 0 = No income support</t>
-  </si>
-  <si>
-    <t>INFORM threshold</t>
   </si>
   <si>
     <r>
@@ -1131,8 +1073,165 @@
     </r>
   </si>
   <si>
+    <t>FOOD SECURITY</t>
+  </si>
+  <si>
+    <t>CONFLICT AND FRAGILITY</t>
+  </si>
+  <si>
+    <t>SOCIO-ECONOMIC VULNERABILITY</t>
+  </si>
+  <si>
+    <t>COVID EXPOSURE AND RESPONSE CAPACITY</t>
+  </si>
+  <si>
+    <t>H_INFORM_rating.Value_norm</t>
+  </si>
+  <si>
+    <t>INFORM COVID vulnerability index (composite index)</t>
+  </si>
+  <si>
+    <t>10 &lt; 2
+0 &lt; 6</t>
+  </si>
+  <si>
+    <t>NH_multihazard_risk_norm</t>
+  </si>
+  <si>
+    <t>ThinkHazard! Database of natural hazard risks (World Bank)</t>
+  </si>
+  <si>
+    <t>10 &gt; 4 high risk hazards 
+0 = 0 high risk hazards</t>
+  </si>
+  <si>
+    <t>Ongoing crisis (ACAPS)</t>
+  </si>
+  <si>
+    <t>Likelihood of state-sponsored violence (ViEWS)</t>
+  </si>
+  <si>
+    <t>Likelihood of non-state violence (ViEWS)</t>
+  </si>
+  <si>
+    <t>Likelihood of one-sided violence (ViEWS)</t>
+  </si>
+  <si>
+    <t>Multi-hazard exposure (WB)</t>
+  </si>
+  <si>
+    <t>COVID RESPONSE AND RESPONSE CAPACITY</t>
+  </si>
+  <si>
+    <t>SOCIOECONOMIC VULNERABILITY</t>
+  </si>
+  <si>
+    <t>M_macrofin_risk_norm</t>
+  </si>
+  <si>
+    <t>WBG Macrofin heatmap</t>
+  </si>
+  <si>
+    <t>10 &lt; 4 risks
+0 = 0 risks</t>
+  </si>
+  <si>
+    <t>F_fpv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metric to track if price of one or more basic food commodities is abnormally high in main markets </t>
+  </si>
+  <si>
+    <t>Country Policy and Institutional Analysis rating</t>
+  </si>
+  <si>
+    <t>10 &lt; 2.9
+0 &gt; 5</t>
+  </si>
+  <si>
+    <t>D_CPIA.scores_norm</t>
+  </si>
+  <si>
+    <t>F_fao_wfp_warning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 = CRW treshold
+9 = Below CRW &amp; IPC5
+8 =  Below CRW &amp; IPC4
+7 =  Below CRW &amp; IPC3
+5 =  Below CRW &amp; IPC2
+3 = Below CRW &amp; IPC1
+0 = Below CRW &amp; no IPC
+</t>
+  </si>
+  <si>
+    <t>FAO / WFP early warning hotspots of acute food insecurity</t>
+  </si>
+  <si>
+    <t>10 = If FAO/WFP hotpot
+0 = Otherwise</t>
+  </si>
+  <si>
+    <t>10 if &gt; 30%
+7 if &gt;= 5 &amp; &lt; 30_
+5 if &gt;= 2 &amp; &lt; 5
+1 if &lt; 2</t>
+  </si>
+  <si>
+    <t>S_Household.risks</t>
+  </si>
+  <si>
+    <t>WBG Macrofin heatmap for household-level risk (index comprised of household debt-to-GDP ratio and existing unemployment rate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 = WBG High risk
+7 = WBG Medium risk
+0 = WBG Low risk
+</t>
+  </si>
+  <si>
+    <t>S_unemployment.RatS_change_unemping_norm</t>
+  </si>
+  <si>
+    <t>10 &gt; 5
+0 &lt; 0</t>
+  </si>
+  <si>
+    <t>Percentage difference between 2019 rate of unemployment and 2020 forecast (IMF)</t>
+  </si>
+  <si>
+    <t>S_pov_prop_19_20_norm</t>
+  </si>
+  <si>
+    <t>S_pov_abs_19_20_norm</t>
+  </si>
+  <si>
+    <t>Growth in the proportion of people below $1.90 poverty line between 2019 and 2020</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">10 = Severity &gt; 3 &amp; Conditions worsening </t>
+      <t xml:space="preserve">Absolute percentage change in the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>number of people below $1.90 poverty line between 2019 and 2020</t>
+    </r>
+  </si>
+  <si>
+    <t>10 &gt; 50
+0 = 0</t>
+  </si>
+  <si>
+    <t>10 &gt; 0.05</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10 = (Severity &gt; 3 &amp; Conditions worsening) </t>
     </r>
     <r>
       <rPr>
@@ -1156,79 +1255,7 @@
     </r>
   </si>
   <si>
-    <t>FOOD SECURITY</t>
-  </si>
-  <si>
-    <t>CONFLICT AND FRAGILITY</t>
-  </si>
-  <si>
-    <t>SOCIO-ECONOMIC VULNERABILITY</t>
-  </si>
-  <si>
-    <t>COVID EXPOSURE AND RESPONSE CAPACITY</t>
-  </si>
-  <si>
-    <t>H_INFORM_rating.Value_norm</t>
-  </si>
-  <si>
-    <t>INFORM COVID vulnerability index (composite index)</t>
-  </si>
-  <si>
-    <t>10 &lt; 2
-0 &lt; 6</t>
-  </si>
-  <si>
-    <t>NH_multihazard_risk_norm</t>
-  </si>
-  <si>
-    <t>ThinkHazard! Database of natural hazard risks (World Bank)</t>
-  </si>
-  <si>
-    <t>10 &gt; 4 high risk hazards 
-0 = 0 high risk hazards</t>
-  </si>
-  <si>
-    <t>Ongoing crisis (ACAPS)</t>
-  </si>
-  <si>
-    <t>Likelihood of state-sponsored violence (ViEWS)</t>
-  </si>
-  <si>
-    <t>Likelihood of non-state violence (ViEWS)</t>
-  </si>
-  <si>
-    <t>Likelihood of one-sided violence (ViEWS)</t>
-  </si>
-  <si>
-    <t>Multi-hazard exposure (WB)</t>
-  </si>
-  <si>
-    <t>COVID RESPONSE AND RESPONSE CAPACITY</t>
-  </si>
-  <si>
-    <t>SOCIOECONOMIC VULNERABILITY</t>
-  </si>
-  <si>
-    <t>M_macrofin_risk_norm</t>
-  </si>
-  <si>
-    <t>WBG Macrofin heatmap</t>
-  </si>
-  <si>
-    <t>10 &lt; 4 risks
-0 = 0 risks</t>
-  </si>
-  <si>
-    <t>F_fpv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metric to track if price of one or more basic food commodities is abnormally high in main markets </t>
-  </si>
-  <si>
-    <t>10 &gt; 30%
-7 &gt;= 5 &amp; &lt; 30
-5 &gt;= 2 &amp; &lt; 5
-1 &lt; 2</t>
+    <t>In the case of food security, FEWSNET is deemed to be a more robust source of information so weighting is carried out hierarchically</t>
   </si>
   <si>
     <r>
@@ -1248,7 +1275,7 @@
         <rFont val="Garamond"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> FEWSNET country then FS = </t>
+      <t xml:space="preserve"> FEWSNET country OR F_fao_wfp_warning valid then FS = </t>
     </r>
     <r>
       <rPr>
@@ -1267,7 +1294,7 @@
         <rFont val="Garamond"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">(F_FEWSNET_SCORE,  F_AFTEMIS)
+      <t xml:space="preserve">(F_FEWSNET_SCORE,  F_AFTEMIS, F_fao_wfp_warning),
 </t>
     </r>
     <r>
@@ -1291,21 +1318,53 @@
     </r>
   </si>
   <si>
-    <t>Country Policy and Institutional Analysis rating</t>
-  </si>
-  <si>
-    <t>10 &lt; 2.9
-0 &gt; 5</t>
-  </si>
-  <si>
-    <t>D_CPIA.scores_norm</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t>IF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> FEWSNET or F_fao_wfp_warning valid then FS_SQ = FS,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ELSE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Garamond"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> FS_SQ = GEOMETRICMEAN(EXISTING_RISK_FS, FS)
+Note: FS calculated as max values</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1415,6 +1474,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="25">
@@ -1563,7 +1628,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1772,6 +1837,35 @@
       <left style="medium">
         <color rgb="FFFFFFFF"/>
       </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color theme="0"/>
       </right>
@@ -1786,7 +1880,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1849,12 +1943,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2034,6 +2122,120 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2058,118 +2260,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3263,17 +3369,17 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:CQ39"/>
+  <dimension ref="A1:CQ41"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="88" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:C21"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30" style="8" customWidth="1"/>
     <col min="2" max="2" width="42.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22" style="24" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" style="24" customWidth="1"/>
     <col min="4" max="4" width="52.6640625" style="7" customWidth="1"/>
     <col min="5" max="5" width="47.33203125" style="7" customWidth="1"/>
     <col min="6" max="95" width="10.83203125" style="14"/>
@@ -3282,29 +3388,29 @@
   <sheetData>
     <row r="1" spans="1:95" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="2" spans="1:95" s="1" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="117" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="119"/>
+      <c r="A2" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="107"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -3396,21 +3502,21 @@
       <c r="CP2" s="14"/>
       <c r="CQ2" s="14"/>
     </row>
-    <row r="3" spans="1:95" s="1" customFormat="1" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="123" t="s">
-        <v>207</v>
-      </c>
-      <c r="E3" s="120" t="s">
-        <v>102</v>
+    <row r="3" spans="1:95" s="1" customFormat="1" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3" s="110" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="108" t="s">
+        <v>222</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
@@ -3504,17 +3610,17 @@
       <c r="CQ3" s="14"/>
     </row>
     <row r="4" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="58" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="123"/>
-      <c r="E4" s="121"/>
+      <c r="A4" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="110"/>
+      <c r="E4" s="109"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -3606,18 +3712,18 @@
       <c r="CP4" s="14"/>
       <c r="CQ4" s="14"/>
     </row>
-    <row r="5" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="124" t="s">
+    <row r="5" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="97" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="98" t="s">
         <v>204</v>
       </c>
-      <c r="B5" s="126" t="s">
+      <c r="C5" s="99" t="s">
         <v>205</v>
       </c>
-      <c r="C5" s="128" t="s">
-        <v>206</v>
-      </c>
-      <c r="D5" s="123"/>
-      <c r="E5" s="121"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="109"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -3709,12 +3815,18 @@
       <c r="CP5" s="14"/>
       <c r="CQ5" s="14"/>
     </row>
-    <row r="6" spans="1:95" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="125"/>
-      <c r="B6" s="127"/>
-      <c r="C6" s="129"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="122"/>
+    <row r="6" spans="1:95" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="91" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="92" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" s="93" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="110"/>
+      <c r="E6" s="109"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -3804,15 +3916,16 @@
       <c r="CN6" s="14"/>
       <c r="CO6" s="14"/>
       <c r="CP6" s="14"/>
+      <c r="CQ6" s="14"/>
     </row>
     <row r="7" spans="1:95" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="117" t="s">
-        <v>185</v>
-      </c>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="119"/>
+      <c r="A7" s="105" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="106"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="106"/>
+      <c r="E7" s="107"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -3904,20 +4017,20 @@
       <c r="CP7" s="14"/>
     </row>
     <row r="8" spans="1:95" s="2" customFormat="1" ht="89" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="72" t="s">
-        <v>173</v>
+      <c r="A8" s="70" t="s">
+        <v>167</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>183</v>
-      </c>
-      <c r="D8" s="130" t="s">
-        <v>182</v>
-      </c>
-      <c r="E8" s="112" t="s">
-        <v>55</v>
+        <v>171</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" s="111" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="100" t="s">
+        <v>54</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -4010,17 +4123,17 @@
       <c r="CP8" s="14"/>
     </row>
     <row r="9" spans="1:95" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="72" t="s">
-        <v>174</v>
+      <c r="A9" s="70" t="s">
+        <v>168</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="D9" s="136"/>
-      <c r="E9" s="113"/>
+        <v>173</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" s="117"/>
+      <c r="E9" s="101"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -4112,17 +4225,17 @@
       <c r="CP9" s="14"/>
     </row>
     <row r="10" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="72" t="s">
-        <v>175</v>
+      <c r="A10" s="70" t="s">
+        <v>169</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="D10" s="136"/>
-      <c r="E10" s="113"/>
+        <v>174</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="D10" s="117"/>
+      <c r="E10" s="101"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -4214,17 +4327,17 @@
       <c r="CP10" s="14"/>
     </row>
     <row r="11" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="134" t="s">
-        <v>176</v>
-      </c>
-      <c r="B11" s="132" t="s">
-        <v>181</v>
-      </c>
-      <c r="C11" s="130" t="s">
-        <v>178</v>
-      </c>
-      <c r="D11" s="136"/>
-      <c r="E11" s="113"/>
+      <c r="A11" s="115" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="113" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="111" t="s">
+        <v>172</v>
+      </c>
+      <c r="D11" s="117"/>
+      <c r="E11" s="101"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -4316,11 +4429,11 @@
       <c r="CP11" s="14"/>
     </row>
     <row r="12" spans="1:95" s="3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="135"/>
-      <c r="B12" s="133"/>
-      <c r="C12" s="131"/>
-      <c r="D12" s="131"/>
-      <c r="E12" s="114"/>
+      <c r="A12" s="116"/>
+      <c r="B12" s="114"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="102"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -4412,13 +4525,13 @@
       <c r="CP12" s="14"/>
     </row>
     <row r="13" spans="1:95" s="3" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="93" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
+      <c r="A13" s="129" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="130"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="130"/>
+      <c r="E13" s="130"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -4511,19 +4624,19 @@
     </row>
     <row r="14" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="123" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="110" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="136" t="s">
         <v>9</v>
-      </c>
-      <c r="E14" s="100" t="s">
-        <v>10</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -4617,16 +4730,16 @@
     </row>
     <row r="15" spans="1:95" s="3" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="123"/>
-      <c r="E15" s="100"/>
+        <v>32</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="110"/>
+      <c r="E15" s="136"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
@@ -4719,16 +4832,16 @@
     </row>
     <row r="16" spans="1:95" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="C16" s="85" t="s">
-        <v>203</v>
-      </c>
-      <c r="D16" s="123"/>
-      <c r="E16" s="100"/>
+        <v>195</v>
+      </c>
+      <c r="C16" s="83" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="110"/>
+      <c r="E16" s="136"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -4820,13 +4933,13 @@
       <c r="CP16" s="14"/>
     </row>
     <row r="17" spans="1:95" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="117" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="118"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="119"/>
+      <c r="A17" s="105" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="106"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="107"/>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
@@ -4919,23 +5032,23 @@
       <c r="CQ17" s="14"/>
     </row>
     <row r="18" spans="1:95" s="4" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="103" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="53" t="s">
-        <v>97</v>
-      </c>
-      <c r="D18" s="115" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" s="115" t="s">
-        <v>11</v>
+      <c r="E18" s="103" t="s">
+        <v>10</v>
       </c>
       <c r="F18" s="14"/>
-      <c r="G18" s="51"/>
+      <c r="G18" s="49"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -5026,17 +5139,17 @@
       <c r="CQ18" s="14"/>
     </row>
     <row r="19" spans="1:95" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="116"/>
-      <c r="E19" s="115"/>
+      <c r="A19" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="104"/>
+      <c r="E19" s="103"/>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -5129,17 +5242,17 @@
       <c r="CQ19" s="14"/>
     </row>
     <row r="20" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="116"/>
-      <c r="E20" s="115"/>
+      <c r="D20" s="104"/>
+      <c r="E20" s="103"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -5232,8 +5345,17 @@
       <c r="CQ20" s="14"/>
     </row>
     <row r="21" spans="1:95" s="4" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="116"/>
-      <c r="E21" s="115"/>
+      <c r="A21" s="137" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="139" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="141" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="104"/>
+      <c r="E21" s="103"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -5325,18 +5447,12 @@
       <c r="CP21" s="14"/>
       <c r="CQ21" s="14"/>
     </row>
-    <row r="22" spans="1:95" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="116"/>
-      <c r="E22" s="115"/>
+    <row r="22" spans="1:95" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="138"/>
+      <c r="B22" s="140"/>
+      <c r="C22" s="142"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="103"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -5429,13 +5545,13 @@
       <c r="CQ22" s="14"/>
     </row>
     <row r="23" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="93" t="s">
-        <v>186</v>
-      </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
+      <c r="A23" s="129" t="s">
+        <v>179</v>
+      </c>
+      <c r="B23" s="130"/>
+      <c r="C23" s="130"/>
+      <c r="D23" s="130"/>
+      <c r="E23" s="130"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -5528,20 +5644,20 @@
       <c r="CQ23" s="14"/>
     </row>
     <row r="24" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A24" s="81" t="s">
-        <v>162</v>
-      </c>
-      <c r="B24" s="82" t="s">
+      <c r="A24" s="79" t="s">
+        <v>213</v>
+      </c>
+      <c r="B24" s="80" t="s">
+        <v>215</v>
+      </c>
+      <c r="C24" s="94" t="s">
+        <v>217</v>
+      </c>
+      <c r="D24" s="131" t="s">
+        <v>164</v>
+      </c>
+      <c r="E24" s="131" t="s">
         <v>165</v>
-      </c>
-      <c r="C24" s="83" t="s">
-        <v>169</v>
-      </c>
-      <c r="D24" s="95" t="s">
-        <v>170</v>
-      </c>
-      <c r="E24" s="95" t="s">
-        <v>171</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -5634,18 +5750,18 @@
       <c r="CP24" s="14"/>
       <c r="CQ24" s="14"/>
     </row>
-    <row r="25" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="81" t="s">
-        <v>163</v>
-      </c>
-      <c r="B25" s="82" t="s">
-        <v>166</v>
-      </c>
-      <c r="C25" s="83" t="s">
-        <v>169</v>
-      </c>
-      <c r="D25" s="96"/>
-      <c r="E25" s="98"/>
+    <row r="25" spans="1:95" s="4" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="79" t="s">
+        <v>214</v>
+      </c>
+      <c r="B25" s="80" t="s">
+        <v>216</v>
+      </c>
+      <c r="C25" s="94" t="s">
+        <v>218</v>
+      </c>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
@@ -5737,18 +5853,18 @@
       <c r="CP25" s="14"/>
       <c r="CQ25" s="14"/>
     </row>
-    <row r="26" spans="1:95" s="4" customFormat="1" ht="119" x14ac:dyDescent="0.2">
-      <c r="A26" s="81" t="s">
-        <v>164</v>
-      </c>
-      <c r="B26" s="82" t="s">
-        <v>167</v>
-      </c>
-      <c r="C26" s="83" t="s">
-        <v>168</v>
-      </c>
-      <c r="D26" s="97"/>
-      <c r="E26" s="99"/>
+    <row r="26" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="B26" s="80" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="94" t="s">
+        <v>211</v>
+      </c>
+      <c r="D26" s="132"/>
+      <c r="E26" s="134"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -5840,14 +5956,18 @@
       <c r="CP26" s="14"/>
       <c r="CQ26" s="14"/>
     </row>
-    <row r="27" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="93" t="s">
-        <v>187</v>
-      </c>
-      <c r="B27" s="94"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="94"/>
+    <row r="27" spans="1:95" s="4" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="79" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" s="80" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" s="94" t="s">
+        <v>209</v>
+      </c>
+      <c r="D27" s="132"/>
+      <c r="E27" s="134"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
@@ -5939,22 +6059,18 @@
       <c r="CP27" s="14"/>
       <c r="CQ27" s="14"/>
     </row>
-    <row r="28" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="B28" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C28" s="49" t="s">
+    <row r="28" spans="1:95" s="4" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A28" s="79" t="s">
         <v>161</v>
       </c>
-      <c r="D28" s="107" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="111" t="s">
-        <v>13</v>
-      </c>
+      <c r="B28" s="80" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="81" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="133"/>
+      <c r="E28" s="135"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
@@ -6046,18 +6162,14 @@
       <c r="CP28" s="14"/>
       <c r="CQ28" s="14"/>
     </row>
-    <row r="29" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="107"/>
-      <c r="E29" s="111"/>
+    <row r="29" spans="1:95" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="129" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29" s="130"/>
+      <c r="C29" s="130"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="130"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
@@ -6149,22 +6261,24 @@
       <c r="CP29" s="14"/>
       <c r="CQ29" s="14"/>
     </row>
-    <row r="30" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:95" s="4" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="107"/>
-      <c r="E30" s="111"/>
+        <v>156</v>
+      </c>
+      <c r="B30" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="124" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="128" t="s">
+        <v>12</v>
+      </c>
       <c r="F30" s="14"/>
-      <c r="G30" s="14" t="s">
-        <v>58</v>
-      </c>
+      <c r="G30" s="14"/>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
@@ -6256,16 +6370,16 @@
     </row>
     <row r="31" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="107"/>
-      <c r="E31" s="111"/>
+        <v>0</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="124"/>
+      <c r="E31" s="128"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
@@ -6359,18 +6473,20 @@
     </row>
     <row r="32" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="107"/>
-      <c r="E32" s="111"/>
+        <v>1</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="124"/>
+      <c r="E32" s="128"/>
       <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
+      <c r="G32" s="14" t="s">
+        <v>57</v>
+      </c>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
@@ -6462,16 +6578,16 @@
     </row>
     <row r="33" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C33" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="107"/>
-      <c r="E33" s="111"/>
+        <v>2</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="124"/>
+      <c r="E33" s="128"/>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
@@ -6565,16 +6681,16 @@
     </row>
     <row r="34" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C34" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="107"/>
-      <c r="E34" s="111"/>
+        <v>3</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" s="124"/>
+      <c r="E34" s="128"/>
       <c r="F34" s="14"/>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
@@ -6666,14 +6782,18 @@
       <c r="CP34" s="14"/>
       <c r="CQ34" s="14"/>
     </row>
-    <row r="35" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="108" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="109"/>
-      <c r="C35" s="109"/>
-      <c r="D35" s="109"/>
-      <c r="E35" s="110"/>
+    <row r="35" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="124"/>
+      <c r="E35" s="128"/>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
@@ -6765,22 +6885,18 @@
       <c r="CP35" s="14"/>
       <c r="CQ35" s="14"/>
     </row>
-    <row r="36" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" s="101" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="104" t="s">
-        <v>57</v>
-      </c>
+    <row r="36" spans="1:95" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="124"/>
+      <c r="E36" s="128"/>
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
@@ -6872,18 +6988,14 @@
       <c r="CP36" s="14"/>
       <c r="CQ36" s="14"/>
     </row>
-    <row r="37" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="102"/>
-      <c r="E37" s="105"/>
+    <row r="37" spans="1:95" s="5" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="125" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="126"/>
+      <c r="C37" s="126"/>
+      <c r="D37" s="126"/>
+      <c r="E37" s="127"/>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
@@ -6975,18 +7087,22 @@
       <c r="CP37" s="14"/>
       <c r="CQ37" s="14"/>
     </row>
-    <row r="38" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:95" s="5" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>97</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="103"/>
-      <c r="E38" s="106"/>
+        <v>52</v>
+      </c>
+      <c r="D38" s="118" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="121" t="s">
+        <v>56</v>
+      </c>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
       <c r="H38" s="14"/>
@@ -7078,19 +7194,239 @@
       <c r="CP38" s="14"/>
       <c r="CQ38" s="14"/>
     </row>
-    <row r="39" spans="1:95" ht="51" x14ac:dyDescent="0.2">
-      <c r="C39" s="19" t="s">
+    <row r="39" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="119"/>
+      <c r="E39" s="122"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="14"/>
+      <c r="U39" s="14"/>
+      <c r="V39" s="14"/>
+      <c r="W39" s="14"/>
+      <c r="X39" s="14"/>
+      <c r="Y39" s="14"/>
+      <c r="Z39" s="14"/>
+      <c r="AA39" s="14"/>
+      <c r="AB39" s="14"/>
+      <c r="AC39" s="14"/>
+      <c r="AD39" s="14"/>
+      <c r="AE39" s="14"/>
+      <c r="AF39" s="14"/>
+      <c r="AG39" s="14"/>
+      <c r="AH39" s="14"/>
+      <c r="AI39" s="14"/>
+      <c r="AJ39" s="14"/>
+      <c r="AK39" s="14"/>
+      <c r="AL39" s="14"/>
+      <c r="AM39" s="14"/>
+      <c r="AN39" s="14"/>
+      <c r="AO39" s="14"/>
+      <c r="AP39" s="14"/>
+      <c r="AQ39" s="14"/>
+      <c r="AR39" s="14"/>
+      <c r="AS39" s="14"/>
+      <c r="AT39" s="14"/>
+      <c r="AU39" s="14"/>
+      <c r="AV39" s="14"/>
+      <c r="AW39" s="14"/>
+      <c r="AX39" s="14"/>
+      <c r="AY39" s="14"/>
+      <c r="AZ39" s="14"/>
+      <c r="BA39" s="14"/>
+      <c r="BB39" s="14"/>
+      <c r="BC39" s="14"/>
+      <c r="BD39" s="14"/>
+      <c r="BE39" s="14"/>
+      <c r="BF39" s="14"/>
+      <c r="BG39" s="14"/>
+      <c r="BH39" s="14"/>
+      <c r="BI39" s="14"/>
+      <c r="BJ39" s="14"/>
+      <c r="BK39" s="14"/>
+      <c r="BL39" s="14"/>
+      <c r="BM39" s="14"/>
+      <c r="BN39" s="14"/>
+      <c r="BO39" s="14"/>
+      <c r="BP39" s="14"/>
+      <c r="BQ39" s="14"/>
+      <c r="BR39" s="14"/>
+      <c r="BS39" s="14"/>
+      <c r="BT39" s="14"/>
+      <c r="BU39" s="14"/>
+      <c r="BV39" s="14"/>
+      <c r="BW39" s="14"/>
+      <c r="BX39" s="14"/>
+      <c r="BY39" s="14"/>
+      <c r="BZ39" s="14"/>
+      <c r="CA39" s="14"/>
+      <c r="CB39" s="14"/>
+      <c r="CC39" s="14"/>
+      <c r="CD39" s="14"/>
+      <c r="CE39" s="14"/>
+      <c r="CF39" s="14"/>
+      <c r="CG39" s="14"/>
+      <c r="CH39" s="14"/>
+      <c r="CI39" s="14"/>
+      <c r="CJ39" s="14"/>
+      <c r="CK39" s="14"/>
+      <c r="CL39" s="14"/>
+      <c r="CM39" s="14"/>
+      <c r="CN39" s="14"/>
+      <c r="CO39" s="14"/>
+      <c r="CP39" s="14"/>
+      <c r="CQ39" s="14"/>
+    </row>
+    <row r="40" spans="1:95" s="5" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="120"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="14"/>
+      <c r="N40" s="14"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="14"/>
+      <c r="Q40" s="14"/>
+      <c r="R40" s="14"/>
+      <c r="S40" s="14"/>
+      <c r="T40" s="14"/>
+      <c r="U40" s="14"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="14"/>
+      <c r="X40" s="14"/>
+      <c r="Y40" s="14"/>
+      <c r="Z40" s="14"/>
+      <c r="AA40" s="14"/>
+      <c r="AB40" s="14"/>
+      <c r="AC40" s="14"/>
+      <c r="AD40" s="14"/>
+      <c r="AE40" s="14"/>
+      <c r="AF40" s="14"/>
+      <c r="AG40" s="14"/>
+      <c r="AH40" s="14"/>
+      <c r="AI40" s="14"/>
+      <c r="AJ40" s="14"/>
+      <c r="AK40" s="14"/>
+      <c r="AL40" s="14"/>
+      <c r="AM40" s="14"/>
+      <c r="AN40" s="14"/>
+      <c r="AO40" s="14"/>
+      <c r="AP40" s="14"/>
+      <c r="AQ40" s="14"/>
+      <c r="AR40" s="14"/>
+      <c r="AS40" s="14"/>
+      <c r="AT40" s="14"/>
+      <c r="AU40" s="14"/>
+      <c r="AV40" s="14"/>
+      <c r="AW40" s="14"/>
+      <c r="AX40" s="14"/>
+      <c r="AY40" s="14"/>
+      <c r="AZ40" s="14"/>
+      <c r="BA40" s="14"/>
+      <c r="BB40" s="14"/>
+      <c r="BC40" s="14"/>
+      <c r="BD40" s="14"/>
+      <c r="BE40" s="14"/>
+      <c r="BF40" s="14"/>
+      <c r="BG40" s="14"/>
+      <c r="BH40" s="14"/>
+      <c r="BI40" s="14"/>
+      <c r="BJ40" s="14"/>
+      <c r="BK40" s="14"/>
+      <c r="BL40" s="14"/>
+      <c r="BM40" s="14"/>
+      <c r="BN40" s="14"/>
+      <c r="BO40" s="14"/>
+      <c r="BP40" s="14"/>
+      <c r="BQ40" s="14"/>
+      <c r="BR40" s="14"/>
+      <c r="BS40" s="14"/>
+      <c r="BT40" s="14"/>
+      <c r="BU40" s="14"/>
+      <c r="BV40" s="14"/>
+      <c r="BW40" s="14"/>
+      <c r="BX40" s="14"/>
+      <c r="BY40" s="14"/>
+      <c r="BZ40" s="14"/>
+      <c r="CA40" s="14"/>
+      <c r="CB40" s="14"/>
+      <c r="CC40" s="14"/>
+      <c r="CD40" s="14"/>
+      <c r="CE40" s="14"/>
+      <c r="CF40" s="14"/>
+      <c r="CG40" s="14"/>
+      <c r="CH40" s="14"/>
+      <c r="CI40" s="14"/>
+      <c r="CJ40" s="14"/>
+      <c r="CK40" s="14"/>
+      <c r="CL40" s="14"/>
+      <c r="CM40" s="14"/>
+      <c r="CN40" s="14"/>
+      <c r="CO40" s="14"/>
+      <c r="CP40" s="14"/>
+      <c r="CQ40" s="14"/>
+    </row>
+    <row r="41" spans="1:95" ht="51" x14ac:dyDescent="0.2">
+      <c r="C41" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="20" t="s">
+      <c r="D41" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="E41" s="20" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="D24:D28"/>
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="D30:D36"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="E30:E36"/>
     <mergeCell ref="E8:E12"/>
     <mergeCell ref="D18:D22"/>
     <mergeCell ref="E18:E22"/>
@@ -7099,33 +7435,19 @@
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="D3:D6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="D8:D12"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="D28:D34"/>
-    <mergeCell ref="A35:E35"/>
-    <mergeCell ref="E28:E34"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="E14:E16"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" location="/dashboard" display="https://acleddata.com/dashboard/ - /dashboard" xr:uid="{F76E7675-2B2E-2D45-8C2B-2CB43E3D6E32}"/>
     <hyperlink ref="B14" r:id="rId2" display="https://www.worldbank.org/en/publication/global-economic-prospects" xr:uid="{6B81CDE3-78BD-FB41-88E5-D7CCF55FBF33}"/>
     <hyperlink ref="B15" r:id="rId3" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{283F4A21-AE52-424B-A454-2015ED782078}"/>
-    <hyperlink ref="B22" r:id="rId4" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
-    <hyperlink ref="B34" r:id="rId5" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
+    <hyperlink ref="B21" r:id="rId4" display="https://www.imf.org/external/pubs/ft/weo/2020/01/weodata/download.aspx" xr:uid="{A46374A5-6C1D-3A40-9101-CF1B60D6931C}"/>
+    <hyperlink ref="B36" r:id="rId5" display="https://www.bsg.ox.ac.uk/research/publications/lockdown-rollback-checklist" xr:uid="{859F7DF3-36B6-344E-923B-6E65426E76CD}"/>
     <hyperlink ref="B3" r:id="rId6" display="https://fews.net/" xr:uid="{3D674EBD-4EF9-1342-883D-87D2B91B65D7}"/>
     <hyperlink ref="B18" r:id="rId7" display="COVID Economic Stimus Index (as measured by Elgin et al)" xr:uid="{999A8B13-E27C-374A-82CC-F226FAFAE1F4}"/>
   </hyperlinks>
@@ -7140,310 +7462,315 @@
   </sheetPr>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.5" style="76" customWidth="1"/>
+    <col min="1" max="1" width="41.5" style="74" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
-    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="62.33203125" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="71" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>14</v>
+    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>13</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+    </row>
+    <row r="3" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="105" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="107"/>
+    </row>
+    <row r="5" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="78" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="107"/>
+    </row>
+    <row r="6" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="129" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="130"/>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="130"/>
+    </row>
+    <row r="7" spans="1:12" ht="159" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="105"/>
+      <c r="I7" s="106"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="107"/>
+    </row>
+    <row r="8" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="117" t="s">
+      <c r="B8" s="106"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="129"/>
+      <c r="I8" s="130"/>
+      <c r="J8" s="130"/>
+      <c r="K8" s="130"/>
+      <c r="L8" s="130"/>
+    </row>
+    <row r="9" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" s="95" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="96" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+    </row>
+    <row r="10" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="129"/>
+      <c r="I10" s="130"/>
+      <c r="J10" s="130"/>
+      <c r="K10" s="130"/>
+      <c r="L10" s="130"/>
+    </row>
+    <row r="11" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="129" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" s="130"/>
+      <c r="C11" s="130"/>
+      <c r="D11" s="130"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="125"/>
+      <c r="I11" s="126"/>
+      <c r="J11" s="126"/>
+      <c r="K11" s="126"/>
+      <c r="L11" s="127"/>
+    </row>
+    <row r="12" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="85"/>
+      <c r="L12" s="85"/>
+    </row>
+    <row r="13" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="68"/>
+      <c r="G13" s="44"/>
+    </row>
+    <row r="14" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="125" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="126"/>
+      <c r="C14" s="126"/>
+      <c r="D14" s="126"/>
+      <c r="G14" s="43"/>
+    </row>
+    <row r="15" spans="1:12" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="61" t="s">
         <v>184</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-    </row>
-    <row r="3" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="117" t="s">
+      <c r="B15" s="63" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="H4" s="117"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
-      <c r="K4" s="118"/>
-      <c r="L4" s="119"/>
-    </row>
-    <row r="5" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="80" t="s">
-        <v>158</v>
-      </c>
-      <c r="B5" s="78" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="H5" s="117"/>
-      <c r="I5" s="118"/>
-      <c r="J5" s="118"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="119"/>
-    </row>
-    <row r="6" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="93" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="94"/>
-      <c r="J6" s="94"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
-    </row>
-    <row r="7" spans="1:12" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="73" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G7" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="117"/>
-      <c r="I7" s="118"/>
-      <c r="J7" s="118"/>
-      <c r="K7" s="118"/>
-      <c r="L7" s="119"/>
-    </row>
-    <row r="8" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="117" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-    </row>
-    <row r="9" spans="1:12" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="B9" s="137" t="s">
-        <v>208</v>
-      </c>
-      <c r="C9" s="138" t="s">
-        <v>209</v>
-      </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="91"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92"/>
-      <c r="L9" s="92"/>
-    </row>
-    <row r="10" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="37" t="s">
+      <c r="C15" s="63" t="s">
+        <v>186</v>
+      </c>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="G15" s="43"/>
+    </row>
+    <row r="16" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="61" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="G16" s="43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="129" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="130"/>
+      <c r="C17" s="130"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="130"/>
+    </row>
+    <row r="18" spans="1:6" ht="248" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" s="93"/>
-      <c r="I10" s="94"/>
-      <c r="J10" s="94"/>
-      <c r="K10" s="94"/>
-      <c r="L10" s="94"/>
-    </row>
-    <row r="11" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="93" t="s">
-        <v>187</v>
-      </c>
-      <c r="B11" s="94"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="108"/>
-      <c r="I11" s="109"/>
-      <c r="J11" s="109"/>
-      <c r="K11" s="109"/>
-      <c r="L11" s="110"/>
-    </row>
-    <row r="12" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="74" t="s">
-        <v>188</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>189</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>190</v>
-      </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="87"/>
-    </row>
-    <row r="13" spans="1:12" ht="68" x14ac:dyDescent="0.2">
-      <c r="A13" s="74" t="s">
+      <c r="E18" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="42" t="s">
         <v>59</v>
-      </c>
-      <c r="B13" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="68" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" s="69" t="s">
-        <v>137</v>
-      </c>
-      <c r="F13" s="70"/>
-      <c r="G13" s="46"/>
-    </row>
-    <row r="14" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="108" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="109"/>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109"/>
-      <c r="G14" s="45"/>
-    </row>
-    <row r="15" spans="1:12" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="63" t="s">
-        <v>191</v>
-      </c>
-      <c r="B15" s="65" t="s">
-        <v>192</v>
-      </c>
-      <c r="C15" s="65" t="s">
-        <v>193</v>
-      </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="G15" s="45"/>
-    </row>
-    <row r="16" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="63" t="s">
-        <v>133</v>
-      </c>
-      <c r="B16" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="67" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="35"/>
-      <c r="G16" s="45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="93" t="s">
-        <v>186</v>
-      </c>
-      <c r="B17" s="94"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-    </row>
-    <row r="18" spans="1:6" ht="248" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="75" t="s">
-        <v>155</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="44" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="H11:L11"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="H4:L4"/>
@@ -7453,11 +7780,6 @@
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="WFP Proteus composite index: " xr:uid="{3B8342E4-A803-C342-923C-31BDAA92A373}"/>
@@ -7486,55 +7808,55 @@
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.1640625" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="35.1640625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="22" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B3" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C3" s="21" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="32" t="s">
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B4" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C4" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C8" s="31"/>
+      <c r="C8" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7556,107 +7878,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>104</v>
+      <c r="A1" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="117"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="119"/>
+        <v>177</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="105"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="107"/>
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>151</v>
-      </c>
-      <c r="E3" s="117"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-      <c r="I3" s="119"/>
+        <v>178</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="105"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="106"/>
+      <c r="I3" s="107"/>
     </row>
     <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" s="93"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
+        <v>34</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="129"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="130"/>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="E5" s="117"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="119"/>
+        <v>27</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="105"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="107"/>
     </row>
     <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>187</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="E6" s="93"/>
-      <c r="F6" s="94"/>
-      <c r="G6" s="94"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="94"/>
+        <v>180</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="129"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="130"/>
     </row>
     <row r="7" spans="1:9" ht="53" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" s="93"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
+        <v>28</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="129"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="130"/>
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>200</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="E8" s="108"/>
-      <c r="F8" s="109"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="109"/>
-      <c r="I8" s="110"/>
+        <v>193</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="125"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="127"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="79" t="s">
-        <v>60</v>
+      <c r="B24" s="77" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -7697,512 +8019,512 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="59" t="s">
+      <c r="A1" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="59" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="59" t="s">
-        <v>107</v>
+      <c r="D1" s="57" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>61</v>
+        <v>177</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="61"/>
+        <v>106</v>
+      </c>
+      <c r="E2" s="59"/>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
-      </c>
-      <c r="E3" s="61"/>
+        <v>191</v>
+      </c>
+      <c r="E3" s="59"/>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
         <v>108</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>157</v>
+        <v>27</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>154</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>199</v>
-      </c>
-      <c r="C7" s="60" t="s">
-        <v>59</v>
+        <v>192</v>
+      </c>
+      <c r="C7" s="58" t="s">
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="63" t="s">
-        <v>133</v>
+        <v>28</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>130</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
-      </c>
-      <c r="C9" s="64" t="s">
-        <v>155</v>
+        <v>193</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>152</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="77" t="s">
-        <v>139</v>
+        <v>177</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="75" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>204</v>
-      </c>
-      <c r="D11" s="77" t="s">
-        <v>138</v>
+        <v>177</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" s="75" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B12" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
-        <v>185</v>
-      </c>
-      <c r="C14" s="72" t="s">
-        <v>173</v>
+        <v>178</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>167</v>
       </c>
       <c r="D14" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B15" t="s">
-        <v>185</v>
-      </c>
-      <c r="C15" s="72" t="s">
-        <v>174</v>
+        <v>178</v>
+      </c>
+      <c r="C15" s="70" t="s">
+        <v>168</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
-      </c>
-      <c r="C16" s="72" t="s">
-        <v>175</v>
+        <v>178</v>
+      </c>
+      <c r="C16" s="70" t="s">
+        <v>169</v>
       </c>
       <c r="D16" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="90" t="s">
-        <v>115</v>
+      <c r="A17" s="88" t="s">
+        <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>185</v>
-      </c>
-      <c r="C17" s="88" t="s">
-        <v>176</v>
-      </c>
-      <c r="D17" s="89" t="s">
-        <v>197</v>
+        <v>178</v>
+      </c>
+      <c r="C17" s="86" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="87" t="s">
+        <v>190</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
-        <v>200</v>
-      </c>
-      <c r="C20" s="84" t="s">
-        <v>162</v>
+        <v>193</v>
+      </c>
+      <c r="C20" s="82" t="s">
+        <v>159</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B21" t="s">
-        <v>200</v>
-      </c>
-      <c r="C21" s="84" t="s">
-        <v>163</v>
+        <v>193</v>
+      </c>
+      <c r="C21" s="82" t="s">
+        <v>160</v>
       </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
-        <v>200</v>
-      </c>
-      <c r="C22" s="84" t="s">
-        <v>164</v>
+        <v>193</v>
+      </c>
+      <c r="C22" s="82" t="s">
+        <v>161</v>
       </c>
       <c r="D22" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>96</v>
+        <v>27</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>100</v>
+        <v>27</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>98</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>91</v>
+        <v>27</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" t="s">
+        <v>192</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" t="s">
         <v>115</v>
-      </c>
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" t="s">
-        <v>199</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="D27" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B28" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B30" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D30" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B31" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D32" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B33" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>